<commit_message>
worked on change password section...
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3785" uniqueCount="1019">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3790" uniqueCount="1025">
   <si>
     <t>Test Objective</t>
   </si>
@@ -4784,12 +4784,31 @@
   <si>
     <t>fn_RemoveImg</t>
   </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>fn_CancelProfilePage</t>
+  </si>
+  <si>
+    <t>fn_ChangePassword</t>
+  </si>
+  <si>
+    <t>fn_ChangeCurrentPassword</t>
+  </si>
+  <si>
+    <t>fn_ValidationPassword</t>
+  </si>
+  <si>
+    <t>fh_CancelChangePassword</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5260,24 +5279,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5703125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.5703125" style="8" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.85546875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.5703125" style="6" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="41.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26" style="6" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" style="6" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="24.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="16.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="8" width="16.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="6" width="31.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="6" width="33.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="41.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="6" width="26.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="6" width="11.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="8" width="24.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -5760,8 +5779,8 @@
       <c r="J18" s="8" t="s">
         <v>922</v>
       </c>
-      <c r="K18" s="19" t="s">
-        <v>909</v>
+      <c r="K18" t="s">
+        <v>1019</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5792,8 +5811,8 @@
       <c r="J19" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K19" s="6" t="s">
-        <v>911</v>
+      <c r="K19" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5806,6 +5825,9 @@
       <c r="C20" s="6" t="s">
         <v>39</v>
       </c>
+      <c r="D20" s="8" t="s">
+        <v>1020</v>
+      </c>
       <c r="E20" s="8" t="s">
         <v>89</v>
       </c>
@@ -5821,8 +5843,8 @@
       <c r="J20" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K20" s="6" t="s">
-        <v>911</v>
+      <c r="K20" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -5835,6 +5857,9 @@
       <c r="C21" s="6" t="s">
         <v>54</v>
       </c>
+      <c r="D21" s="8" t="s">
+        <v>1021</v>
+      </c>
       <c r="E21" s="8" t="s">
         <v>56</v>
       </c>
@@ -5850,13 +5875,13 @@
       <c r="J21" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K21" s="6" t="s">
-        <v>911</v>
+      <c r="K21" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>42</v>
@@ -5864,6 +5889,9 @@
       <c r="C22" s="6" t="s">
         <v>54</v>
       </c>
+      <c r="D22" s="8" t="s">
+        <v>1022</v>
+      </c>
       <c r="E22" s="8" t="s">
         <v>59</v>
       </c>
@@ -5879,13 +5907,13 @@
       <c r="J22" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K22" s="6" t="s">
-        <v>911</v>
+      <c r="K22" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>42</v>
@@ -5893,6 +5921,9 @@
       <c r="C23" s="6" t="s">
         <v>54</v>
       </c>
+      <c r="D23" s="8" t="s">
+        <v>1023</v>
+      </c>
       <c r="E23" s="8" t="s">
         <v>63</v>
       </c>
@@ -5908,13 +5939,13 @@
       <c r="J23" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K23" s="6" t="s">
-        <v>911</v>
+      <c r="K23" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>42</v>
@@ -5923,7 +5954,7 @@
         <v>54</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>1004</v>
+        <v>1024</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>65</v>
@@ -5940,13 +5971,13 @@
       <c r="J24" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K24" s="6" t="s">
-        <v>911</v>
+      <c r="K24" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>9</v>
@@ -5975,7 +6006,7 @@
     </row>
     <row r="26" spans="1:12" ht="210" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>9</v>
@@ -6004,7 +6035,7 @@
     </row>
     <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>102</v>
@@ -6033,7 +6064,7 @@
     </row>
     <row r="28" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>42</v>
@@ -6062,7 +6093,7 @@
     </row>
     <row r="29" spans="1:12" ht="315" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>42</v>
@@ -6091,7 +6122,7 @@
     </row>
     <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>42</v>
@@ -6120,7 +6151,7 @@
     </row>
     <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>120</v>
@@ -6149,7 +6180,7 @@
     </row>
     <row r="32" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>120</v>
@@ -6178,7 +6209,7 @@
     </row>
     <row r="33" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>120</v>
@@ -6207,7 +6238,7 @@
     </row>
     <row r="34" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>120</v>
@@ -6236,7 +6267,7 @@
     </row>
     <row r="35" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>120</v>
@@ -6265,7 +6296,7 @@
     </row>
     <row r="36" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>120</v>
@@ -6297,7 +6328,7 @@
     </row>
     <row r="37" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>154</v>
@@ -6329,7 +6360,7 @@
     </row>
     <row r="38" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>154</v>
@@ -6358,7 +6389,7 @@
     </row>
     <row r="39" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>154</v>
@@ -6387,7 +6418,7 @@
     </row>
     <row r="40" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>154</v>
@@ -6419,7 +6450,7 @@
     </row>
     <row r="41" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>174</v>
@@ -6448,7 +6479,7 @@
     </row>
     <row r="42" spans="1:12" ht="270" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>174</v>
@@ -6483,7 +6514,7 @@
     </row>
     <row r="43" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>174</v>
@@ -6512,7 +6543,7 @@
     </row>
     <row r="44" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>174</v>
@@ -6541,7 +6572,7 @@
     </row>
     <row r="45" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>174</v>
@@ -6570,7 +6601,7 @@
     </row>
     <row r="46" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>174</v>
@@ -6599,7 +6630,7 @@
     </row>
     <row r="47" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>174</v>
@@ -6628,7 +6659,7 @@
     </row>
     <row r="48" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>208</v>
@@ -6657,7 +6688,7 @@
     </row>
     <row r="49" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>208</v>
@@ -6689,7 +6720,7 @@
     </row>
     <row r="50" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>208</v>
@@ -6718,7 +6749,7 @@
     </row>
     <row r="51" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>208</v>
@@ -6747,7 +6778,7 @@
     </row>
     <row r="52" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>208</v>
@@ -6776,7 +6807,7 @@
     </row>
     <row r="53" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>208</v>
@@ -6802,7 +6833,7 @@
     </row>
     <row r="54" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>208</v>
@@ -6837,7 +6868,7 @@
     </row>
     <row r="55" spans="1:12" ht="285" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>208</v>
@@ -6866,7 +6897,7 @@
     </row>
     <row r="56" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>208</v>
@@ -6895,7 +6926,7 @@
     </row>
     <row r="57" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>208</v>
@@ -6924,7 +6955,7 @@
     </row>
     <row r="58" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>208</v>
@@ -6953,7 +6984,7 @@
     </row>
     <row r="59" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>208</v>
@@ -6982,7 +7013,7 @@
     </row>
     <row r="60" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>208</v>
@@ -7011,7 +7042,7 @@
     </row>
     <row r="61" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>208</v>
@@ -7040,7 +7071,7 @@
     </row>
     <row r="62" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>208</v>
@@ -7069,7 +7100,7 @@
     </row>
     <row r="63" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>208</v>
@@ -7098,7 +7129,7 @@
     </row>
     <row r="64" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>277</v>
@@ -7127,7 +7158,7 @@
     </row>
     <row r="65" spans="1:15" ht="180" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>277</v>
@@ -7156,7 +7187,7 @@
     </row>
     <row r="66" spans="1:15" ht="255" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>277</v>
@@ -7185,7 +7216,7 @@
     </row>
     <row r="67" spans="1:15" ht="285" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>277</v>
@@ -7214,7 +7245,7 @@
     </row>
     <row r="68" spans="1:15" ht="315" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>277</v>
@@ -7243,7 +7274,7 @@
     </row>
     <row r="69" spans="1:15" ht="180" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>277</v>
@@ -7272,7 +7303,7 @@
     </row>
     <row r="70" spans="1:15" ht="270" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>277</v>
@@ -7301,7 +7332,7 @@
     </row>
     <row r="71" spans="1:15" ht="300" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>277</v>
@@ -7330,7 +7361,7 @@
     </row>
     <row r="72" spans="1:15" ht="360" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>277</v>
@@ -7359,7 +7390,7 @@
     </row>
     <row r="73" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>277</v>
@@ -7388,7 +7419,7 @@
     </row>
     <row r="74" spans="1:15" ht="180" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>277</v>
@@ -7417,7 +7448,7 @@
     </row>
     <row r="75" spans="1:15" ht="225" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>277</v>
@@ -7446,7 +7477,7 @@
     </row>
     <row r="76" spans="1:15" ht="300" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>277</v>
@@ -7479,7 +7510,7 @@
     </row>
     <row r="77" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>277</v>
@@ -7508,7 +7539,7 @@
     </row>
     <row r="78" spans="1:15" ht="180" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>277</v>
@@ -7537,7 +7568,7 @@
     </row>
     <row r="79" spans="1:15" ht="195" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>277</v>
@@ -7566,7 +7597,7 @@
     </row>
     <row r="80" spans="1:15" ht="285" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>277</v>
@@ -7598,7 +7629,7 @@
     </row>
     <row r="81" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>277</v>
@@ -7627,7 +7658,7 @@
     </row>
     <row r="82" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>277</v>
@@ -7656,7 +7687,7 @@
     </row>
     <row r="83" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>277</v>
@@ -7685,7 +7716,7 @@
     </row>
     <row r="84" spans="1:13" ht="240" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>277</v>
@@ -7714,7 +7745,7 @@
     </row>
     <row r="85" spans="1:13" ht="270" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>277</v>
@@ -7743,7 +7774,7 @@
     </row>
     <row r="86" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>277</v>
@@ -7770,7 +7801,7 @@
     </row>
     <row r="87" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>277</v>
@@ -7797,7 +7828,7 @@
     </row>
     <row r="88" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>277</v>
@@ -7821,7 +7852,7 @@
     </row>
     <row r="89" spans="1:13" ht="360" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>277</v>
@@ -11464,17 +11495,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Validations for mandatory fields in forgot password...
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3805" uniqueCount="1033">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3804" uniqueCount="1034">
   <si>
     <t>Test Objective</t>
   </si>
@@ -4841,13 +4841,16 @@
   <si>
     <t>fn_SignOut</t>
   </si>
+  <si>
+    <t>1.  School logo should be visible 
+2.  Quick links Home, Bookmarks, My Class, Notifications, Reports, Marks Entry and My Profile should be visible</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5318,24 +5321,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F27" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="F28" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="18.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="16.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="8" width="16.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="6" width="31.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="6" width="33.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="41.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="6" width="26.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="6" width="11.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="8" width="24.28515625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.5703125" style="8" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.85546875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.5703125" style="6" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="41.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26" style="6" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" style="6" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="24.28515625" style="8" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -6168,7 +6171,7 @@
         <v>1027</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>109</v>
+        <v>1033</v>
       </c>
       <c r="J29" s="6" t="s">
         <v>972</v>
@@ -11581,17 +11584,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="31.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="37.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
forgot password section done and Bookmark section started...
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3804" uniqueCount="1034">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3808" uniqueCount="1037">
   <si>
     <t>Test Objective</t>
   </si>
@@ -4845,12 +4845,22 @@
     <t>1.  School logo should be visible 
 2.  Quick links Home, Bookmarks, My Class, Notifications, Reports, Marks Entry and My Profile should be visible</t>
   </si>
+  <si>
+    <t>fn_HeaderDashboard</t>
+  </si>
+  <si>
+    <t>fn_FooterDashboard</t>
+  </si>
+  <si>
+    <t>fn_VisibilitySubjectandCalendar</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5321,24 +5331,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F28" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5703125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.5703125" style="8" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.85546875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.5703125" style="6" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="41.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26" style="6" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" style="6" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="24.28515625" style="8" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="16.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="8" width="16.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="6" width="31.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="6" width="33.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="41.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="6" width="26.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="6" width="11.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="8" width="24.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -6161,6 +6171,9 @@
       <c r="C29" s="6" t="s">
         <v>106</v>
       </c>
+      <c r="D29" s="8" t="s">
+        <v>1034</v>
+      </c>
       <c r="E29" s="8" t="s">
         <v>107</v>
       </c>
@@ -6176,8 +6189,8 @@
       <c r="J29" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K29" s="6" t="s">
-        <v>911</v>
+      <c r="K29" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="315" x14ac:dyDescent="0.25">
@@ -6190,6 +6203,9 @@
       <c r="C30" s="6" t="s">
         <v>111</v>
       </c>
+      <c r="D30" s="8" t="s">
+        <v>1035</v>
+      </c>
       <c r="E30" s="8" t="s">
         <v>110</v>
       </c>
@@ -6205,8 +6221,8 @@
       <c r="J30" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K30" s="6" t="s">
-        <v>911</v>
+      <c r="K30" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -6219,6 +6235,9 @@
       <c r="C31" s="8" t="s">
         <v>116</v>
       </c>
+      <c r="D31" s="8" t="s">
+        <v>1036</v>
+      </c>
       <c r="E31" s="8" t="s">
         <v>122</v>
       </c>
@@ -6234,8 +6253,8 @@
       <c r="J31" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K31" s="6" t="s">
-        <v>911</v>
+      <c r="K31" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -11584,17 +11603,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Assessment reports ended and learning report started...
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3849" uniqueCount="1081">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3856" uniqueCount="1086">
   <si>
     <t>Test Objective</t>
   </si>
@@ -4991,12 +4991,28 @@
   <si>
     <t xml:space="preserve">Query: Some reports have no navigate icon and some are having  </t>
   </si>
+  <si>
+    <t>fn_ViewAssessmentReports</t>
+  </si>
+  <si>
+    <t>fn_SubjectwiseDetailedReportofStudent</t>
+  </si>
+  <si>
+    <t>fn_LandingSectionwiseLearningReports</t>
+  </si>
+  <si>
+    <t>fn_ViewSectionwiseDetailedLearningReports</t>
+  </si>
+  <si>
+    <t>fn_ViewAveragePerformanceofaLessonPlanandActivitywisePerformance</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5467,25 +5483,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F67" workbookViewId="0">
-      <selection activeCell="I67" sqref="I67"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5703125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.5703125" style="8" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.85546875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.5703125" style="6" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="41.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26" style="6" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" style="6" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="52.7109375" style="8" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="16.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="8" width="16.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="6" width="31.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="6" width="33.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="41.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="6" width="26.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="6" width="11.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="8" width="52.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -7575,8 +7591,8 @@
       <c r="J67" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K67" s="6" t="s">
-        <v>911</v>
+      <c r="K67" t="s">
+        <v>1012</v>
       </c>
       <c r="L67" s="20" t="s">
         <v>1080</v>
@@ -7592,6 +7608,9 @@
       <c r="C68" s="8" t="s">
         <v>298</v>
       </c>
+      <c r="D68" s="8" t="s">
+        <v>1081</v>
+      </c>
       <c r="E68" s="8" t="s">
         <v>290</v>
       </c>
@@ -7607,8 +7626,8 @@
       <c r="J68" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K68" s="6" t="s">
-        <v>911</v>
+      <c r="K68" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="69" spans="1:15" ht="315" x14ac:dyDescent="0.25">
@@ -7621,6 +7640,9 @@
       <c r="C69" s="8" t="s">
         <v>298</v>
       </c>
+      <c r="D69" s="8" t="s">
+        <v>1082</v>
+      </c>
       <c r="E69" s="8" t="s">
         <v>295</v>
       </c>
@@ -7650,6 +7672,9 @@
       <c r="C70" s="8" t="s">
         <v>299</v>
       </c>
+      <c r="D70" s="8" t="s">
+        <v>1083</v>
+      </c>
       <c r="E70" s="8" t="s">
         <v>301</v>
       </c>
@@ -7665,8 +7690,8 @@
       <c r="J70" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K70" s="6" t="s">
-        <v>911</v>
+      <c r="K70" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="71" spans="1:15" ht="270" x14ac:dyDescent="0.25">
@@ -7679,6 +7704,9 @@
       <c r="C71" s="8" t="s">
         <v>299</v>
       </c>
+      <c r="D71" s="8" t="s">
+        <v>1084</v>
+      </c>
       <c r="E71" s="8" t="s">
         <v>286</v>
       </c>
@@ -7707,6 +7735,9 @@
       </c>
       <c r="C72" s="8" t="s">
         <v>299</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>1085</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>308</v>
@@ -11863,17 +11894,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Started tracking report in report portion...
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3856" uniqueCount="1086">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3858" uniqueCount="1091">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5006,13 +5006,28 @@
   <si>
     <t>fn_ViewAveragePerformanceofaLessonPlanandActivitywisePerformance</t>
   </si>
+  <si>
+    <t>fn_ViewSubjectwiseDetailedReportofRespectiveStudent</t>
+  </si>
+  <si>
+    <t>1.Sectionwise detailed reports not showing navigate arrow
+2. No learning report available</t>
+  </si>
+  <si>
+    <t>fn_ViewTrackingReport</t>
+  </si>
+  <si>
+    <t>fn_ViewTrackingLearningReport</t>
+  </si>
+  <si>
+    <t>fn_ViewAvrgPerformanceofLessonandActivitywisePerformance</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5483,25 +5498,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="18.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="16.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="8" width="16.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="6" width="31.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="6" width="33.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="41.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="6" width="26.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="6" width="11.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="8" width="52.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.5703125" style="8" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.85546875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.5703125" style="6" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="41.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26" style="6" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" style="6" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="52.7109375" style="8" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -7658,8 +7673,8 @@
       <c r="J69" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K69" s="6" t="s">
-        <v>911</v>
+      <c r="K69" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="70" spans="1:15" ht="180" x14ac:dyDescent="0.25">
@@ -7768,6 +7783,9 @@
       <c r="C73" s="8" t="s">
         <v>299</v>
       </c>
+      <c r="D73" s="8" t="s">
+        <v>1086</v>
+      </c>
       <c r="E73" s="8" t="s">
         <v>295</v>
       </c>
@@ -7784,7 +7802,7 @@
         <v>931</v>
       </c>
       <c r="L73" s="20" t="s">
-        <v>979</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="74" spans="1:15" ht="105" x14ac:dyDescent="0.25">
@@ -7797,6 +7815,9 @@
       <c r="C74" s="8" t="s">
         <v>316</v>
       </c>
+      <c r="D74" s="8" t="s">
+        <v>1088</v>
+      </c>
       <c r="E74" s="8" t="s">
         <v>315</v>
       </c>
@@ -7809,8 +7830,8 @@
       <c r="I74" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="K74" s="21" t="s">
-        <v>911</v>
+      <c r="K74" t="s">
+        <v>1012</v>
       </c>
       <c r="L74" s="20" t="s">
         <v>932</v>
@@ -7826,6 +7847,9 @@
       <c r="C75" s="8" t="s">
         <v>316</v>
       </c>
+      <c r="D75" s="8" t="s">
+        <v>1089</v>
+      </c>
       <c r="E75" s="8" t="s">
         <v>319</v>
       </c>
@@ -7854,6 +7878,9 @@
       </c>
       <c r="C76" s="8" t="s">
         <v>316</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>1090</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>323</v>
@@ -11894,17 +11921,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="31.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="37.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added script for view report in learning resources...
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3858" uniqueCount="1091">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3860" uniqueCount="1094">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5021,6 +5021,21 @@
   </si>
   <si>
     <t>fn_ViewAvrgPerformanceofLessonandActivitywisePerformance</t>
+  </si>
+  <si>
+    <t>1. Click Reports tab on dashboard
+2. Click on Menu icon and select Tracking  Reports
+3. Click View Learning Reports under Tracking Reports on the left pane
+4. Click on View Details link corresponding to a Subject
+5. Click on Lesson Plan Name link
+6. Click on Activity Name tab
+7. Click on the View details link corresponding to the student’s name</t>
+  </si>
+  <si>
+    <t>fn_ViewSubjectwiseDetailedReportofRespectiveStudentLearning</t>
+  </si>
+  <si>
+    <t>Query: where from can we add activities to learning report</t>
   </si>
 </sst>
 </file>
@@ -5498,8 +5513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7911,6 +7926,9 @@
       <c r="C77" s="8" t="s">
         <v>316</v>
       </c>
+      <c r="D77" s="8" t="s">
+        <v>1092</v>
+      </c>
       <c r="E77" s="8" t="s">
         <v>327</v>
       </c>
@@ -7918,7 +7936,7 @@
         <v>38</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>328</v>
+        <v>1091</v>
       </c>
       <c r="I77" s="2" t="s">
         <v>329</v>
@@ -7929,7 +7947,9 @@
       <c r="K77" s="21" t="s">
         <v>911</v>
       </c>
-      <c r="L77" s="20"/>
+      <c r="L77" s="20" t="s">
+        <v>1093</v>
+      </c>
       <c r="O77" t="s">
         <v>934</v>
       </c>

</xml_diff>

<commit_message>
started working on application usage report
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3863" uniqueCount="1097">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3864" uniqueCount="1098">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5045,6 +5045,9 @@
   </si>
   <si>
     <t>fn_PrintUsageReport</t>
+  </si>
+  <si>
+    <t>fn_ViewSectionwiseUsageReport</t>
   </si>
 </sst>
 </file>
@@ -5522,8 +5525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B80" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="B81" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8068,6 +8071,9 @@
       </c>
       <c r="C81" s="8" t="s">
         <v>330</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>1097</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>343</v>

</xml_diff>

<commit_message>
Student Individual report ended.....
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3864" uniqueCount="1098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3969" uniqueCount="1196">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5048,6 +5048,300 @@
   </si>
   <si>
     <t>fn_ViewSectionwiseUsageReport</t>
+  </si>
+  <si>
+    <t>fn_ViewOverallandSubjectwisePerformanceofStudent</t>
+  </si>
+  <si>
+    <t>fL_ViewlessonsfortheplannedofView</t>
+  </si>
+  <si>
+    <t>fl_MarktolessonasmarkofMark</t>
+  </si>
+  <si>
+    <t>fA_ViewviewDueForAssignmentsofView</t>
+  </si>
+  <si>
+    <t>fA_AddRemarkforstudent'sFeedbackofView</t>
+  </si>
+  <si>
+    <t>fn_ViewofLessonwiseoverview</t>
+  </si>
+  <si>
+    <t>fn_PreviewofPreviewLesson</t>
+  </si>
+  <si>
+    <t>fn_ViewofTeachingresources</t>
+  </si>
+  <si>
+    <t>fn_ViewofLessonPlan</t>
+  </si>
+  <si>
+    <t>fn_ViewofRecommendedLesson</t>
+  </si>
+  <si>
+    <t>fn_ViewofMyLessons</t>
+  </si>
+  <si>
+    <t>fn_FunctionalityofPlanLessons</t>
+  </si>
+  <si>
+    <t>fn_FunctionalityToDeleteofMyLessons)</t>
+  </si>
+  <si>
+    <t>fi_FunctionalityofLearningResource</t>
+  </si>
+  <si>
+    <t>fi_FunctionalityofLearningResources</t>
+  </si>
+  <si>
+    <t>fi_FunctionalityToofLearningResources</t>
+  </si>
+  <si>
+    <t>fi_FunctionalityofPlayContent</t>
+  </si>
+  <si>
+    <t>fi_ValidationsForMandatoryFieldsOnSaveAssessmentWindowofAssessmentGeneration</t>
+  </si>
+  <si>
+    <t>f-_FunctionalityofEditsection</t>
+  </si>
+  <si>
+    <t>f-_FunctionalityofDeletesection</t>
+  </si>
+  <si>
+    <t>f-_FunctionalityToSearchSpecificQuestionWithAdvancedofQuestionBank</t>
+  </si>
+  <si>
+    <t>f-_FunctionalityToSearchSpecificQuestionFromLeftofQuestionBank</t>
+  </si>
+  <si>
+    <t>f-_FunctionalityToTryoutAofQuestionBank</t>
+  </si>
+  <si>
+    <t>f-_FunctionalityToDeleteTestofNobutton</t>
+  </si>
+  <si>
+    <t>f-_TeacherIsNotAbleofRecommendedtests</t>
+  </si>
+  <si>
+    <t>fv_ValidationToofTimefields</t>
+  </si>
+  <si>
+    <t>fP_ViewofPlannedLessons</t>
+  </si>
+  <si>
+    <t>fe_ManageAssignmentIsofCalendarsection</t>
+  </si>
+  <si>
+    <t>fn_ViewAverageScoreofSelectedSubject</t>
+  </si>
+  <si>
+    <t>fl_FunctionalityofClassperformances</t>
+  </si>
+  <si>
+    <t>fl_FunctionalityToofWisePerformance</t>
+  </si>
+  <si>
+    <t>fl_FunctionalityToCalculateofByActivity</t>
+  </si>
+  <si>
+    <t>fc_ViewChapterWiseofWiseperformance</t>
+  </si>
+  <si>
+    <t>fc_ViewAllTheLessonsUnderTheParticularSubjectAndTheNameOfTheActivitiesThatAreTaggedofRespectivelessons</t>
+  </si>
+  <si>
+    <t>fc_ViewTheAverageofThelesson</t>
+  </si>
+  <si>
+    <t>fc_ViewDetailsAboutTheSubmissionOfTheofBystudents</t>
+  </si>
+  <si>
+    <t>fc_ViewOverallPerformanceAndSubjectWiseofThestudent</t>
+  </si>
+  <si>
+    <t>fc_ViewActivityWisePerformanceOfTheStudentofParticularlesson</t>
+  </si>
+  <si>
+    <t>f-_ViewRespectiveSubjectsAndRecentActivitiesofAclass</t>
+  </si>
+  <si>
+    <t>f-_ViewTheRespectiveChaptersAndLessonPlansLearningResourcesofAndTest</t>
+  </si>
+  <si>
+    <t>fn_OfofOftext</t>
+  </si>
+  <si>
+    <t>fn_ViewofThelessons</t>
+  </si>
+  <si>
+    <t>fn_ViewTheUsageofThelesson</t>
+  </si>
+  <si>
+    <t>fn_ViewTheChapterofForchapter</t>
+  </si>
+  <si>
+    <t>fn_ViewAllTheAssetsAssociatedofLearningresource</t>
+  </si>
+  <si>
+    <t>fn_FunctionalityToAssignofThestudents</t>
+  </si>
+  <si>
+    <t>fi_OfofOftext</t>
+  </si>
+  <si>
+    <t>fi_FunctionalityToCreateofSelectingchapter</t>
+  </si>
+  <si>
+    <t>fi_FunctionalityofAnotherresources</t>
+  </si>
+  <si>
+    <t>fi_ForMandatoryFieldsOnofPopupwindow</t>
+  </si>
+  <si>
+    <t>fi_FunctionalityofOtherresources</t>
+  </si>
+  <si>
+    <t>fi_FunctionalityToTagMetadataofUploadedlink</t>
+  </si>
+  <si>
+    <t>fi_ValidationsForMandatoryFieldsofPopupwindow</t>
+  </si>
+  <si>
+    <t>fi_FunctionalityToDeleteLearningResourcesByClickingOn'No'InConfirmationPopupofTotalnumber</t>
+  </si>
+  <si>
+    <t>fi_FunctionalityToofPlayedresource</t>
+  </si>
+  <si>
+    <t>fi_FunctionalityToofLearningresource</t>
+  </si>
+  <si>
+    <t>fi_FunctionalityToRemoveofLearningresource</t>
+  </si>
+  <si>
+    <t>fi_FunctionalityToofLessonplayer</t>
+  </si>
+  <si>
+    <t>fi_ViewofAllquestions</t>
+  </si>
+  <si>
+    <t>fi_ViewofRecommendedquestions</t>
+  </si>
+  <si>
+    <t>fi_ViewofCreatedquestions</t>
+  </si>
+  <si>
+    <t>fi_PreviewofRespectivequestion</t>
+  </si>
+  <si>
+    <t>fi_ValidationForMandatoryFieldsofAssessmentwindow</t>
+  </si>
+  <si>
+    <t>fi_CancelofAssessmentwindow</t>
+  </si>
+  <si>
+    <t>f-_ForofMandatoryfield</t>
+  </si>
+  <si>
+    <t>f-_FunctionalityofDeletetest</t>
+  </si>
+  <si>
+    <t>f-_FunctionalityToAssignofAGroup</t>
+  </si>
+  <si>
+    <t>f-_FunctionalityToAssignTestToAFutureDateofToindividuals</t>
+  </si>
+  <si>
+    <t>f-_FunctionalityToAssignTestToAFutureDateAndofAGroup</t>
+  </si>
+  <si>
+    <t>f-_StartTimeCannotBeLessThanCurrentTimeToAssignTestToAofAndtime</t>
+  </si>
+  <si>
+    <t>fd_VisibilityofOndashboard</t>
+  </si>
+  <si>
+    <t>fv_ValidationsofMandatoryfields</t>
+  </si>
+  <si>
+    <t>fv_CancelofEventpopup</t>
+  </si>
+  <si>
+    <t>ft_ViewofLessonplan</t>
+  </si>
+  <si>
+    <t>fe_ViewAllTheLessonPlansofYouTeacher)</t>
+  </si>
+  <si>
+    <t>fe_ViewAllTheofSpecifieddates</t>
+  </si>
+  <si>
+    <t>fe_ViewAllTheActivitiesOfLearningofSpecifieddates</t>
+  </si>
+  <si>
+    <t>fe_ViewTheofStudent'slearning</t>
+  </si>
+  <si>
+    <t>fe_ViewAllTheTestsWithinofDaterange</t>
+  </si>
+  <si>
+    <t>fe_ViewofSubmissiondetails</t>
+  </si>
+  <si>
+    <t>fe_SaveRemarkFeedbackForTheofTestactivity)</t>
+  </si>
+  <si>
+    <t>fe_ViewofTestreport</t>
+  </si>
+  <si>
+    <t>fe_ViewAllTheAssignmentsWithinofDaterange</t>
+  </si>
+  <si>
+    <t>f _MarksEntryLinkofInheader</t>
+  </si>
+  <si>
+    <t>f _FunctionalityToGradeStudentsOnReadingSkillsWritingSkillsSpeakingSkillsAndListeningSkillsAndAlsoToEnterTheMarksScoredInofTermtest</t>
+  </si>
+  <si>
+    <t>f _MarksEntryFeatureIsEnabledOnlyofClassteacher</t>
+  </si>
+  <si>
+    <t>fn_DisplayPracticeTestDetails</t>
+  </si>
+  <si>
+    <t>fn_BookmarkTheResource</t>
+  </si>
+  <si>
+    <t>fi_ForMandatoryFieldsOnAddLinkPopupWindow</t>
+  </si>
+  <si>
+    <t>fi_FunctionalityOfAssessmentGenerationCorrespondingToTheQuestions</t>
+  </si>
+  <si>
+    <t>f-_TeacherIsNotAllowedToRemoveTheTestAfterSubmissionFromTheStudent</t>
+  </si>
+  <si>
+    <t>fL_ViewLessonsPlannedForTheWeek</t>
+  </si>
+  <si>
+    <t>fe_ViewTheStudentResourceMarkingReport</t>
+  </si>
+  <si>
+    <t>fe_EvaluateTheRespectiveTest</t>
+  </si>
+  <si>
+    <t>fe_UploadingWorksheet</t>
+  </si>
+  <si>
+    <t>fn_ViewOverallPerformanceandStudentSubmissionStatusReport</t>
+  </si>
+  <si>
+    <t>fn_ViewTheQuestionAnswerChoicestudentAnswerandrightReport</t>
+  </si>
+  <si>
+    <t>fi_FunctionalityToTagmetadataTotheuploadedSubjec</t>
   </si>
 </sst>
 </file>
@@ -5525,8 +5819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B81" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="E86" workbookViewId="0">
+      <selection activeCell="I86" sqref="I86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7956,8 +8250,8 @@
       <c r="J77" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K77" s="21" t="s">
-        <v>911</v>
+      <c r="K77" t="s">
+        <v>1012</v>
       </c>
       <c r="L77" s="20" t="s">
         <v>1093</v>
@@ -7991,8 +8285,8 @@
       <c r="I78" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="K78" s="21" t="s">
-        <v>911</v>
+      <c r="K78" t="s">
+        <v>1012</v>
       </c>
       <c r="L78" s="20" t="s">
         <v>978</v>
@@ -8026,8 +8320,8 @@
       <c r="J79" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K79" s="21" t="s">
-        <v>911</v>
+      <c r="K79" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="80" spans="1:15" ht="195" x14ac:dyDescent="0.25">
@@ -8055,8 +8349,8 @@
       <c r="I80" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="K80" s="6" t="s">
-        <v>911</v>
+      <c r="K80" t="s">
+        <v>1012</v>
       </c>
       <c r="L80" s="20" t="s">
         <v>936</v>
@@ -8087,8 +8381,8 @@
       <c r="I81" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="K81" s="19" t="s">
-        <v>931</v>
+      <c r="K81" t="s">
+        <v>1012</v>
       </c>
       <c r="L81" s="20" t="s">
         <v>977</v>
@@ -8107,6 +8401,9 @@
       <c r="C82" s="8" t="s">
         <v>347</v>
       </c>
+      <c r="D82" s="8" t="s">
+        <v>1098</v>
+      </c>
       <c r="E82" s="8" t="s">
         <v>349</v>
       </c>
@@ -8119,8 +8416,8 @@
       <c r="I82" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="K82" s="6" t="s">
-        <v>911</v>
+      <c r="K82" t="s">
+        <v>1012</v>
       </c>
       <c r="L82" s="8" t="s">
         <v>937</v>
@@ -8136,6 +8433,9 @@
       <c r="C83" s="8" t="s">
         <v>347</v>
       </c>
+      <c r="D83" s="8" t="s">
+        <v>1126</v>
+      </c>
       <c r="E83" s="8" t="s">
         <v>352</v>
       </c>
@@ -8151,8 +8451,8 @@
       <c r="J83" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K83" s="6" t="s">
-        <v>911</v>
+      <c r="K83" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="195" x14ac:dyDescent="0.25">
@@ -8165,6 +8465,9 @@
       <c r="C84" s="8" t="s">
         <v>347</v>
       </c>
+      <c r="D84" s="8" t="s">
+        <v>1184</v>
+      </c>
       <c r="E84" s="8" t="s">
         <v>355</v>
       </c>
@@ -8194,6 +8497,9 @@
       <c r="C85" s="8" t="s">
         <v>347</v>
       </c>
+      <c r="D85" s="8" t="s">
+        <v>1193</v>
+      </c>
       <c r="E85" s="8" t="s">
         <v>360</v>
       </c>
@@ -8223,6 +8529,9 @@
       <c r="C86" s="8" t="s">
         <v>347</v>
       </c>
+      <c r="D86" s="8" t="s">
+        <v>1194</v>
+      </c>
       <c r="E86" s="8" t="s">
         <v>364</v>
       </c>
@@ -8306,6 +8615,9 @@
       <c r="C89" s="8" t="s">
         <v>377</v>
       </c>
+      <c r="D89" s="8" t="s">
+        <v>1103</v>
+      </c>
       <c r="E89" s="8" t="s">
         <v>382</v>
       </c>
@@ -8330,6 +8642,9 @@
       <c r="C90" s="8" t="s">
         <v>904</v>
       </c>
+      <c r="D90" s="8" t="s">
+        <v>1127</v>
+      </c>
       <c r="E90" s="8" t="s">
         <v>890</v>
       </c>
@@ -8379,6 +8694,9 @@
       <c r="C92" s="8" t="s">
         <v>896</v>
       </c>
+      <c r="D92" s="8" t="s">
+        <v>1128</v>
+      </c>
       <c r="E92" s="8" t="s">
         <v>897</v>
       </c>
@@ -8402,6 +8720,9 @@
       <c r="C93" s="8" t="s">
         <v>900</v>
       </c>
+      <c r="D93" s="8" t="s">
+        <v>1129</v>
+      </c>
       <c r="E93" s="8" t="s">
         <v>901</v>
       </c>
@@ -8425,6 +8746,9 @@
       <c r="C94" s="8" t="s">
         <v>381</v>
       </c>
+      <c r="D94" s="8" t="s">
+        <v>1130</v>
+      </c>
       <c r="E94" s="8" t="s">
         <v>384</v>
       </c>
@@ -8454,6 +8778,9 @@
       <c r="C95" s="8" t="s">
         <v>381</v>
       </c>
+      <c r="D95" s="8" t="s">
+        <v>1131</v>
+      </c>
       <c r="E95" s="8" t="s">
         <v>386</v>
       </c>
@@ -8483,6 +8810,9 @@
       <c r="C96" s="8" t="s">
         <v>381</v>
       </c>
+      <c r="D96" s="8" t="s">
+        <v>1132</v>
+      </c>
       <c r="E96" s="8" t="s">
         <v>390</v>
       </c>
@@ -8512,6 +8842,9 @@
       <c r="C97" s="8" t="s">
         <v>381</v>
       </c>
+      <c r="D97" s="8" t="s">
+        <v>1133</v>
+      </c>
       <c r="E97" s="8" t="s">
         <v>394</v>
       </c>
@@ -8541,6 +8874,9 @@
       <c r="C98" s="8" t="s">
         <v>381</v>
       </c>
+      <c r="D98" s="8" t="s">
+        <v>1134</v>
+      </c>
       <c r="E98" s="8" t="s">
         <v>398</v>
       </c>
@@ -8599,6 +8935,9 @@
       <c r="C100" s="8" t="s">
         <v>381</v>
       </c>
+      <c r="D100" s="8" t="s">
+        <v>1135</v>
+      </c>
       <c r="E100" s="8" t="s">
         <v>407</v>
       </c>
@@ -8618,7 +8957,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>435</v>
       </c>
@@ -8628,6 +8967,9 @@
       <c r="C101" s="6" t="s">
         <v>414</v>
       </c>
+      <c r="D101" s="8" t="s">
+        <v>1136</v>
+      </c>
       <c r="E101" s="8" t="s">
         <v>412</v>
       </c>
@@ -8647,7 +8989,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>437</v>
       </c>
@@ -8656,6 +8998,9 @@
       </c>
       <c r="C102" s="6" t="s">
         <v>414</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>1137</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>416</v>
@@ -8686,6 +9031,9 @@
       <c r="C103" s="8" t="s">
         <v>425</v>
       </c>
+      <c r="D103" s="8" t="s">
+        <v>1138</v>
+      </c>
       <c r="E103" s="8" t="s">
         <v>424</v>
       </c>
@@ -8715,6 +9063,9 @@
       <c r="C104" s="8" t="s">
         <v>422</v>
       </c>
+      <c r="D104" s="8" t="s">
+        <v>1139</v>
+      </c>
       <c r="E104" s="8" t="s">
         <v>427</v>
       </c>
@@ -8744,6 +9095,9 @@
       <c r="C105" s="8" t="s">
         <v>422</v>
       </c>
+      <c r="D105" s="8" t="s">
+        <v>1140</v>
+      </c>
       <c r="E105" s="8" t="s">
         <v>429</v>
       </c>
@@ -8773,6 +9127,9 @@
       <c r="C106" s="8" t="s">
         <v>422</v>
       </c>
+      <c r="D106" s="8" t="s">
+        <v>1141</v>
+      </c>
       <c r="E106" s="8" t="s">
         <v>436</v>
       </c>
@@ -8828,6 +9185,9 @@
       <c r="C108" s="8" t="s">
         <v>442</v>
       </c>
+      <c r="D108" s="8" t="s">
+        <v>1104</v>
+      </c>
       <c r="E108" s="6" t="s">
         <v>443</v>
       </c>
@@ -8857,6 +9217,9 @@
       <c r="C109" s="8" t="s">
         <v>442</v>
       </c>
+      <c r="D109" s="8" t="s">
+        <v>1142</v>
+      </c>
       <c r="E109" s="8" t="s">
         <v>446</v>
       </c>
@@ -8886,6 +9249,9 @@
       <c r="C110" s="8" t="s">
         <v>442</v>
       </c>
+      <c r="D110" s="8" t="s">
+        <v>1105</v>
+      </c>
       <c r="E110" s="8" t="s">
         <v>451</v>
       </c>
@@ -8915,6 +9281,9 @@
       <c r="C111" s="8" t="s">
         <v>442</v>
       </c>
+      <c r="D111" s="8" t="s">
+        <v>1185</v>
+      </c>
       <c r="E111" s="8" t="s">
         <v>455</v>
       </c>
@@ -8941,6 +9310,9 @@
       <c r="C112" s="8" t="s">
         <v>458</v>
       </c>
+      <c r="D112" s="8" t="s">
+        <v>1106</v>
+      </c>
       <c r="E112" s="6" t="s">
         <v>460</v>
       </c>
@@ -8967,6 +9339,9 @@
       <c r="C113" s="8" t="s">
         <v>458</v>
       </c>
+      <c r="D113" s="8" t="s">
+        <v>1107</v>
+      </c>
       <c r="E113" s="8" t="s">
         <v>620</v>
       </c>
@@ -8993,6 +9368,9 @@
       <c r="C114" s="8" t="s">
         <v>458</v>
       </c>
+      <c r="D114" s="8" t="s">
+        <v>1108</v>
+      </c>
       <c r="E114" s="8" t="s">
         <v>621</v>
       </c>
@@ -9019,6 +9397,9 @@
       <c r="C115" s="8" t="s">
         <v>464</v>
       </c>
+      <c r="D115" s="8" t="s">
+        <v>1109</v>
+      </c>
       <c r="E115" s="8" t="s">
         <v>465</v>
       </c>
@@ -9045,6 +9426,9 @@
       <c r="C116" s="8" t="s">
         <v>468</v>
       </c>
+      <c r="D116" s="8" t="s">
+        <v>1110</v>
+      </c>
       <c r="E116" s="8" t="s">
         <v>471</v>
       </c>
@@ -9071,6 +9455,9 @@
       <c r="C117" s="8" t="s">
         <v>472</v>
       </c>
+      <c r="D117" s="8" t="s">
+        <v>1143</v>
+      </c>
       <c r="E117" s="8" t="s">
         <v>474</v>
       </c>
@@ -9097,6 +9484,9 @@
       <c r="C118" s="8" t="s">
         <v>481</v>
       </c>
+      <c r="D118" s="8" t="s">
+        <v>1144</v>
+      </c>
       <c r="E118" s="8" t="s">
         <v>424</v>
       </c>
@@ -9126,6 +9516,9 @@
       <c r="C119" s="9" t="s">
         <v>477</v>
       </c>
+      <c r="D119" s="8" t="s">
+        <v>1111</v>
+      </c>
       <c r="E119" s="8" t="s">
         <v>478</v>
       </c>
@@ -9155,6 +9548,9 @@
       <c r="C120" s="8" t="s">
         <v>486</v>
       </c>
+      <c r="D120" s="8" t="s">
+        <v>1112</v>
+      </c>
       <c r="E120" s="8" t="s">
         <v>487</v>
       </c>
@@ -9184,6 +9580,9 @@
       <c r="C121" s="8" t="s">
         <v>490</v>
       </c>
+      <c r="D121" s="8" t="s">
+        <v>1112</v>
+      </c>
       <c r="E121" s="8" t="s">
         <v>491</v>
       </c>
@@ -9213,6 +9612,9 @@
       <c r="C122" s="8" t="s">
         <v>490</v>
       </c>
+      <c r="D122" s="8" t="s">
+        <v>1113</v>
+      </c>
       <c r="E122" s="8" t="s">
         <v>495</v>
       </c>
@@ -9277,6 +9679,9 @@
       <c r="C124" s="8" t="s">
         <v>498</v>
       </c>
+      <c r="D124" s="8" t="s">
+        <v>1145</v>
+      </c>
       <c r="E124" s="8" t="s">
         <v>505</v>
       </c>
@@ -9306,6 +9711,9 @@
       <c r="C125" s="8" t="s">
         <v>498</v>
       </c>
+      <c r="D125" s="8" t="s">
+        <v>1186</v>
+      </c>
       <c r="E125" s="8" t="s">
         <v>508</v>
       </c>
@@ -9339,6 +9747,9 @@
       <c r="C126" s="8" t="s">
         <v>498</v>
       </c>
+      <c r="D126" s="8" t="s">
+        <v>1146</v>
+      </c>
       <c r="E126" s="8" t="s">
         <v>513</v>
       </c>
@@ -9369,6 +9780,9 @@
       <c r="C127" s="8" t="s">
         <v>498</v>
       </c>
+      <c r="D127" s="8" t="s">
+        <v>1195</v>
+      </c>
       <c r="E127" s="8" t="s">
         <v>521</v>
       </c>
@@ -9434,6 +9848,9 @@
       <c r="C129" s="8" t="s">
         <v>517</v>
       </c>
+      <c r="D129" s="8" t="s">
+        <v>1145</v>
+      </c>
       <c r="E129" s="8" t="s">
         <v>525</v>
       </c>
@@ -9463,6 +9880,9 @@
       <c r="C130" s="8" t="s">
         <v>517</v>
       </c>
+      <c r="D130" s="8" t="s">
+        <v>1147</v>
+      </c>
       <c r="E130" s="8" t="s">
         <v>528</v>
       </c>
@@ -9493,6 +9913,9 @@
       <c r="C131" s="8" t="s">
         <v>517</v>
       </c>
+      <c r="D131" s="8" t="s">
+        <v>1148</v>
+      </c>
       <c r="E131" s="8" t="s">
         <v>533</v>
       </c>
@@ -9523,6 +9946,9 @@
       <c r="C132" s="8" t="s">
         <v>517</v>
       </c>
+      <c r="D132" s="8" t="s">
+        <v>1149</v>
+      </c>
       <c r="E132" s="8" t="s">
         <v>521</v>
       </c>
@@ -9585,6 +10011,9 @@
       <c r="C134" s="8" t="s">
         <v>540</v>
       </c>
+      <c r="D134" s="8" t="s">
+        <v>1150</v>
+      </c>
       <c r="E134" s="8" t="s">
         <v>548</v>
       </c>
@@ -9615,6 +10044,9 @@
       <c r="C135" s="8" t="s">
         <v>552</v>
       </c>
+      <c r="D135" s="8" t="s">
+        <v>1112</v>
+      </c>
       <c r="E135" s="8" t="s">
         <v>553</v>
       </c>
@@ -9644,6 +10076,9 @@
       <c r="C136" s="8" t="s">
         <v>552</v>
       </c>
+      <c r="D136" s="8" t="s">
+        <v>1151</v>
+      </c>
       <c r="E136" s="8" t="s">
         <v>557</v>
       </c>
@@ -9673,6 +10108,9 @@
       <c r="C137" s="8" t="s">
         <v>561</v>
       </c>
+      <c r="D137" s="8" t="s">
+        <v>1114</v>
+      </c>
       <c r="E137" s="8" t="s">
         <v>562</v>
       </c>
@@ -9702,6 +10140,9 @@
       <c r="C138" s="8" t="s">
         <v>561</v>
       </c>
+      <c r="D138" s="8" t="s">
+        <v>1152</v>
+      </c>
       <c r="E138" s="8" t="s">
         <v>565</v>
       </c>
@@ -9731,6 +10172,9 @@
       <c r="C139" s="8" t="s">
         <v>561</v>
       </c>
+      <c r="D139" s="8" t="s">
+        <v>1153</v>
+      </c>
       <c r="E139" s="8" t="s">
         <v>568</v>
       </c>
@@ -9760,6 +10204,9 @@
       <c r="C140" s="8" t="s">
         <v>561</v>
       </c>
+      <c r="D140" s="8" t="s">
+        <v>1154</v>
+      </c>
       <c r="E140" s="8" t="s">
         <v>572</v>
       </c>
@@ -9789,6 +10236,9 @@
       <c r="C141" s="8" t="s">
         <v>561</v>
       </c>
+      <c r="D141" s="8" t="s">
+        <v>1155</v>
+      </c>
       <c r="E141" s="8" t="s">
         <v>576</v>
       </c>
@@ -9818,6 +10268,9 @@
       <c r="C142" s="8" t="s">
         <v>581</v>
       </c>
+      <c r="D142" s="8" t="s">
+        <v>1156</v>
+      </c>
       <c r="E142" s="6" t="s">
         <v>582</v>
       </c>
@@ -9847,6 +10300,9 @@
       <c r="C143" s="8" t="s">
         <v>581</v>
       </c>
+      <c r="D143" s="8" t="s">
+        <v>1157</v>
+      </c>
       <c r="E143" s="8" t="s">
         <v>625</v>
       </c>
@@ -9876,6 +10332,9 @@
       <c r="C144" s="8" t="s">
         <v>581</v>
       </c>
+      <c r="D144" s="8" t="s">
+        <v>1158</v>
+      </c>
       <c r="E144" s="8" t="s">
         <v>628</v>
       </c>
@@ -9905,6 +10364,9 @@
       <c r="C145" s="8" t="s">
         <v>581</v>
       </c>
+      <c r="D145" s="8" t="s">
+        <v>1159</v>
+      </c>
       <c r="E145" s="8" t="s">
         <v>586</v>
       </c>
@@ -9934,6 +10396,9 @@
       <c r="C146" s="8" t="s">
         <v>594</v>
       </c>
+      <c r="D146" s="8" t="s">
+        <v>1187</v>
+      </c>
       <c r="E146" s="8" t="s">
         <v>593</v>
       </c>
@@ -9966,6 +10431,9 @@
       <c r="C147" s="8" t="s">
         <v>595</v>
       </c>
+      <c r="D147" s="8" t="s">
+        <v>1160</v>
+      </c>
       <c r="E147" s="8" t="s">
         <v>596</v>
       </c>
@@ -9995,6 +10463,9 @@
       <c r="C148" s="8" t="s">
         <v>595</v>
       </c>
+      <c r="D148" s="8" t="s">
+        <v>1161</v>
+      </c>
       <c r="E148" s="8" t="s">
         <v>600</v>
       </c>
@@ -10056,6 +10527,9 @@
       <c r="C150" s="8" t="s">
         <v>595</v>
       </c>
+      <c r="D150" s="8" t="s">
+        <v>1115</v>
+      </c>
       <c r="E150" s="8" t="s">
         <v>609</v>
       </c>
@@ -10085,6 +10559,9 @@
       <c r="C151" s="8" t="s">
         <v>595</v>
       </c>
+      <c r="D151" s="8" t="s">
+        <v>1161</v>
+      </c>
       <c r="E151" s="8" t="s">
         <v>612</v>
       </c>
@@ -10381,6 +10858,9 @@
       <c r="C161" s="6" t="s">
         <v>665</v>
       </c>
+      <c r="D161" s="8" t="s">
+        <v>1162</v>
+      </c>
       <c r="E161" s="8" t="s">
         <v>694</v>
       </c>
@@ -10443,6 +10923,9 @@
       <c r="C163" s="6" t="s">
         <v>665</v>
       </c>
+      <c r="D163" s="8" t="s">
+        <v>1116</v>
+      </c>
       <c r="E163" s="8" t="s">
         <v>675</v>
       </c>
@@ -10472,6 +10955,9 @@
       <c r="C164" s="6" t="s">
         <v>665</v>
       </c>
+      <c r="D164" s="8" t="s">
+        <v>1117</v>
+      </c>
       <c r="E164" s="8" t="s">
         <v>679</v>
       </c>
@@ -10501,6 +10987,9 @@
       <c r="C165" s="6" t="s">
         <v>665</v>
       </c>
+      <c r="D165" s="8" t="s">
+        <v>1118</v>
+      </c>
       <c r="E165" s="8" t="s">
         <v>683</v>
       </c>
@@ -10530,6 +11019,9 @@
       <c r="C166" s="6" t="s">
         <v>665</v>
       </c>
+      <c r="D166" s="8" t="s">
+        <v>1119</v>
+      </c>
       <c r="E166" s="8" t="s">
         <v>687</v>
       </c>
@@ -10559,6 +11051,9 @@
       <c r="C167" s="6" t="s">
         <v>665</v>
       </c>
+      <c r="D167" s="8" t="s">
+        <v>1120</v>
+      </c>
       <c r="E167" s="8" t="s">
         <v>691</v>
       </c>
@@ -10588,6 +11083,9 @@
       <c r="C168" s="6" t="s">
         <v>699</v>
       </c>
+      <c r="D168" s="8" t="s">
+        <v>1188</v>
+      </c>
       <c r="E168" s="8" t="s">
         <v>700</v>
       </c>
@@ -10614,6 +11112,9 @@
       <c r="C169" s="6" t="s">
         <v>699</v>
       </c>
+      <c r="D169" s="8" t="s">
+        <v>1163</v>
+      </c>
       <c r="E169" s="8" t="s">
         <v>704</v>
       </c>
@@ -10643,6 +11144,9 @@
       <c r="C170" s="6" t="s">
         <v>699</v>
       </c>
+      <c r="D170" s="8" t="s">
+        <v>1121</v>
+      </c>
       <c r="E170" s="8" t="s">
         <v>707</v>
       </c>
@@ -10672,6 +11176,9 @@
       <c r="C171" s="6" t="s">
         <v>699</v>
       </c>
+      <c r="D171" s="8" t="s">
+        <v>1122</v>
+      </c>
       <c r="E171" s="8" t="s">
         <v>710</v>
       </c>
@@ -10730,6 +11237,9 @@
       <c r="C173" s="6" t="s">
         <v>713</v>
       </c>
+      <c r="D173" s="8" t="s">
+        <v>1164</v>
+      </c>
       <c r="E173" s="8" t="s">
         <v>718</v>
       </c>
@@ -10759,6 +11269,9 @@
       <c r="C174" s="6" t="s">
         <v>713</v>
       </c>
+      <c r="D174" s="8" t="s">
+        <v>1165</v>
+      </c>
       <c r="E174" s="8" t="s">
         <v>722</v>
       </c>
@@ -10788,6 +11301,9 @@
       <c r="C175" s="6" t="s">
         <v>713</v>
       </c>
+      <c r="D175" s="8" t="s">
+        <v>1166</v>
+      </c>
       <c r="E175" s="8" t="s">
         <v>726</v>
       </c>
@@ -10816,6 +11332,9 @@
       </c>
       <c r="C176" s="10" t="s">
         <v>713</v>
+      </c>
+      <c r="D176" s="8" t="s">
+        <v>1167</v>
       </c>
       <c r="E176" s="10" t="s">
         <v>731</v>
@@ -10863,6 +11382,9 @@
       <c r="C177" s="10" t="s">
         <v>735</v>
       </c>
+      <c r="D177" s="8" t="s">
+        <v>1168</v>
+      </c>
       <c r="E177" s="14" t="s">
         <v>748</v>
       </c>
@@ -10938,6 +11460,9 @@
       <c r="C179" s="8" t="s">
         <v>736</v>
       </c>
+      <c r="D179" s="8" t="s">
+        <v>1189</v>
+      </c>
       <c r="E179" s="8" t="s">
         <v>741</v>
       </c>
@@ -10970,6 +11495,9 @@
       <c r="C180" s="8" t="s">
         <v>736</v>
       </c>
+      <c r="D180" s="8" t="s">
+        <v>1099</v>
+      </c>
       <c r="E180" s="8" t="s">
         <v>745</v>
       </c>
@@ -11072,6 +11600,9 @@
       <c r="C183" s="6" t="s">
         <v>753</v>
       </c>
+      <c r="D183" s="8" t="s">
+        <v>1169</v>
+      </c>
       <c r="E183" s="8" t="s">
         <v>764</v>
       </c>
@@ -11101,6 +11632,9 @@
       <c r="C184" s="6" t="s">
         <v>753</v>
       </c>
+      <c r="D184" s="8" t="s">
+        <v>1123</v>
+      </c>
       <c r="E184" s="8" t="s">
         <v>768</v>
       </c>
@@ -11130,6 +11664,9 @@
       <c r="C185" s="6" t="s">
         <v>753</v>
       </c>
+      <c r="D185" s="8" t="s">
+        <v>1123</v>
+      </c>
       <c r="E185" s="8" t="s">
         <v>768</v>
       </c>
@@ -11160,6 +11697,9 @@
       <c r="C186" s="6" t="s">
         <v>753</v>
       </c>
+      <c r="D186" s="8" t="s">
+        <v>1123</v>
+      </c>
       <c r="E186" s="8" t="s">
         <v>768</v>
       </c>
@@ -11190,6 +11730,9 @@
       <c r="C187" s="6" t="s">
         <v>753</v>
       </c>
+      <c r="D187" s="8" t="s">
+        <v>1170</v>
+      </c>
       <c r="E187" s="8" t="s">
         <v>776</v>
       </c>
@@ -11219,6 +11762,9 @@
       <c r="C188" s="8" t="s">
         <v>779</v>
       </c>
+      <c r="D188" s="8" t="s">
+        <v>1124</v>
+      </c>
       <c r="E188" s="6" t="s">
         <v>786</v>
       </c>
@@ -11248,6 +11794,9 @@
       <c r="C189" s="8" t="s">
         <v>784</v>
       </c>
+      <c r="D189" s="8" t="s">
+        <v>1171</v>
+      </c>
       <c r="E189" s="6" t="s">
         <v>785</v>
       </c>
@@ -11277,6 +11826,9 @@
       <c r="C190" s="8" t="s">
         <v>790</v>
       </c>
+      <c r="D190" s="8" t="s">
+        <v>1100</v>
+      </c>
       <c r="E190" s="8" t="s">
         <v>791</v>
       </c>
@@ -11306,6 +11858,9 @@
       <c r="C191" s="8" t="s">
         <v>796</v>
       </c>
+      <c r="D191" s="8" t="s">
+        <v>1101</v>
+      </c>
       <c r="E191" s="8" t="s">
         <v>795</v>
       </c>
@@ -11335,6 +11890,9 @@
       <c r="C192" s="8" t="s">
         <v>796</v>
       </c>
+      <c r="D192" s="8" t="s">
+        <v>1102</v>
+      </c>
       <c r="E192" s="8" t="s">
         <v>800</v>
       </c>
@@ -11357,7 +11915,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="193" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="6" t="s">
         <v>822</v>
       </c>
@@ -11367,6 +11925,9 @@
       <c r="C193" s="8" t="s">
         <v>805</v>
       </c>
+      <c r="D193" s="8" t="s">
+        <v>1125</v>
+      </c>
       <c r="E193" s="8" t="s">
         <v>806</v>
       </c>
@@ -11386,7 +11947,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="194" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="6" t="s">
         <v>825</v>
       </c>
@@ -11395,6 +11956,9 @@
       </c>
       <c r="C194" s="8" t="s">
         <v>805</v>
+      </c>
+      <c r="D194" s="8" t="s">
+        <v>1172</v>
       </c>
       <c r="E194" s="8" t="s">
         <v>809</v>
@@ -11425,6 +11989,9 @@
       <c r="C195" s="8" t="s">
         <v>805</v>
       </c>
+      <c r="D195" s="8" t="s">
+        <v>1173</v>
+      </c>
       <c r="E195" s="8" t="s">
         <v>814</v>
       </c>
@@ -11454,6 +12021,9 @@
       <c r="C196" s="8" t="s">
         <v>805</v>
       </c>
+      <c r="D196" s="8" t="s">
+        <v>1174</v>
+      </c>
       <c r="E196" s="8" t="s">
         <v>826</v>
       </c>
@@ -11483,6 +12053,9 @@
       <c r="C197" s="8" t="s">
         <v>805</v>
       </c>
+      <c r="D197" s="8" t="s">
+        <v>1190</v>
+      </c>
       <c r="E197" s="8" t="s">
         <v>820</v>
       </c>
@@ -11515,6 +12088,9 @@
       <c r="C198" s="8" t="s">
         <v>805</v>
       </c>
+      <c r="D198" s="8" t="s">
+        <v>1175</v>
+      </c>
       <c r="E198" s="8" t="s">
         <v>823</v>
       </c>
@@ -11544,6 +12120,9 @@
       <c r="C199" s="8" t="s">
         <v>805</v>
       </c>
+      <c r="D199" s="8" t="s">
+        <v>1176</v>
+      </c>
       <c r="E199" s="8" t="s">
         <v>830</v>
       </c>
@@ -11573,6 +12152,9 @@
       <c r="C200" s="8" t="s">
         <v>805</v>
       </c>
+      <c r="D200" s="8" t="s">
+        <v>1177</v>
+      </c>
       <c r="E200" s="8" t="s">
         <v>837</v>
       </c>
@@ -11602,6 +12184,9 @@
       <c r="C201" s="8" t="s">
         <v>805</v>
       </c>
+      <c r="D201" s="8" t="s">
+        <v>1178</v>
+      </c>
       <c r="E201" s="8" t="s">
         <v>838</v>
       </c>
@@ -11631,6 +12216,9 @@
       <c r="C202" s="8" t="s">
         <v>805</v>
       </c>
+      <c r="D202" s="8" t="s">
+        <v>1179</v>
+      </c>
       <c r="E202" s="8" t="s">
         <v>842</v>
       </c>
@@ -11660,6 +12248,9 @@
       <c r="C203" s="8" t="s">
         <v>805</v>
       </c>
+      <c r="D203" s="8" t="s">
+        <v>1191</v>
+      </c>
       <c r="E203" s="8" t="s">
         <v>846</v>
       </c>
@@ -11689,6 +12280,9 @@
       <c r="C204" s="8" t="s">
         <v>805</v>
       </c>
+      <c r="D204" s="8" t="s">
+        <v>1192</v>
+      </c>
       <c r="E204" s="8" t="s">
         <v>850</v>
       </c>
@@ -11718,6 +12312,9 @@
       <c r="C205" s="8" t="s">
         <v>805</v>
       </c>
+      <c r="D205" s="8" t="s">
+        <v>1180</v>
+      </c>
       <c r="E205" s="8" t="s">
         <v>855</v>
       </c>
@@ -11747,6 +12344,9 @@
       <c r="C206" s="8" t="s">
         <v>805</v>
       </c>
+      <c r="D206" s="8" t="s">
+        <v>1177</v>
+      </c>
       <c r="E206" s="8" t="s">
         <v>862</v>
       </c>
@@ -11859,7 +12459,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="210" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A210" s="6" t="s">
         <v>907</v>
       </c>
@@ -11868,6 +12468,9 @@
       </c>
       <c r="C210" s="6" t="s">
         <v>874</v>
+      </c>
+      <c r="D210" s="8" t="s">
+        <v>1181</v>
       </c>
       <c r="E210" s="8" t="s">
         <v>879</v>
@@ -11898,6 +12501,9 @@
       <c r="C211" s="8" t="s">
         <v>875</v>
       </c>
+      <c r="D211" s="8" t="s">
+        <v>1182</v>
+      </c>
       <c r="E211" s="8" t="s">
         <v>876</v>
       </c>
@@ -11917,7 +12523,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="212" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A212" s="6" t="s">
         <v>917</v>
       </c>
@@ -11926,6 +12532,9 @@
       </c>
       <c r="C212" s="8" t="s">
         <v>885</v>
+      </c>
+      <c r="D212" s="8" t="s">
+        <v>1183</v>
       </c>
       <c r="E212" s="8" t="s">
         <v>886</v>

</xml_diff>

<commit_message>
Started Learning resources section...
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3944" uniqueCount="1198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3949" uniqueCount="1202">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5065,24 +5065,6 @@
     <t>fA_AddRemarkforstudent'sFeedbackofView</t>
   </si>
   <si>
-    <t>fn_ViewofLessonPlan</t>
-  </si>
-  <si>
-    <t>fn_ViewofRecommendedLesson</t>
-  </si>
-  <si>
-    <t>fn_ViewofMyLessons</t>
-  </si>
-  <si>
-    <t>fn_FunctionalityofPlanLessons</t>
-  </si>
-  <si>
-    <t>fn_FunctionalityToDeleteofMyLessons)</t>
-  </si>
-  <si>
-    <t>fi_FunctionalityofLearningResource</t>
-  </si>
-  <si>
     <t>fi_FunctionalityofLearningResources</t>
   </si>
   <si>
@@ -5128,12 +5110,6 @@
     <t>fn_ViewAverageScoreofSelectedSubject</t>
   </si>
   <si>
-    <t>fn_FunctionalityToAssignofThestudents</t>
-  </si>
-  <si>
-    <t>fi_OfofOftext</t>
-  </si>
-  <si>
     <t>fi_FunctionalityToCreateofSelectingchapter</t>
   </si>
   <si>
@@ -5348,6 +5324,42 @@
   </si>
   <si>
     <t>fn_BookmarktheResource</t>
+  </si>
+  <si>
+    <t>fn_ViewLessonPlan</t>
+  </si>
+  <si>
+    <t>fn_ViewRecommendedLesson</t>
+  </si>
+  <si>
+    <t>fn_ViewMyLessons</t>
+  </si>
+  <si>
+    <t>fn_PlanLessons</t>
+  </si>
+  <si>
+    <t>fn_DeleteMyLessons</t>
+  </si>
+  <si>
+    <t>fn_AddLessonPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lesson Plans-Add Plan Lessons </t>
+  </si>
+  <si>
+    <t>fn_AssignLessonToStudents</t>
+  </si>
+  <si>
+    <t>fn_VisibilityofLearningResourceText</t>
+  </si>
+  <si>
+    <t>fn_PreviewLearningResource</t>
+  </si>
+  <si>
+    <t>fn_FilterLearningResources</t>
+  </si>
+  <si>
+    <t>fn_SearchLearningResources</t>
   </si>
 </sst>
 </file>
@@ -5823,10 +5835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA209"/>
+  <dimension ref="A1:AA210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8440,7 +8452,7 @@
         <v>347</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>1123</v>
+        <v>1117</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>352</v>
@@ -8472,7 +8484,7 @@
         <v>347</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>1165</v>
+        <v>1157</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>355</v>
@@ -8504,7 +8516,7 @@
         <v>347</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>1173</v>
+        <v>1165</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>360</v>
@@ -8536,7 +8548,7 @@
         <v>347</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>1174</v>
+        <v>1166</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>364</v>
@@ -8568,7 +8580,7 @@
         <v>368</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>1176</v>
+        <v>1168</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>370</v>
@@ -8600,7 +8612,7 @@
         <v>368</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>1177</v>
+        <v>1169</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>374</v>
@@ -8630,7 +8642,7 @@
         <v>377</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>1178</v>
+        <v>1170</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>382</v>
@@ -8659,7 +8671,7 @@
         <v>381</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>1179</v>
+        <v>1171</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>384</v>
@@ -8691,7 +8703,7 @@
         <v>381</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>1180</v>
+        <v>1172</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>386</v>
@@ -8723,7 +8735,7 @@
         <v>381</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>1181</v>
+        <v>1173</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>390</v>
@@ -8755,7 +8767,7 @@
         <v>381</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>1182</v>
+        <v>1174</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>394</v>
@@ -8787,7 +8799,7 @@
         <v>381</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>1183</v>
+        <v>1175</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>398</v>
@@ -8819,7 +8831,7 @@
         <v>381</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>1184</v>
+        <v>1176</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>403</v>
@@ -8851,7 +8863,7 @@
         <v>381</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>1185</v>
+        <v>1177</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>407</v>
@@ -8883,7 +8895,7 @@
         <v>414</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>1186</v>
+        <v>1178</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>412</v>
@@ -8915,7 +8927,7 @@
         <v>414</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>1187</v>
+        <v>1179</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>416</v>
@@ -8947,7 +8959,7 @@
         <v>425</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>1188</v>
+        <v>1180</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>424</v>
@@ -8979,7 +8991,7 @@
         <v>422</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>1189</v>
+        <v>1181</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>427</v>
@@ -9011,7 +9023,7 @@
         <v>422</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>1190</v>
+        <v>1182</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>429</v>
@@ -9032,7 +9044,7 @@
         <v>1012</v>
       </c>
       <c r="L101" s="8" t="s">
-        <v>1191</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="195" x14ac:dyDescent="0.25">
@@ -9046,7 +9058,7 @@
         <v>422</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>1192</v>
+        <v>1184</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>436</v>
@@ -9078,7 +9090,7 @@
         <v>422</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
       <c r="E103" s="8" t="s">
         <v>438</v>
@@ -9107,7 +9119,7 @@
         <v>442</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>1194</v>
+        <v>1186</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>443</v>
@@ -9139,7 +9151,7 @@
         <v>442</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>1195</v>
+        <v>1187</v>
       </c>
       <c r="E105" s="8" t="s">
         <v>446</v>
@@ -9171,7 +9183,7 @@
         <v>442</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>1196</v>
+        <v>1188</v>
       </c>
       <c r="E106" s="8" t="s">
         <v>451</v>
@@ -9203,7 +9215,7 @@
         <v>442</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>1197</v>
+        <v>1189</v>
       </c>
       <c r="E107" s="8" t="s">
         <v>455</v>
@@ -9232,7 +9244,7 @@
         <v>458</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>1103</v>
+        <v>1190</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>460</v>
@@ -9261,7 +9273,7 @@
         <v>458</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>1104</v>
+        <v>1191</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>620</v>
@@ -9275,8 +9287,8 @@
       <c r="J109" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K109" s="6" t="s">
-        <v>911</v>
+      <c r="K109" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="110" spans="1:12" ht="135" x14ac:dyDescent="0.25">
@@ -9290,7 +9302,7 @@
         <v>458</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>1105</v>
+        <v>1192</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>621</v>
@@ -9304,8 +9316,8 @@
       <c r="J110" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K110" s="6" t="s">
-        <v>911</v>
+      <c r="K110" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="111" spans="1:12" ht="150" x14ac:dyDescent="0.25">
@@ -9319,7 +9331,7 @@
         <v>464</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>1106</v>
+        <v>1193</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>465</v>
@@ -9333,11 +9345,11 @@
       <c r="J111" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K111" s="6" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="K111" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
         <v>480</v>
       </c>
@@ -9345,28 +9357,19 @@
         <v>411</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>468</v>
+        <v>1196</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>1107</v>
-      </c>
-      <c r="E112" s="8" t="s">
-        <v>471</v>
-      </c>
-      <c r="G112" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="I112" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="J112" s="6" t="s">
-        <v>972</v>
-      </c>
-      <c r="K112" s="6" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="113" spans="1:12" ht="210" x14ac:dyDescent="0.25">
+        <v>1195</v>
+      </c>
+      <c r="E112" s="8"/>
+      <c r="G112" s="2"/>
+      <c r="I112" s="2"/>
+      <c r="K112" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
         <v>484</v>
       </c>
@@ -9374,28 +9377,28 @@
         <v>411</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>1124</v>
+        <v>1194</v>
       </c>
       <c r="E113" s="8" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="I113" s="2" t="s">
-        <v>476</v>
+        <v>470</v>
+      </c>
+      <c r="J113" s="6" t="s">
+        <v>972</v>
       </c>
       <c r="K113" s="6" t="s">
         <v>911</v>
       </c>
-      <c r="L113" s="8" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="114" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:12" ht="210" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
         <v>485</v>
       </c>
@@ -9403,54 +9406,51 @@
         <v>411</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>1125</v>
+        <v>1197</v>
       </c>
       <c r="E114" s="8" t="s">
-        <v>424</v>
-      </c>
-      <c r="F114" s="6" t="s">
-        <v>38</v>
+        <v>474</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>418</v>
+        <v>475</v>
       </c>
       <c r="I114" s="2" t="s">
-        <v>947</v>
-      </c>
-      <c r="J114" s="6" t="s">
-        <v>972</v>
-      </c>
-      <c r="K114" s="6" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="115" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+        <v>476</v>
+      </c>
+      <c r="K114" t="s">
+        <v>1012</v>
+      </c>
+      <c r="L114" s="8" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
         <v>494</v>
       </c>
       <c r="B115" s="6" t="s">
         <v>411</v>
       </c>
-      <c r="C115" s="9" t="s">
-        <v>477</v>
+      <c r="C115" s="8" t="s">
+        <v>481</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>1108</v>
+        <v>1198</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>478</v>
+        <v>424</v>
       </c>
       <c r="F115" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>482</v>
+        <v>418</v>
       </c>
       <c r="I115" s="2" t="s">
-        <v>483</v>
+        <v>947</v>
       </c>
       <c r="J115" s="6" t="s">
         <v>972</v>
@@ -9459,30 +9459,30 @@
         <v>911</v>
       </c>
     </row>
-    <row r="116" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
         <v>499</v>
       </c>
       <c r="B116" s="6" t="s">
         <v>411</v>
       </c>
-      <c r="C116" s="8" t="s">
-        <v>486</v>
+      <c r="C116" s="9" t="s">
+        <v>477</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>1109</v>
+        <v>1199</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="F116" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="I116" s="2" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="J116" s="6" t="s">
         <v>972</v>
@@ -9491,7 +9491,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="117" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
         <v>504</v>
       </c>
@@ -9499,22 +9499,22 @@
         <v>411</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>1109</v>
+        <v>1200</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="F117" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="I117" s="2" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="J117" s="6" t="s">
         <v>972</v>
@@ -9523,7 +9523,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="118" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>509</v>
       </c>
@@ -9534,19 +9534,19 @@
         <v>490</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>1110</v>
+        <v>1201</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="F118" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="I118" s="2" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="J118" s="6" t="s">
         <v>972</v>
@@ -9555,7 +9555,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="119" spans="1:12" ht="315" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
         <v>512</v>
       </c>
@@ -9563,34 +9563,31 @@
         <v>411</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>999</v>
+        <v>1104</v>
       </c>
       <c r="E119" s="8" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="F119" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G119" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="H119" s="2" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="I119" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="K119" s="8" t="s">
-        <v>911</v>
-      </c>
-      <c r="L119" s="20" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="120" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>497</v>
+      </c>
+      <c r="J119" s="6" t="s">
+        <v>972</v>
+      </c>
+      <c r="K119" s="6" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" ht="315" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
         <v>516</v>
       </c>
@@ -9601,28 +9598,31 @@
         <v>498</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>1126</v>
+        <v>999</v>
       </c>
       <c r="E120" s="8" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="F120" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>506</v>
+        <v>501</v>
+      </c>
+      <c r="H120" s="2" t="s">
+        <v>503</v>
       </c>
       <c r="I120" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="J120" s="6" t="s">
-        <v>972</v>
-      </c>
-      <c r="K120" s="6" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12" ht="270" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+      <c r="K120" s="8" t="s">
+        <v>911</v>
+      </c>
+      <c r="L120" s="20" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
         <v>524</v>
       </c>
@@ -9633,32 +9633,28 @@
         <v>498</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>1166</v>
+        <v>1118</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F121" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="H121" s="2"/>
+        <v>506</v>
+      </c>
       <c r="I121" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="J121" s="8" t="s">
-        <v>972</v>
-      </c>
-      <c r="K121" s="8" t="s">
-        <v>911</v>
-      </c>
-      <c r="L121" s="8" t="s">
-        <v>974</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12" ht="345" x14ac:dyDescent="0.25">
+        <v>507</v>
+      </c>
+      <c r="J121" s="6" t="s">
+        <v>972</v>
+      </c>
+      <c r="K121" s="6" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" ht="270" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
         <v>536</v>
       </c>
@@ -9669,26 +9665,29 @@
         <v>498</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>1127</v>
+        <v>1158</v>
       </c>
       <c r="E122" s="8" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="F122" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="H122" s="2"/>
       <c r="I122" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="J122" s="8" t="s">
         <v>972</v>
       </c>
       <c r="K122" s="8" t="s">
         <v>911</v>
+      </c>
+      <c r="L122" s="8" t="s">
+        <v>974</v>
       </c>
     </row>
     <row r="123" spans="1:12" ht="345" x14ac:dyDescent="0.25">
@@ -9702,29 +9701,29 @@
         <v>498</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>1175</v>
+        <v>1119</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="F123" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="H123" s="2"/>
       <c r="I123" s="2" t="s">
-        <v>523</v>
+        <v>515</v>
+      </c>
+      <c r="J123" s="8" t="s">
+        <v>972</v>
       </c>
       <c r="K123" s="8" t="s">
         <v>911</v>
       </c>
-      <c r="L123" s="8" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12" ht="360" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:12" ht="345" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
         <v>538</v>
       </c>
@@ -9732,34 +9731,32 @@
         <v>411</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>517</v>
+        <v>498</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>999</v>
+        <v>1167</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="F124" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="H124" s="2" t="s">
-        <v>542</v>
-      </c>
+        <v>522</v>
+      </c>
+      <c r="H124" s="2"/>
       <c r="I124" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="K124" s="22" t="s">
-        <v>911</v>
-      </c>
-      <c r="L124" s="20" t="s">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="125" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+      <c r="K124" s="8" t="s">
+        <v>911</v>
+      </c>
+      <c r="L124" s="8" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" ht="360" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
         <v>539</v>
       </c>
@@ -9770,28 +9767,31 @@
         <v>517</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>1126</v>
+        <v>999</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="F125" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>526</v>
+        <v>531</v>
+      </c>
+      <c r="H125" s="2" t="s">
+        <v>542</v>
       </c>
       <c r="I125" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="J125" s="6" t="s">
-        <v>972</v>
-      </c>
-      <c r="K125" s="8" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="126" spans="1:12" ht="255" x14ac:dyDescent="0.25">
+        <v>532</v>
+      </c>
+      <c r="K125" s="22" t="s">
+        <v>911</v>
+      </c>
+      <c r="L125" s="20" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
         <v>541</v>
       </c>
@@ -9802,29 +9802,28 @@
         <v>517</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>1128</v>
+        <v>1118</v>
       </c>
       <c r="E126" s="8" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="F126" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="H126" s="2"/>
+        <v>526</v>
+      </c>
       <c r="I126" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="J126" s="8" t="s">
+        <v>527</v>
+      </c>
+      <c r="J126" s="6" t="s">
         <v>972</v>
       </c>
       <c r="K126" s="8" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="127" spans="1:12" ht="375" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" ht="255" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
         <v>547</v>
       </c>
@@ -9835,20 +9834,20 @@
         <v>517</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>1129</v>
+        <v>1120</v>
       </c>
       <c r="E127" s="8" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="F127" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>519</v>
+        <v>529</v>
       </c>
       <c r="H127" s="2"/>
       <c r="I127" s="2" t="s">
-        <v>520</v>
+        <v>530</v>
       </c>
       <c r="J127" s="8" t="s">
         <v>972</v>
@@ -9857,7 +9856,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="128" spans="1:12" ht="360" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" ht="375" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
         <v>551</v>
       </c>
@@ -9868,20 +9867,20 @@
         <v>517</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>1130</v>
+        <v>1121</v>
       </c>
       <c r="E128" s="8" t="s">
-        <v>521</v>
+        <v>533</v>
       </c>
       <c r="F128" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>534</v>
+        <v>519</v>
       </c>
       <c r="H128" s="2"/>
       <c r="I128" s="2" t="s">
-        <v>535</v>
+        <v>520</v>
       </c>
       <c r="J128" s="8" t="s">
         <v>972</v>
@@ -9890,7 +9889,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="375" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" ht="360" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>556</v>
       </c>
@@ -9898,31 +9897,32 @@
         <v>411</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>540</v>
+        <v>517</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>999</v>
+        <v>1122</v>
       </c>
       <c r="E129" s="8" t="s">
-        <v>543</v>
+        <v>521</v>
       </c>
       <c r="F129" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="H129" s="2" t="s">
-        <v>544</v>
-      </c>
+        <v>534</v>
+      </c>
+      <c r="H129" s="2"/>
       <c r="I129" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="K129" s="20" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="130" spans="1:12" ht="330" x14ac:dyDescent="0.25">
+        <v>535</v>
+      </c>
+      <c r="J129" s="8" t="s">
+        <v>972</v>
+      </c>
+      <c r="K129" s="8" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" ht="375" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
         <v>560</v>
       </c>
@@ -9933,29 +9933,28 @@
         <v>540</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>1131</v>
+        <v>999</v>
       </c>
       <c r="E130" s="8" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="F130" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="H130" s="2"/>
+        <v>545</v>
+      </c>
+      <c r="H130" s="2" t="s">
+        <v>544</v>
+      </c>
       <c r="I130" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="J130" s="8" t="s">
-        <v>972</v>
-      </c>
-      <c r="K130" s="8" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="131" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+        <v>546</v>
+      </c>
+      <c r="K130" s="20" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" ht="330" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>566</v>
       </c>
@@ -9963,24 +9962,25 @@
         <v>411</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>552</v>
+        <v>540</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>1109</v>
+        <v>1123</v>
       </c>
       <c r="E131" s="8" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="F131" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>554</v>
-      </c>
+        <v>549</v>
+      </c>
+      <c r="H131" s="2"/>
       <c r="I131" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="J131" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="J131" s="8" t="s">
         <v>972</v>
       </c>
       <c r="K131" s="8" t="s">
@@ -9998,19 +9998,19 @@
         <v>552</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>1132</v>
+        <v>1103</v>
       </c>
       <c r="E132" s="8" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="F132" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="I132" s="2" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="J132" s="6" t="s">
         <v>972</v>
@@ -10019,7 +10019,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="133" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>571</v>
       </c>
@@ -10027,22 +10027,22 @@
         <v>411</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>561</v>
+        <v>552</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>1111</v>
+        <v>1124</v>
       </c>
       <c r="E133" s="8" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="F133" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G133" s="2" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="I133" s="2" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="J133" s="6" t="s">
         <v>972</v>
@@ -10051,7 +10051,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="134" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
         <v>577</v>
       </c>
@@ -10062,19 +10062,19 @@
         <v>561</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>1133</v>
+        <v>1105</v>
       </c>
       <c r="E134" s="8" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F134" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G134" s="2" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="I134" s="2" t="s">
-        <v>952</v>
+        <v>564</v>
       </c>
       <c r="J134" s="6" t="s">
         <v>972</v>
@@ -10094,19 +10094,19 @@
         <v>561</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>1134</v>
+        <v>1125</v>
       </c>
       <c r="E135" s="8" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="F135" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G135" s="2" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="I135" s="2" t="s">
-        <v>575</v>
+        <v>952</v>
       </c>
       <c r="J135" s="6" t="s">
         <v>972</v>
@@ -10115,7 +10115,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="136" spans="1:12" ht="225" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
         <v>585</v>
       </c>
@@ -10126,19 +10126,19 @@
         <v>561</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>1135</v>
+        <v>1126</v>
       </c>
       <c r="E136" s="8" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="F136" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="I136" s="2" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="J136" s="6" t="s">
         <v>972</v>
@@ -10158,19 +10158,19 @@
         <v>561</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>1136</v>
+        <v>1127</v>
       </c>
       <c r="E137" s="8" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="F137" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G137" s="2" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="I137" s="2" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J137" s="6" t="s">
         <v>972</v>
@@ -10179,7 +10179,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="138" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
         <v>592</v>
       </c>
@@ -10187,22 +10187,22 @@
         <v>411</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>581</v>
+        <v>561</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>1137</v>
-      </c>
-      <c r="E138" s="6" t="s">
-        <v>582</v>
+        <v>1128</v>
+      </c>
+      <c r="E138" s="8" t="s">
+        <v>576</v>
       </c>
       <c r="F138" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="I138" s="2" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J138" s="6" t="s">
         <v>972</v>
@@ -10211,7 +10211,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="139" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
         <v>599</v>
       </c>
@@ -10222,19 +10222,19 @@
         <v>581</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>1138</v>
-      </c>
-      <c r="E139" s="8" t="s">
-        <v>625</v>
+        <v>1129</v>
+      </c>
+      <c r="E139" s="6" t="s">
+        <v>582</v>
       </c>
       <c r="F139" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G139" s="2" t="s">
-        <v>626</v>
+        <v>583</v>
       </c>
       <c r="I139" s="2" t="s">
-        <v>627</v>
+        <v>584</v>
       </c>
       <c r="J139" s="6" t="s">
         <v>972</v>
@@ -10254,19 +10254,19 @@
         <v>581</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>1139</v>
+        <v>1130</v>
       </c>
       <c r="E140" s="8" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="F140" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G140" s="2" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="I140" s="2" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="J140" s="6" t="s">
         <v>972</v>
@@ -10286,19 +10286,19 @@
         <v>581</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>1140</v>
+        <v>1131</v>
       </c>
       <c r="E141" s="8" t="s">
-        <v>586</v>
+        <v>628</v>
       </c>
       <c r="F141" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G141" s="2" t="s">
-        <v>587</v>
+        <v>629</v>
       </c>
       <c r="I141" s="2" t="s">
-        <v>588</v>
+        <v>630</v>
       </c>
       <c r="J141" s="6" t="s">
         <v>972</v>
@@ -10307,7 +10307,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
         <v>606</v>
       </c>
@@ -10315,22 +10315,22 @@
         <v>411</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>594</v>
+        <v>581</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>1167</v>
+        <v>1132</v>
       </c>
       <c r="E142" s="8" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
       <c r="F142" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G142" s="2" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="I142" s="2" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="J142" s="6" t="s">
         <v>972</v>
@@ -10338,11 +10338,8 @@
       <c r="K142" s="8" t="s">
         <v>911</v>
       </c>
-      <c r="L142" s="8" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="143" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
         <v>607</v>
       </c>
@@ -10350,22 +10347,22 @@
         <v>411</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>1141</v>
+        <v>1159</v>
       </c>
       <c r="E143" s="8" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="F143" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G143" s="2" t="s">
-        <v>597</v>
+        <v>590</v>
       </c>
       <c r="I143" s="2" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
       <c r="J143" s="6" t="s">
         <v>972</v>
@@ -10373,8 +10370,11 @@
       <c r="K143" s="8" t="s">
         <v>911</v>
       </c>
-    </row>
-    <row r="144" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+      <c r="L143" s="8" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
         <v>608</v>
       </c>
@@ -10385,19 +10385,19 @@
         <v>595</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>1142</v>
+        <v>1133</v>
       </c>
       <c r="E144" s="8" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="F144" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G144" s="2" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="I144" s="2" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="J144" s="6" t="s">
         <v>972</v>
@@ -10406,7 +10406,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="145" spans="1:12" ht="330" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
         <v>624</v>
       </c>
@@ -10416,17 +10416,20 @@
       <c r="C145" s="8" t="s">
         <v>595</v>
       </c>
+      <c r="D145" s="8" t="s">
+        <v>1134</v>
+      </c>
       <c r="E145" s="8" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="F145" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G145" s="2" t="s">
-        <v>615</v>
+        <v>601</v>
       </c>
       <c r="I145" s="2" t="s">
-        <v>616</v>
+        <v>602</v>
       </c>
       <c r="J145" s="6" t="s">
         <v>972</v>
@@ -10434,11 +10437,8 @@
       <c r="K145" s="8" t="s">
         <v>911</v>
       </c>
-      <c r="L145" s="8" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="146" spans="1:12" ht="240" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:12" ht="330" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
         <v>631</v>
       </c>
@@ -10448,20 +10448,17 @@
       <c r="C146" s="8" t="s">
         <v>595</v>
       </c>
-      <c r="D146" s="8" t="s">
-        <v>1112</v>
-      </c>
       <c r="E146" s="8" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="F146" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G146" s="2" t="s">
-        <v>610</v>
+        <v>615</v>
       </c>
       <c r="I146" s="2" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
       <c r="J146" s="6" t="s">
         <v>972</v>
@@ -10469,8 +10466,11 @@
       <c r="K146" s="8" t="s">
         <v>911</v>
       </c>
-    </row>
-    <row r="147" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+      <c r="L146" s="8" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" ht="240" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
         <v>632</v>
       </c>
@@ -10481,19 +10481,19 @@
         <v>595</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>1142</v>
+        <v>1106</v>
       </c>
       <c r="E147" s="8" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="F147" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G147" s="2" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="I147" s="2" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="J147" s="6" t="s">
         <v>972</v>
@@ -10502,27 +10502,30 @@
         <v>911</v>
       </c>
     </row>
-    <row r="148" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
         <v>636</v>
       </c>
       <c r="B148" s="6" t="s">
         <v>411</v>
       </c>
-      <c r="C148" s="6" t="s">
-        <v>617</v>
-      </c>
-      <c r="E148" s="6" t="s">
-        <v>635</v>
+      <c r="C148" s="8" t="s">
+        <v>595</v>
+      </c>
+      <c r="D148" s="8" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E148" s="8" t="s">
+        <v>612</v>
       </c>
       <c r="F148" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G148" s="2" t="s">
-        <v>633</v>
+        <v>613</v>
       </c>
       <c r="I148" s="2" t="s">
-        <v>634</v>
+        <v>614</v>
       </c>
       <c r="J148" s="6" t="s">
         <v>972</v>
@@ -10531,7 +10534,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="149" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
         <v>637</v>
       </c>
@@ -10541,17 +10544,17 @@
       <c r="C149" s="6" t="s">
         <v>617</v>
       </c>
-      <c r="E149" s="8" t="s">
-        <v>638</v>
+      <c r="E149" s="6" t="s">
+        <v>635</v>
       </c>
       <c r="F149" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G149" s="2" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="I149" s="2" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="J149" s="6" t="s">
         <v>972</v>
@@ -10570,17 +10573,17 @@
       <c r="C150" s="6" t="s">
         <v>617</v>
       </c>
-      <c r="E150" s="6" t="s">
-        <v>641</v>
+      <c r="E150" s="8" t="s">
+        <v>638</v>
       </c>
       <c r="F150" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G150" s="2" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="I150" s="2" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="J150" s="6" t="s">
         <v>972</v>
@@ -10599,17 +10602,17 @@
       <c r="C151" s="6" t="s">
         <v>617</v>
       </c>
-      <c r="E151" s="8" t="s">
-        <v>645</v>
+      <c r="E151" s="6" t="s">
+        <v>641</v>
       </c>
       <c r="F151" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G151" s="2" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="I151" s="2" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="J151" s="6" t="s">
         <v>972</v>
@@ -10618,7 +10621,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="152" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A152" s="6" t="s">
         <v>652</v>
       </c>
@@ -10629,16 +10632,16 @@
         <v>617</v>
       </c>
       <c r="E152" s="8" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="F152" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G152" s="2" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="I152" s="2" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="J152" s="6" t="s">
         <v>972</v>
@@ -10647,7 +10650,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="153" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
         <v>656</v>
       </c>
@@ -10658,16 +10661,16 @@
         <v>617</v>
       </c>
       <c r="E153" s="8" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="F153" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G153" s="2" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="I153" s="2" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="J153" s="6" t="s">
         <v>972</v>
@@ -10687,16 +10690,16 @@
         <v>617</v>
       </c>
       <c r="E154" s="8" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="F154" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G154" s="2" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="I154" s="2" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="J154" s="6" t="s">
         <v>972</v>
@@ -10716,16 +10719,16 @@
         <v>617</v>
       </c>
       <c r="E155" s="8" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="F155" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="I155" s="2" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="J155" s="6" t="s">
         <v>972</v>
@@ -10734,7 +10737,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="156" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A156" s="6" t="s">
         <v>670</v>
       </c>
@@ -10742,34 +10745,28 @@
         <v>411</v>
       </c>
       <c r="C156" s="6" t="s">
-        <v>665</v>
-      </c>
-      <c r="D156" s="8" t="s">
-        <v>1000</v>
+        <v>617</v>
       </c>
       <c r="E156" s="8" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="F156" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>668</v>
-      </c>
-      <c r="H156" s="8" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>669</v>
-      </c>
-      <c r="K156" s="20" t="s">
-        <v>909</v>
-      </c>
-      <c r="L156" s="20" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="157" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+        <v>663</v>
+      </c>
+      <c r="J156" s="6" t="s">
+        <v>972</v>
+      </c>
+      <c r="K156" s="8" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A157" s="6" t="s">
         <v>674</v>
       </c>
@@ -10780,29 +10777,31 @@
         <v>665</v>
       </c>
       <c r="D157" s="8" t="s">
-        <v>1143</v>
+        <v>1000</v>
       </c>
       <c r="E157" s="8" t="s">
-        <v>694</v>
+        <v>666</v>
       </c>
       <c r="F157" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G157" s="2" t="s">
-        <v>695</v>
-      </c>
-      <c r="H157" s="8"/>
+        <v>668</v>
+      </c>
+      <c r="H157" s="8" t="s">
+        <v>667</v>
+      </c>
       <c r="I157" s="2" t="s">
-        <v>696</v>
-      </c>
-      <c r="J157" s="6" t="s">
-        <v>972</v>
-      </c>
-      <c r="K157" s="8" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="158" spans="1:12" ht="240" x14ac:dyDescent="0.25">
+        <v>669</v>
+      </c>
+      <c r="K157" s="20" t="s">
+        <v>909</v>
+      </c>
+      <c r="L157" s="20" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A158" s="6" t="s">
         <v>678</v>
       </c>
@@ -10812,17 +10811,21 @@
       <c r="C158" s="6" t="s">
         <v>665</v>
       </c>
+      <c r="D158" s="8" t="s">
+        <v>1135</v>
+      </c>
       <c r="E158" s="8" t="s">
-        <v>671</v>
+        <v>694</v>
       </c>
       <c r="F158" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G158" s="2" t="s">
-        <v>673</v>
-      </c>
+        <v>695</v>
+      </c>
+      <c r="H158" s="8"/>
       <c r="I158" s="2" t="s">
-        <v>672</v>
+        <v>696</v>
       </c>
       <c r="J158" s="6" t="s">
         <v>972</v>
@@ -10830,11 +10833,8 @@
       <c r="K158" s="8" t="s">
         <v>911</v>
       </c>
-      <c r="L158" s="8" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="159" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="159" spans="1:12" ht="240" x14ac:dyDescent="0.25">
       <c r="A159" s="6" t="s">
         <v>682</v>
       </c>
@@ -10844,26 +10844,26 @@
       <c r="C159" s="6" t="s">
         <v>665</v>
       </c>
-      <c r="D159" s="8" t="s">
-        <v>1113</v>
-      </c>
       <c r="E159" s="8" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="F159" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="I159" s="2" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="J159" s="6" t="s">
         <v>972</v>
       </c>
       <c r="K159" s="8" t="s">
         <v>911</v>
+      </c>
+      <c r="L159" s="8" t="s">
+        <v>955</v>
       </c>
     </row>
     <row r="160" spans="1:12" ht="165" x14ac:dyDescent="0.25">
@@ -10877,19 +10877,19 @@
         <v>665</v>
       </c>
       <c r="D160" s="8" t="s">
-        <v>1114</v>
+        <v>1107</v>
       </c>
       <c r="E160" s="8" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="F160" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="I160" s="2" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="J160" s="6" t="s">
         <v>972</v>
@@ -10898,7 +10898,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="161" spans="1:27" ht="315" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:27" ht="165" x14ac:dyDescent="0.25">
       <c r="A161" s="6" t="s">
         <v>690</v>
       </c>
@@ -10909,28 +10909,28 @@
         <v>665</v>
       </c>
       <c r="D161" s="8" t="s">
-        <v>1115</v>
+        <v>1108</v>
       </c>
       <c r="E161" s="8" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="F161" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G161" s="2" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="I161" s="2" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="J161" s="6" t="s">
-        <v>964</v>
+        <v>972</v>
       </c>
       <c r="K161" s="8" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="162" spans="1:27" ht="285" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:27" ht="315" x14ac:dyDescent="0.25">
       <c r="A162" s="6" t="s">
         <v>697</v>
       </c>
@@ -10941,19 +10941,19 @@
         <v>665</v>
       </c>
       <c r="D162" s="8" t="s">
-        <v>1116</v>
+        <v>1109</v>
       </c>
       <c r="E162" s="8" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="F162" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G162" s="2" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="I162" s="2" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="J162" s="6" t="s">
         <v>964</v>
@@ -10962,7 +10962,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="163" spans="1:27" ht="315" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:27" ht="285" x14ac:dyDescent="0.25">
       <c r="A163" s="6" t="s">
         <v>698</v>
       </c>
@@ -10973,19 +10973,19 @@
         <v>665</v>
       </c>
       <c r="D163" s="8" t="s">
-        <v>1117</v>
+        <v>1110</v>
       </c>
       <c r="E163" s="8" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="F163" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G163" s="2" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="I163" s="2" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="J163" s="6" t="s">
         <v>964</v>
@@ -10994,7 +10994,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="164" spans="1:27" ht="150" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:27" ht="315" x14ac:dyDescent="0.25">
       <c r="A164" s="6" t="s">
         <v>703</v>
       </c>
@@ -11002,28 +11002,31 @@
         <v>411</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>699</v>
+        <v>665</v>
       </c>
       <c r="D164" s="8" t="s">
-        <v>1168</v>
+        <v>1111</v>
       </c>
       <c r="E164" s="8" t="s">
-        <v>700</v>
+        <v>691</v>
       </c>
       <c r="F164" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>701</v>
+        <v>692</v>
       </c>
       <c r="I164" s="2" t="s">
-        <v>702</v>
-      </c>
-      <c r="L164" s="20" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="165" spans="1:27" ht="180" x14ac:dyDescent="0.25">
+        <v>693</v>
+      </c>
+      <c r="J164" s="6" t="s">
+        <v>964</v>
+      </c>
+      <c r="K164" s="8" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="165" spans="1:27" ht="150" x14ac:dyDescent="0.25">
       <c r="A165" s="6" t="s">
         <v>706</v>
       </c>
@@ -11034,25 +11037,22 @@
         <v>699</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>1144</v>
+        <v>1160</v>
       </c>
       <c r="E165" s="8" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="F165" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G165" s="2" t="s">
-        <v>957</v>
+        <v>701</v>
       </c>
       <c r="I165" s="2" t="s">
-        <v>705</v>
-      </c>
-      <c r="J165" s="6" t="s">
-        <v>964</v>
-      </c>
-      <c r="K165" s="6" t="s">
-        <v>911</v>
+        <v>702</v>
+      </c>
+      <c r="L165" s="20" t="s">
+        <v>956</v>
       </c>
     </row>
     <row r="166" spans="1:27" ht="180" x14ac:dyDescent="0.25">
@@ -11066,19 +11066,19 @@
         <v>699</v>
       </c>
       <c r="D166" s="8" t="s">
-        <v>1118</v>
+        <v>1136</v>
       </c>
       <c r="E166" s="8" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="F166" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="I166" s="2" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="J166" s="6" t="s">
         <v>964</v>
@@ -11087,7 +11087,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="167" spans="1:27" ht="225" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:27" ht="180" x14ac:dyDescent="0.25">
       <c r="A167" s="6" t="s">
         <v>712</v>
       </c>
@@ -11098,19 +11098,19 @@
         <v>699</v>
       </c>
       <c r="D167" s="8" t="s">
-        <v>1119</v>
+        <v>1112</v>
       </c>
       <c r="E167" s="8" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="F167" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G167" s="2" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I167" s="2" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="J167" s="6" t="s">
         <v>964</v>
@@ -11127,25 +11127,28 @@
         <v>411</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>713</v>
+        <v>699</v>
+      </c>
+      <c r="D168" s="8" t="s">
+        <v>1113</v>
       </c>
       <c r="E168" s="8" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="F168" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G168" s="2" t="s">
-        <v>715</v>
+        <v>959</v>
       </c>
       <c r="I168" s="2" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="J168" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="L168" s="20" t="s">
-        <v>971</v>
+      <c r="K168" s="6" t="s">
+        <v>911</v>
       </c>
     </row>
     <row r="169" spans="1:27" ht="225" x14ac:dyDescent="0.25">
@@ -11158,29 +11161,26 @@
       <c r="C169" s="6" t="s">
         <v>713</v>
       </c>
-      <c r="D169" s="8" t="s">
-        <v>1145</v>
-      </c>
       <c r="E169" s="8" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="F169" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G169" s="2" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="I169" s="2" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="J169" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K169" s="6" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="170" spans="1:27" ht="270" x14ac:dyDescent="0.25">
+      <c r="L169" s="20" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="170" spans="1:27" ht="225" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
         <v>725</v>
       </c>
@@ -11191,19 +11191,19 @@
         <v>713</v>
       </c>
       <c r="D170" s="8" t="s">
-        <v>1146</v>
+        <v>1137</v>
       </c>
       <c r="E170" s="8" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="F170" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G170" s="2" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="I170" s="2" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="J170" s="6" t="s">
         <v>964</v>
@@ -11212,7 +11212,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="171" spans="1:27" ht="285.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:27" ht="270" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
         <v>729</v>
       </c>
@@ -11223,19 +11223,19 @@
         <v>713</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>1147</v>
+        <v>1138</v>
       </c>
       <c r="E171" s="8" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="F171" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G171" s="2" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="I171" s="2" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="J171" s="6" t="s">
         <v>964</v>
@@ -11244,134 +11244,137 @@
         <v>911</v>
       </c>
     </row>
-    <row r="172" spans="1:27" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:27" ht="285.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="6" t="s">
         <v>734</v>
       </c>
-      <c r="B172" s="10" t="s">
-        <v>730</v>
-      </c>
-      <c r="C172" s="10" t="s">
+      <c r="B172" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="C172" s="6" t="s">
         <v>713</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>1148</v>
-      </c>
-      <c r="E172" s="10" t="s">
-        <v>731</v>
+        <v>1139</v>
+      </c>
+      <c r="E172" s="8" t="s">
+        <v>726</v>
       </c>
       <c r="F172" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G172" s="12" t="s">
-        <v>732</v>
-      </c>
-      <c r="H172" s="11"/>
-      <c r="I172" s="12" t="s">
-        <v>733</v>
-      </c>
-      <c r="J172" s="23" t="s">
+      <c r="G172" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="I172" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="J172" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K172" s="23" t="s">
-        <v>911</v>
-      </c>
-      <c r="L172" s="23"/>
-      <c r="M172" s="11"/>
-      <c r="N172" s="11"/>
-      <c r="O172" s="11"/>
-      <c r="P172" s="11"/>
-      <c r="Q172" s="11"/>
-      <c r="R172" s="11"/>
-      <c r="S172" s="11"/>
-      <c r="T172" s="11"/>
-      <c r="U172" s="11"/>
-      <c r="V172" s="11"/>
-      <c r="W172" s="11"/>
-      <c r="X172" s="11"/>
-      <c r="Y172" s="11"/>
-      <c r="Z172" s="11"/>
-      <c r="AA172" s="11"/>
-    </row>
-    <row r="173" spans="1:27" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K172" s="6" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="173" spans="1:27" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="6" t="s">
         <v>740</v>
       </c>
       <c r="B173" s="10" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="C173" s="10" t="s">
-        <v>735</v>
+        <v>713</v>
       </c>
       <c r="D173" s="8" t="s">
-        <v>1149</v>
-      </c>
-      <c r="E173" s="14" t="s">
-        <v>748</v>
+        <v>1140</v>
+      </c>
+      <c r="E173" s="10" t="s">
+        <v>731</v>
       </c>
       <c r="F173" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G173" s="13" t="s">
-        <v>750</v>
-      </c>
-      <c r="H173" s="16"/>
-      <c r="I173" s="15" t="s">
-        <v>749</v>
-      </c>
-      <c r="J173" s="24" t="s">
+      <c r="G173" s="12" t="s">
+        <v>732</v>
+      </c>
+      <c r="H173" s="11"/>
+      <c r="I173" s="12" t="s">
+        <v>733</v>
+      </c>
+      <c r="J173" s="23" t="s">
         <v>964</v>
       </c>
-      <c r="K173" s="24" t="s">
-        <v>911</v>
-      </c>
-      <c r="L173" s="24"/>
-      <c r="M173" s="16"/>
-      <c r="N173" s="16"/>
-      <c r="O173" s="16"/>
-      <c r="P173" s="16"/>
-      <c r="Q173" s="16"/>
-      <c r="R173" s="16"/>
-      <c r="S173" s="16"/>
-      <c r="T173" s="16"/>
-      <c r="U173" s="16"/>
-      <c r="V173" s="16"/>
-      <c r="W173" s="16"/>
-      <c r="X173" s="16"/>
-      <c r="Y173" s="16"/>
-      <c r="Z173" s="16"/>
-      <c r="AA173" s="16"/>
-    </row>
-    <row r="174" spans="1:27" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K173" s="23" t="s">
+        <v>911</v>
+      </c>
+      <c r="L173" s="23"/>
+      <c r="M173" s="11"/>
+      <c r="N173" s="11"/>
+      <c r="O173" s="11"/>
+      <c r="P173" s="11"/>
+      <c r="Q173" s="11"/>
+      <c r="R173" s="11"/>
+      <c r="S173" s="11"/>
+      <c r="T173" s="11"/>
+      <c r="U173" s="11"/>
+      <c r="V173" s="11"/>
+      <c r="W173" s="11"/>
+      <c r="X173" s="11"/>
+      <c r="Y173" s="11"/>
+      <c r="Z173" s="11"/>
+      <c r="AA173" s="11"/>
+    </row>
+    <row r="174" spans="1:27" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="6" t="s">
         <v>744</v>
       </c>
       <c r="B174" s="10" t="s">
         <v>735</v>
       </c>
-      <c r="C174" s="8" t="s">
-        <v>736</v>
-      </c>
-      <c r="E174" s="8" t="s">
-        <v>737</v>
+      <c r="C174" s="10" t="s">
+        <v>735</v>
+      </c>
+      <c r="D174" s="8" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E174" s="14" t="s">
+        <v>748</v>
       </c>
       <c r="F174" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G174" s="13" t="s">
-        <v>738</v>
-      </c>
-      <c r="I174" s="13" t="s">
-        <v>739</v>
-      </c>
-      <c r="K174" s="19" t="s">
-        <v>909</v>
-      </c>
-      <c r="L174" s="20" t="s">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="175" spans="1:27" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>750</v>
+      </c>
+      <c r="H174" s="16"/>
+      <c r="I174" s="15" t="s">
+        <v>749</v>
+      </c>
+      <c r="J174" s="24" t="s">
+        <v>964</v>
+      </c>
+      <c r="K174" s="24" t="s">
+        <v>911</v>
+      </c>
+      <c r="L174" s="24"/>
+      <c r="M174" s="16"/>
+      <c r="N174" s="16"/>
+      <c r="O174" s="16"/>
+      <c r="P174" s="16"/>
+      <c r="Q174" s="16"/>
+      <c r="R174" s="16"/>
+      <c r="S174" s="16"/>
+      <c r="T174" s="16"/>
+      <c r="U174" s="16"/>
+      <c r="V174" s="16"/>
+      <c r="W174" s="16"/>
+      <c r="X174" s="16"/>
+      <c r="Y174" s="16"/>
+      <c r="Z174" s="16"/>
+      <c r="AA174" s="16"/>
+    </row>
+    <row r="175" spans="1:27" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="6" t="s">
         <v>751</v>
       </c>
@@ -11381,29 +11384,23 @@
       <c r="C175" s="8" t="s">
         <v>736</v>
       </c>
-      <c r="D175" s="8" t="s">
-        <v>1169</v>
-      </c>
       <c r="E175" s="8" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="F175" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G175" s="13" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="I175" s="13" t="s">
-        <v>743</v>
-      </c>
-      <c r="J175" s="6" t="s">
-        <v>964</v>
-      </c>
-      <c r="K175" s="6" t="s">
-        <v>911</v>
-      </c>
-      <c r="L175" s="8" t="s">
-        <v>969</v>
+        <v>739</v>
+      </c>
+      <c r="K175" s="19" t="s">
+        <v>909</v>
+      </c>
+      <c r="L175" s="20" t="s">
+        <v>970</v>
       </c>
     </row>
     <row r="176" spans="1:27" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11417,63 +11414,63 @@
         <v>736</v>
       </c>
       <c r="D176" s="8" t="s">
-        <v>1099</v>
+        <v>1161</v>
       </c>
       <c r="E176" s="8" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="F176" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G176" s="13" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="I176" s="13" t="s">
-        <v>747</v>
-      </c>
-      <c r="K176" s="19" t="s">
-        <v>909</v>
-      </c>
-      <c r="L176" s="20" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="177" spans="1:12" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>743</v>
+      </c>
+      <c r="J176" s="6" t="s">
+        <v>964</v>
+      </c>
+      <c r="K176" s="6" t="s">
+        <v>911</v>
+      </c>
+      <c r="L176" s="8" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="6" t="s">
         <v>758</v>
       </c>
       <c r="B177" s="10" t="s">
         <v>735</v>
       </c>
-      <c r="C177" s="6" t="s">
-        <v>753</v>
+      <c r="C177" s="8" t="s">
+        <v>736</v>
       </c>
       <c r="D177" s="8" t="s">
-        <v>1001</v>
+        <v>1099</v>
       </c>
       <c r="E177" s="8" t="s">
-        <v>754</v>
+        <v>745</v>
       </c>
       <c r="F177" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G177" s="13" t="s">
-        <v>755</v>
-      </c>
-      <c r="H177" s="2" t="s">
-        <v>756</v>
+        <v>746</v>
       </c>
       <c r="I177" s="13" t="s">
-        <v>757</v>
-      </c>
-      <c r="J177" s="25" t="s">
-        <v>964</v>
-      </c>
-      <c r="K177" s="25" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="178" spans="1:12" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>747</v>
+      </c>
+      <c r="K177" s="19" t="s">
+        <v>909</v>
+      </c>
+      <c r="L177" s="20" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="6" t="s">
         <v>763</v>
       </c>
@@ -11484,22 +11481,22 @@
         <v>753</v>
       </c>
       <c r="D178" s="8" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E178" s="8" t="s">
-        <v>759</v>
+        <v>754</v>
       </c>
       <c r="F178" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G178" s="13" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
       <c r="H178" s="2" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="I178" s="13" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
       <c r="J178" s="25" t="s">
         <v>964</v>
@@ -11507,11 +11504,8 @@
       <c r="K178" s="25" t="s">
         <v>911</v>
       </c>
-      <c r="L178" s="25" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="179" spans="1:12" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="179" spans="1:12" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="6" t="s">
         <v>767</v>
       </c>
@@ -11522,25 +11516,31 @@
         <v>753</v>
       </c>
       <c r="D179" s="8" t="s">
-        <v>1150</v>
+        <v>1002</v>
       </c>
       <c r="E179" s="8" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="F179" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G179" s="13" t="s">
-        <v>765</v>
-      </c>
-      <c r="I179" s="2" t="s">
-        <v>766</v>
-      </c>
-      <c r="J179" s="6" t="s">
+        <v>761</v>
+      </c>
+      <c r="H179" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="I179" s="13" t="s">
+        <v>762</v>
+      </c>
+      <c r="J179" s="25" t="s">
         <v>964</v>
       </c>
-      <c r="K179" s="6" t="s">
-        <v>911</v>
+      <c r="K179" s="25" t="s">
+        <v>911</v>
+      </c>
+      <c r="L179" s="25" t="s">
+        <v>968</v>
       </c>
     </row>
     <row r="180" spans="1:12" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11554,10 +11554,10 @@
         <v>753</v>
       </c>
       <c r="D180" s="8" t="s">
-        <v>1120</v>
+        <v>1142</v>
       </c>
       <c r="E180" s="8" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="F180" s="6" t="s">
         <v>38</v>
@@ -11575,7 +11575,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="181" spans="1:12" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:12" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="6" t="s">
         <v>772</v>
       </c>
@@ -11586,7 +11586,7 @@
         <v>753</v>
       </c>
       <c r="D181" s="8" t="s">
-        <v>1120</v>
+        <v>1114</v>
       </c>
       <c r="E181" s="8" t="s">
         <v>768</v>
@@ -11595,20 +11595,19 @@
         <v>38</v>
       </c>
       <c r="G181" s="13" t="s">
-        <v>770</v>
-      </c>
-      <c r="H181" s="2"/>
-      <c r="I181" s="13" t="s">
-        <v>771</v>
-      </c>
-      <c r="J181" s="25" t="s">
+        <v>765</v>
+      </c>
+      <c r="I181" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="J181" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K181" s="25" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="182" spans="1:12" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K181" s="6" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="6" t="s">
         <v>775</v>
       </c>
@@ -11619,7 +11618,7 @@
         <v>753</v>
       </c>
       <c r="D182" s="8" t="s">
-        <v>1120</v>
+        <v>1114</v>
       </c>
       <c r="E182" s="8" t="s">
         <v>768</v>
@@ -11628,11 +11627,11 @@
         <v>38</v>
       </c>
       <c r="G182" s="13" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="H182" s="2"/>
       <c r="I182" s="13" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="J182" s="25" t="s">
         <v>964</v>
@@ -11641,7 +11640,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="183" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:12" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="6" t="s">
         <v>780</v>
       </c>
@@ -11652,51 +11651,52 @@
         <v>753</v>
       </c>
       <c r="D183" s="8" t="s">
-        <v>1151</v>
+        <v>1114</v>
       </c>
       <c r="E183" s="8" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="F183" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G183" s="2" t="s">
-        <v>777</v>
-      </c>
-      <c r="I183" s="2" t="s">
-        <v>778</v>
-      </c>
-      <c r="J183" s="6" t="s">
+      <c r="G183" s="13" t="s">
+        <v>773</v>
+      </c>
+      <c r="H183" s="2"/>
+      <c r="I183" s="13" t="s">
+        <v>774</v>
+      </c>
+      <c r="J183" s="25" t="s">
         <v>964</v>
       </c>
       <c r="K183" s="25" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="184" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="6" t="s">
         <v>783</v>
       </c>
       <c r="B184" s="10" t="s">
         <v>735</v>
       </c>
-      <c r="C184" s="8" t="s">
-        <v>779</v>
+      <c r="C184" s="6" t="s">
+        <v>753</v>
       </c>
       <c r="D184" s="8" t="s">
-        <v>1121</v>
-      </c>
-      <c r="E184" s="6" t="s">
-        <v>786</v>
+        <v>1143</v>
+      </c>
+      <c r="E184" s="8" t="s">
+        <v>776</v>
       </c>
       <c r="F184" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G184" s="2" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="I184" s="2" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="J184" s="6" t="s">
         <v>964</v>
@@ -11705,7 +11705,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="185" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="6" t="s">
         <v>789</v>
       </c>
@@ -11713,22 +11713,22 @@
         <v>735</v>
       </c>
       <c r="C185" s="8" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="D185" s="8" t="s">
-        <v>1152</v>
+        <v>1115</v>
       </c>
       <c r="E185" s="6" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="F185" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G185" s="2" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="I185" s="2" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
       <c r="J185" s="6" t="s">
         <v>964</v>
@@ -11737,7 +11737,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="186" spans="1:12" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="6" t="s">
         <v>794</v>
       </c>
@@ -11745,31 +11745,31 @@
         <v>735</v>
       </c>
       <c r="C186" s="8" t="s">
-        <v>790</v>
+        <v>784</v>
       </c>
       <c r="D186" s="8" t="s">
-        <v>1100</v>
-      </c>
-      <c r="E186" s="8" t="s">
-        <v>791</v>
+        <v>1144</v>
+      </c>
+      <c r="E186" s="6" t="s">
+        <v>785</v>
       </c>
       <c r="F186" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G186" s="2" t="s">
-        <v>792</v>
+        <v>787</v>
       </c>
       <c r="I186" s="2" t="s">
-        <v>793</v>
-      </c>
-      <c r="K186" s="26" t="s">
-        <v>909</v>
-      </c>
-      <c r="L186" s="20" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="187" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>788</v>
+      </c>
+      <c r="J186" s="6" t="s">
+        <v>964</v>
+      </c>
+      <c r="K186" s="25" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="6" t="s">
         <v>799</v>
       </c>
@@ -11777,22 +11777,22 @@
         <v>735</v>
       </c>
       <c r="C187" s="8" t="s">
-        <v>796</v>
+        <v>790</v>
       </c>
       <c r="D187" s="8" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="E187" s="8" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="F187" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G187" s="2" t="s">
-        <v>798</v>
+        <v>792</v>
       </c>
       <c r="I187" s="2" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="K187" s="26" t="s">
         <v>909</v>
@@ -11801,7 +11801,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="188" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="6" t="s">
         <v>804</v>
       </c>
@@ -11812,22 +11812,19 @@
         <v>796</v>
       </c>
       <c r="D188" s="8" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="E188" s="8" t="s">
-        <v>800</v>
+        <v>795</v>
       </c>
       <c r="F188" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G188" s="2" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="I188" s="2" t="s">
-        <v>803</v>
-      </c>
-      <c r="J188" s="6" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
       <c r="K188" s="26" t="s">
         <v>909</v>
@@ -11836,7 +11833,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="189" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="6" t="s">
         <v>810</v>
       </c>
@@ -11844,28 +11841,31 @@
         <v>735</v>
       </c>
       <c r="C189" s="8" t="s">
-        <v>805</v>
+        <v>796</v>
       </c>
       <c r="D189" s="8" t="s">
-        <v>1122</v>
+        <v>1102</v>
       </c>
       <c r="E189" s="8" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
       <c r="F189" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G189" s="2" t="s">
-        <v>807</v>
+        <v>801</v>
       </c>
       <c r="I189" s="2" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
       <c r="J189" s="6" t="s">
-        <v>964</v>
-      </c>
-      <c r="K189" s="27" t="s">
-        <v>911</v>
+        <v>802</v>
+      </c>
+      <c r="K189" s="26" t="s">
+        <v>909</v>
+      </c>
+      <c r="L189" s="20" t="s">
+        <v>961</v>
       </c>
     </row>
     <row r="190" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11879,19 +11879,19 @@
         <v>805</v>
       </c>
       <c r="D190" s="8" t="s">
-        <v>1153</v>
+        <v>1116</v>
       </c>
       <c r="E190" s="8" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="F190" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G190" s="2" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="I190" s="2" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="J190" s="6" t="s">
         <v>964</v>
@@ -11900,7 +11900,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="191" spans="1:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="6" t="s">
         <v>817</v>
       </c>
@@ -11911,19 +11911,19 @@
         <v>805</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>1154</v>
+        <v>1145</v>
       </c>
       <c r="E191" s="8" t="s">
-        <v>814</v>
+        <v>809</v>
       </c>
       <c r="F191" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G191" s="2" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="I191" s="2" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="J191" s="6" t="s">
         <v>964</v>
@@ -11932,7 +11932,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="192" spans="1:12" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="6" t="s">
         <v>819</v>
       </c>
@@ -11943,19 +11943,19 @@
         <v>805</v>
       </c>
       <c r="D192" s="8" t="s">
-        <v>1155</v>
+        <v>1146</v>
       </c>
       <c r="E192" s="8" t="s">
-        <v>826</v>
+        <v>814</v>
       </c>
       <c r="F192" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G192" s="2" t="s">
-        <v>829</v>
+        <v>815</v>
       </c>
       <c r="I192" s="2" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="J192" s="6" t="s">
         <v>964</v>
@@ -11964,7 +11964,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="193" spans="1:12" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:12" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="6" t="s">
         <v>822</v>
       </c>
@@ -11975,28 +11975,25 @@
         <v>805</v>
       </c>
       <c r="D193" s="8" t="s">
-        <v>1170</v>
+        <v>1147</v>
       </c>
       <c r="E193" s="8" t="s">
-        <v>820</v>
+        <v>826</v>
       </c>
       <c r="F193" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G193" s="2" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="I193" s="2" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="J193" s="6" t="s">
         <v>964</v>
       </c>
       <c r="K193" s="27" t="s">
         <v>911</v>
-      </c>
-      <c r="L193" s="8" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="194" spans="1:12" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12010,19 +12007,19 @@
         <v>805</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>1156</v>
+        <v>1162</v>
       </c>
       <c r="E194" s="8" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="F194" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G194" s="2" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="I194" s="2" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="J194" s="6" t="s">
         <v>964</v>
@@ -12030,8 +12027,11 @@
       <c r="K194" s="27" t="s">
         <v>911</v>
       </c>
-    </row>
-    <row r="195" spans="1:12" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L194" s="8" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="6" t="s">
         <v>833</v>
       </c>
@@ -12042,19 +12042,19 @@
         <v>805</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>1157</v>
+        <v>1148</v>
       </c>
       <c r="E195" s="8" t="s">
-        <v>830</v>
+        <v>823</v>
       </c>
       <c r="F195" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G195" s="2" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="I195" s="2" t="s">
-        <v>832</v>
+        <v>824</v>
       </c>
       <c r="J195" s="6" t="s">
         <v>964</v>
@@ -12063,7 +12063,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="196" spans="1:12" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:12" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="6" t="s">
         <v>836</v>
       </c>
@@ -12074,19 +12074,19 @@
         <v>805</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>1158</v>
+        <v>1149</v>
       </c>
       <c r="E196" s="8" t="s">
-        <v>837</v>
+        <v>830</v>
       </c>
       <c r="F196" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G196" s="2" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="I196" s="2" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="J196" s="6" t="s">
         <v>964</v>
@@ -12095,7 +12095,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="197" spans="1:12" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:12" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="6" t="s">
         <v>841</v>
       </c>
@@ -12106,19 +12106,19 @@
         <v>805</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>1159</v>
+        <v>1150</v>
       </c>
       <c r="E197" s="8" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="F197" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G197" s="2" t="s">
-        <v>839</v>
+        <v>834</v>
       </c>
       <c r="I197" s="2" t="s">
-        <v>840</v>
+        <v>835</v>
       </c>
       <c r="J197" s="6" t="s">
         <v>964</v>
@@ -12127,7 +12127,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="198" spans="1:12" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:12" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="6" t="s">
         <v>845</v>
       </c>
@@ -12138,19 +12138,19 @@
         <v>805</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>1160</v>
+        <v>1151</v>
       </c>
       <c r="E198" s="8" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="F198" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G198" s="2" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="I198" s="2" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="J198" s="6" t="s">
         <v>964</v>
@@ -12159,7 +12159,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="199" spans="1:12" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:12" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="6" t="s">
         <v>849</v>
       </c>
@@ -12170,28 +12170,28 @@
         <v>805</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>1171</v>
+        <v>1152</v>
       </c>
       <c r="E199" s="8" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
       <c r="F199" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G199" s="2" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
       <c r="I199" s="2" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="J199" s="6" t="s">
-        <v>853</v>
-      </c>
-      <c r="L199" s="20" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="200" spans="1:12" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>964</v>
+      </c>
+      <c r="K199" s="27" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="6" t="s">
         <v>854</v>
       </c>
@@ -12202,19 +12202,19 @@
         <v>805</v>
       </c>
       <c r="D200" s="8" t="s">
-        <v>1172</v>
+        <v>1163</v>
       </c>
       <c r="E200" s="8" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="F200" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G200" s="2" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="I200" s="2" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="J200" s="6" t="s">
         <v>853</v>
@@ -12234,28 +12234,28 @@
         <v>805</v>
       </c>
       <c r="D201" s="8" t="s">
-        <v>1161</v>
+        <v>1164</v>
       </c>
       <c r="E201" s="8" t="s">
-        <v>855</v>
+        <v>850</v>
       </c>
       <c r="F201" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G201" s="2" t="s">
-        <v>856</v>
+        <v>851</v>
       </c>
       <c r="I201" s="2" t="s">
-        <v>857</v>
+        <v>852</v>
       </c>
       <c r="J201" s="6" t="s">
-        <v>964</v>
-      </c>
-      <c r="K201" s="27" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="202" spans="1:12" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>853</v>
+      </c>
+      <c r="L201" s="20" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="6" t="s">
         <v>861</v>
       </c>
@@ -12266,19 +12266,19 @@
         <v>805</v>
       </c>
       <c r="D202" s="8" t="s">
-        <v>1158</v>
+        <v>1153</v>
       </c>
       <c r="E202" s="8" t="s">
-        <v>862</v>
+        <v>855</v>
       </c>
       <c r="F202" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G202" s="2" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="I202" s="2" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="J202" s="6" t="s">
         <v>964</v>
@@ -12287,7 +12287,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="203" spans="1:12" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:12" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="6" t="s">
         <v>866</v>
       </c>
@@ -12297,26 +12297,29 @@
       <c r="C203" s="8" t="s">
         <v>805</v>
       </c>
+      <c r="D203" s="8" t="s">
+        <v>1150</v>
+      </c>
       <c r="E203" s="8" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F203" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G203" s="2" t="s">
-        <v>864</v>
+        <v>859</v>
       </c>
       <c r="I203" s="2" t="s">
-        <v>865</v>
-      </c>
-      <c r="K203" s="26" t="s">
-        <v>909</v>
-      </c>
-      <c r="L203" s="20" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="204" spans="1:12" ht="240.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>860</v>
+      </c>
+      <c r="J203" s="6" t="s">
+        <v>964</v>
+      </c>
+      <c r="K203" s="27" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="6" t="s">
         <v>870</v>
       </c>
@@ -12327,19 +12330,16 @@
         <v>805</v>
       </c>
       <c r="E204" s="8" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="F204" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G204" s="2" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="I204" s="2" t="s">
-        <v>869</v>
-      </c>
-      <c r="J204" s="6" t="s">
-        <v>853</v>
+        <v>865</v>
       </c>
       <c r="K204" s="26" t="s">
         <v>909</v>
@@ -12348,7 +12348,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="205" spans="1:12" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:12" ht="240.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="6" t="s">
         <v>873</v>
       </c>
@@ -12359,83 +12359,83 @@
         <v>805</v>
       </c>
       <c r="E205" s="8" t="s">
-        <v>820</v>
+        <v>867</v>
       </c>
       <c r="F205" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G205" s="2" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="I205" s="2" t="s">
-        <v>872</v>
-      </c>
-      <c r="J205" s="8" t="s">
-        <v>966</v>
-      </c>
-      <c r="K205" s="20" t="s">
+        <v>869</v>
+      </c>
+      <c r="J205" s="6" t="s">
+        <v>853</v>
+      </c>
+      <c r="K205" s="26" t="s">
         <v>909</v>
       </c>
       <c r="L205" s="20" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="206" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="6" t="s">
         <v>878</v>
       </c>
-      <c r="B206" s="6" t="s">
-        <v>874</v>
-      </c>
-      <c r="C206" s="6" t="s">
-        <v>874</v>
-      </c>
-      <c r="D206" s="8" t="s">
-        <v>1162</v>
+      <c r="B206" s="10" t="s">
+        <v>735</v>
+      </c>
+      <c r="C206" s="8" t="s">
+        <v>805</v>
       </c>
       <c r="E206" s="8" t="s">
-        <v>879</v>
+        <v>820</v>
       </c>
       <c r="F206" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G206" s="2" t="s">
-        <v>880</v>
+        <v>871</v>
       </c>
       <c r="I206" s="2" t="s">
-        <v>881</v>
-      </c>
-      <c r="J206" s="6" t="s">
-        <v>964</v>
-      </c>
-      <c r="K206" s="22" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="207" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+        <v>872</v>
+      </c>
+      <c r="J206" s="8" t="s">
+        <v>966</v>
+      </c>
+      <c r="K206" s="20" t="s">
+        <v>909</v>
+      </c>
+      <c r="L206" s="20" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A207" s="6" t="s">
         <v>884</v>
       </c>
       <c r="B207" s="6" t="s">
         <v>874</v>
       </c>
-      <c r="C207" s="8" t="s">
-        <v>875</v>
+      <c r="C207" s="6" t="s">
+        <v>874</v>
       </c>
       <c r="D207" s="8" t="s">
-        <v>1163</v>
+        <v>1154</v>
       </c>
       <c r="E207" s="8" t="s">
-        <v>876</v>
+        <v>879</v>
       </c>
       <c r="F207" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G207" s="2" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="I207" s="2" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="J207" s="6" t="s">
         <v>964</v>
@@ -12444,7 +12444,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="208" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A208" s="6" t="s">
         <v>905</v>
       </c>
@@ -12452,22 +12452,22 @@
         <v>874</v>
       </c>
       <c r="C208" s="8" t="s">
-        <v>885</v>
+        <v>875</v>
       </c>
       <c r="D208" s="8" t="s">
-        <v>1164</v>
+        <v>1155</v>
       </c>
       <c r="E208" s="8" t="s">
-        <v>886</v>
+        <v>876</v>
       </c>
       <c r="F208" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G208" s="2" t="s">
-        <v>877</v>
+        <v>882</v>
       </c>
       <c r="I208" s="2" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="J208" s="6" t="s">
         <v>964</v>
@@ -12476,8 +12476,40 @@
         <v>911</v>
       </c>
     </row>
-    <row r="209" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E209" s="8"/>
+    <row r="209" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A209" s="6" t="s">
+        <v>906</v>
+      </c>
+      <c r="B209" s="6" t="s">
+        <v>874</v>
+      </c>
+      <c r="C209" s="8" t="s">
+        <v>885</v>
+      </c>
+      <c r="D209" s="8" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E209" s="8" t="s">
+        <v>886</v>
+      </c>
+      <c r="F209" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G209" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="I209" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="J209" s="6" t="s">
+        <v>964</v>
+      </c>
+      <c r="K209" s="22" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E210" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working on create resource under learning resource...
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3949" uniqueCount="1202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3951" uniqueCount="1212">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5068,9 +5068,6 @@
     <t>fi_FunctionalityofLearningResources</t>
   </si>
   <si>
-    <t>fi_FunctionalityToofLearningResources</t>
-  </si>
-  <si>
     <t>fi_FunctionalityofPlayContent</t>
   </si>
   <si>
@@ -5110,21 +5107,6 @@
     <t>fn_ViewAverageScoreofSelectedSubject</t>
   </si>
   <si>
-    <t>fi_FunctionalityToCreateofSelectingchapter</t>
-  </si>
-  <si>
-    <t>fi_FunctionalityofAnotherresources</t>
-  </si>
-  <si>
-    <t>fi_ForMandatoryFieldsOnofPopupwindow</t>
-  </si>
-  <si>
-    <t>fi_FunctionalityofOtherresources</t>
-  </si>
-  <si>
-    <t>fi_FunctionalityToTagMetadataofUploadedlink</t>
-  </si>
-  <si>
     <t>fi_ValidationsForMandatoryFieldsofPopupwindow</t>
   </si>
   <si>
@@ -5230,9 +5212,6 @@
     <t>fn_DisplayPracticeTestDetails</t>
   </si>
   <si>
-    <t>fi_ForMandatoryFieldsOnAddLinkPopupWindow</t>
-  </si>
-  <si>
     <t>fi_FunctionalityOfAssessmentGenerationCorrespondingToTheQuestions</t>
   </si>
   <si>
@@ -5257,9 +5236,6 @@
     <t>fn_ViewTheQuestionAnswerChoicestudentAnswerandrightReport</t>
   </si>
   <si>
-    <t>fi_FunctionalityToTagmetadataTotheuploadedSubjec</t>
-  </si>
-  <si>
     <t>fn_ViewMarkSheetofSelectedStudent</t>
   </si>
   <si>
@@ -5359,7 +5335,82 @@
     <t>fn_FilterLearningResources</t>
   </si>
   <si>
-    <t>fn_SearchLearningResources</t>
+    <t>fn_SearchLearningResource</t>
+  </si>
+  <si>
+    <t>fn_SearchInvalidLearningResources</t>
+  </si>
+  <si>
+    <t>fn_CreateLink</t>
+  </si>
+  <si>
+    <t>fn_CreatelinkWithoutSelectingchapter</t>
+  </si>
+  <si>
+    <t>fn_ValidationforMandatoryFieldsonAddLinkPopupWindow</t>
+  </si>
+  <si>
+    <t>fn_UploadAnotherresources</t>
+  </si>
+  <si>
+    <t>fn_TagmetadataToUploadedSubject</t>
+  </si>
+  <si>
+    <t>Need discussion over it
+1. after selecting metadata option window is misaligned and covered by header</t>
+  </si>
+  <si>
+    <t>fn_CreateAssignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learning Resources-Create Resource  </t>
+  </si>
+  <si>
+    <t>fn_CreateResource</t>
+  </si>
+  <si>
+    <t>To verify the functionality to create Resource</t>
+  </si>
+  <si>
+    <t>Name: Testing Resource
+Description: This is a testing Resource name</t>
+  </si>
+  <si>
+    <t>fn_CreateResourceWithoutSelectingchapter</t>
+  </si>
+  <si>
+    <t>fn_ValidationforMandatoryFieldsonAddResourcePopupWindow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.  On dashboard click on a Subject
+2. Select a subject for Class-Subject drop-down list 
+3. On Subjects page, click Learning Resources  tab
+4. Select a class and subject from Class-Subject drop-down list at the left top corner of the page
+5. Select a chapter on the left pane to which you wish to add a link
+6. Select Resource option from Create drop-down list
+7. Click on Upload link without entering name
+8. Enter name and click Upload link without choosing  file field
+</t>
+  </si>
+  <si>
+    <t>1.  On dashboard click on a Subject
+2. Select a subject for Class-Subject drop-down list 
+3. On Subjects page, click Learning Resources  tab
+4. Select a class and subject from Class-Subject drop-down list at the left top corner of the page
+5. Select a chapter on the left pane to which you wish to add a link
+6. Select Resource option from Create drop-down list
+7. Enter a name for the link in Name text box
+8. Set the time duration for the resource from Hours and Minutes drop-down lists
+9. Enter a brief description about the resource link in Description text box
+10. Enter a purpose for the resource link in Purpose text box
+11. Enter a valid link in Upload link text box
+12.  Click on Upload Link</t>
+  </si>
+  <si>
+    <t>fn_UploadAnotherLearningResource</t>
+  </si>
+  <si>
+    <t>After deleted loader is moving on for long time</t>
   </si>
 </sst>
 </file>
@@ -5837,8 +5888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8452,7 +8503,7 @@
         <v>347</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>352</v>
@@ -8484,7 +8535,7 @@
         <v>347</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>1157</v>
+        <v>1151</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>355</v>
@@ -8516,7 +8567,7 @@
         <v>347</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>1165</v>
+        <v>1158</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>360</v>
@@ -8548,7 +8599,7 @@
         <v>347</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>1166</v>
+        <v>1159</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>364</v>
@@ -8580,7 +8631,7 @@
         <v>368</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>1168</v>
+        <v>1160</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>370</v>
@@ -8612,7 +8663,7 @@
         <v>368</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>1169</v>
+        <v>1161</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>374</v>
@@ -8642,7 +8693,7 @@
         <v>377</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>1170</v>
+        <v>1162</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>382</v>
@@ -8671,7 +8722,7 @@
         <v>381</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>1171</v>
+        <v>1163</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>384</v>
@@ -8703,7 +8754,7 @@
         <v>381</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>1172</v>
+        <v>1164</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>386</v>
@@ -8735,7 +8786,7 @@
         <v>381</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>1173</v>
+        <v>1165</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>390</v>
@@ -8767,7 +8818,7 @@
         <v>381</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>1174</v>
+        <v>1166</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>394</v>
@@ -8799,7 +8850,7 @@
         <v>381</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>1175</v>
+        <v>1167</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>398</v>
@@ -8831,7 +8882,7 @@
         <v>381</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>1176</v>
+        <v>1168</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>403</v>
@@ -8863,7 +8914,7 @@
         <v>381</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>1177</v>
+        <v>1169</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>407</v>
@@ -8895,7 +8946,7 @@
         <v>414</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>1178</v>
+        <v>1170</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>412</v>
@@ -8927,7 +8978,7 @@
         <v>414</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>1179</v>
+        <v>1171</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>416</v>
@@ -8959,7 +9010,7 @@
         <v>425</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>1180</v>
+        <v>1172</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>424</v>
@@ -8991,7 +9042,7 @@
         <v>422</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>1181</v>
+        <v>1173</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>427</v>
@@ -9023,7 +9074,7 @@
         <v>422</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>1182</v>
+        <v>1174</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>429</v>
@@ -9044,7 +9095,7 @@
         <v>1012</v>
       </c>
       <c r="L101" s="8" t="s">
-        <v>1183</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="195" x14ac:dyDescent="0.25">
@@ -9058,7 +9109,7 @@
         <v>422</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>1184</v>
+        <v>1176</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>436</v>
@@ -9090,7 +9141,7 @@
         <v>422</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>1185</v>
+        <v>1177</v>
       </c>
       <c r="E103" s="8" t="s">
         <v>438</v>
@@ -9119,7 +9170,7 @@
         <v>442</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>1186</v>
+        <v>1178</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>443</v>
@@ -9151,7 +9202,7 @@
         <v>442</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>1187</v>
+        <v>1179</v>
       </c>
       <c r="E105" s="8" t="s">
         <v>446</v>
@@ -9183,7 +9234,7 @@
         <v>442</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>1188</v>
+        <v>1180</v>
       </c>
       <c r="E106" s="8" t="s">
         <v>451</v>
@@ -9215,7 +9266,7 @@
         <v>442</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>1189</v>
+        <v>1181</v>
       </c>
       <c r="E107" s="8" t="s">
         <v>455</v>
@@ -9244,7 +9295,7 @@
         <v>458</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>1190</v>
+        <v>1182</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>460</v>
@@ -9258,8 +9309,8 @@
       <c r="J108" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K108" s="6" t="s">
-        <v>911</v>
+      <c r="K108" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="109" spans="1:12" ht="135" x14ac:dyDescent="0.25">
@@ -9273,7 +9324,7 @@
         <v>458</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>1191</v>
+        <v>1183</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>620</v>
@@ -9302,7 +9353,7 @@
         <v>458</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>1192</v>
+        <v>1184</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>621</v>
@@ -9331,7 +9382,7 @@
         <v>464</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>465</v>
@@ -9357,10 +9408,10 @@
         <v>411</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>1196</v>
+        <v>1188</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>1195</v>
+        <v>1187</v>
       </c>
       <c r="E112" s="8"/>
       <c r="G112" s="2"/>
@@ -9380,7 +9431,7 @@
         <v>468</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>1194</v>
+        <v>1186</v>
       </c>
       <c r="E113" s="8" t="s">
         <v>471</v>
@@ -9394,8 +9445,8 @@
       <c r="J113" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K113" s="6" t="s">
-        <v>911</v>
+      <c r="K113" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="114" spans="1:12" ht="210" x14ac:dyDescent="0.25">
@@ -9409,7 +9460,7 @@
         <v>472</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>1197</v>
+        <v>1189</v>
       </c>
       <c r="E114" s="8" t="s">
         <v>474</v>
@@ -9438,7 +9489,7 @@
         <v>481</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>1198</v>
+        <v>1190</v>
       </c>
       <c r="E115" s="8" t="s">
         <v>424</v>
@@ -9455,8 +9506,8 @@
       <c r="J115" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K115" s="6" t="s">
-        <v>911</v>
+      <c r="K115" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="116" spans="1:12" ht="150" x14ac:dyDescent="0.25">
@@ -9470,7 +9521,7 @@
         <v>477</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>1199</v>
+        <v>1191</v>
       </c>
       <c r="E116" s="8" t="s">
         <v>478</v>
@@ -9487,8 +9538,8 @@
       <c r="J116" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K116" s="6" t="s">
-        <v>911</v>
+      <c r="K116" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="117" spans="1:12" ht="165" x14ac:dyDescent="0.25">
@@ -9502,7 +9553,7 @@
         <v>486</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>1200</v>
+        <v>1192</v>
       </c>
       <c r="E117" s="8" t="s">
         <v>487</v>
@@ -9534,7 +9585,7 @@
         <v>490</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>1201</v>
+        <v>1193</v>
       </c>
       <c r="E118" s="8" t="s">
         <v>491</v>
@@ -9551,8 +9602,8 @@
       <c r="J118" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K118" s="6" t="s">
-        <v>911</v>
+      <c r="K118" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="119" spans="1:12" ht="150" x14ac:dyDescent="0.25">
@@ -9566,7 +9617,7 @@
         <v>490</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>1104</v>
+        <v>1194</v>
       </c>
       <c r="E119" s="8" t="s">
         <v>495</v>
@@ -9583,8 +9634,8 @@
       <c r="J119" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K119" s="6" t="s">
-        <v>911</v>
+      <c r="K119" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="120" spans="1:12" ht="315" x14ac:dyDescent="0.25">
@@ -9598,7 +9649,7 @@
         <v>498</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>999</v>
+        <v>1195</v>
       </c>
       <c r="E120" s="8" t="s">
         <v>500</v>
@@ -9633,7 +9684,7 @@
         <v>498</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>1118</v>
+        <v>1196</v>
       </c>
       <c r="E121" s="8" t="s">
         <v>505</v>
@@ -9665,7 +9716,7 @@
         <v>498</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>1158</v>
+        <v>1197</v>
       </c>
       <c r="E122" s="8" t="s">
         <v>508</v>
@@ -9683,10 +9734,10 @@
       <c r="J122" s="8" t="s">
         <v>972</v>
       </c>
-      <c r="K122" s="8" t="s">
-        <v>911</v>
-      </c>
-      <c r="L122" s="8" t="s">
+      <c r="K122" t="s">
+        <v>1012</v>
+      </c>
+      <c r="L122" s="20" t="s">
         <v>974</v>
       </c>
     </row>
@@ -9701,7 +9752,7 @@
         <v>498</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>1119</v>
+        <v>1198</v>
       </c>
       <c r="E123" s="8" t="s">
         <v>513</v>
@@ -9734,7 +9785,7 @@
         <v>498</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>1167</v>
+        <v>1199</v>
       </c>
       <c r="E124" s="8" t="s">
         <v>521</v>
@@ -9752,11 +9803,11 @@
       <c r="K124" s="8" t="s">
         <v>911</v>
       </c>
-      <c r="L124" s="8" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="125" spans="1:12" ht="360" x14ac:dyDescent="0.25">
+      <c r="L124" s="20" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" ht="315" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
         <v>539</v>
       </c>
@@ -9764,31 +9815,31 @@
         <v>411</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>517</v>
+        <v>1202</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>999</v>
+        <v>1203</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>518</v>
+        <v>1204</v>
       </c>
       <c r="F125" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>531</v>
+        <v>1209</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>542</v>
+        <v>1205</v>
       </c>
       <c r="I125" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="K125" s="22" t="s">
+        <v>502</v>
+      </c>
+      <c r="K125" s="8" t="s">
         <v>911</v>
       </c>
       <c r="L125" s="20" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
     </row>
     <row r="126" spans="1:12" ht="75" x14ac:dyDescent="0.25">
@@ -9799,31 +9850,31 @@
         <v>411</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>517</v>
+        <v>498</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>1118</v>
+        <v>1206</v>
       </c>
       <c r="E126" s="8" t="s">
-        <v>525</v>
+        <v>505</v>
       </c>
       <c r="F126" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>526</v>
+        <v>506</v>
       </c>
       <c r="I126" s="2" t="s">
-        <v>527</v>
+        <v>507</v>
       </c>
       <c r="J126" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K126" s="8" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="127" spans="1:12" ht="255" x14ac:dyDescent="0.25">
+      <c r="K126" s="6" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" ht="270" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
         <v>547</v>
       </c>
@@ -9831,23 +9882,23 @@
         <v>411</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>517</v>
+        <v>498</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>1120</v>
+        <v>1207</v>
       </c>
       <c r="E127" s="8" t="s">
-        <v>528</v>
+        <v>508</v>
       </c>
       <c r="F127" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>529</v>
+        <v>1208</v>
       </c>
       <c r="H127" s="2"/>
       <c r="I127" s="2" t="s">
-        <v>530</v>
+        <v>511</v>
       </c>
       <c r="J127" s="8" t="s">
         <v>972</v>
@@ -9855,8 +9906,11 @@
       <c r="K127" s="8" t="s">
         <v>911</v>
       </c>
-    </row>
-    <row r="128" spans="1:12" ht="375" x14ac:dyDescent="0.25">
+      <c r="L127" s="20" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" ht="345" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
         <v>551</v>
       </c>
@@ -9864,23 +9918,23 @@
         <v>411</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>517</v>
+        <v>498</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>1121</v>
+        <v>1210</v>
       </c>
       <c r="E128" s="8" t="s">
-        <v>533</v>
+        <v>513</v>
       </c>
       <c r="F128" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="H128" s="2"/>
       <c r="I128" s="2" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="J128" s="8" t="s">
         <v>972</v>
@@ -9889,7 +9943,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="360" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" ht="345" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>556</v>
       </c>
@@ -9897,10 +9951,10 @@
         <v>411</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>517</v>
+        <v>498</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>1122</v>
+        <v>1199</v>
       </c>
       <c r="E129" s="8" t="s">
         <v>521</v>
@@ -9909,17 +9963,17 @@
         <v>38</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>534</v>
+        <v>522</v>
       </c>
       <c r="H129" s="2"/>
       <c r="I129" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="J129" s="8" t="s">
-        <v>972</v>
+        <v>523</v>
       </c>
       <c r="K129" s="8" t="s">
         <v>911</v>
+      </c>
+      <c r="L129" s="20" t="s">
+        <v>1200</v>
       </c>
     </row>
     <row r="130" spans="1:12" ht="375" x14ac:dyDescent="0.25">
@@ -9933,7 +9987,7 @@
         <v>540</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>999</v>
+        <v>1201</v>
       </c>
       <c r="E130" s="8" t="s">
         <v>543</v>
@@ -9965,7 +10019,7 @@
         <v>540</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>1123</v>
+        <v>1117</v>
       </c>
       <c r="E131" s="8" t="s">
         <v>548</v>
@@ -10018,6 +10072,9 @@
       <c r="K132" s="8" t="s">
         <v>911</v>
       </c>
+      <c r="L132" s="20" t="s">
+        <v>1211</v>
+      </c>
     </row>
     <row r="133" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
@@ -10030,7 +10087,7 @@
         <v>552</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>1124</v>
+        <v>1118</v>
       </c>
       <c r="E133" s="8" t="s">
         <v>557</v>
@@ -10062,7 +10119,7 @@
         <v>561</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="E134" s="8" t="s">
         <v>562</v>
@@ -10094,7 +10151,7 @@
         <v>561</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>1125</v>
+        <v>1119</v>
       </c>
       <c r="E135" s="8" t="s">
         <v>565</v>
@@ -10126,7 +10183,7 @@
         <v>561</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>1126</v>
+        <v>1120</v>
       </c>
       <c r="E136" s="8" t="s">
         <v>568</v>
@@ -10158,7 +10215,7 @@
         <v>561</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>1127</v>
+        <v>1121</v>
       </c>
       <c r="E137" s="8" t="s">
         <v>572</v>
@@ -10190,7 +10247,7 @@
         <v>561</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>1128</v>
+        <v>1122</v>
       </c>
       <c r="E138" s="8" t="s">
         <v>576</v>
@@ -10222,7 +10279,7 @@
         <v>581</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>1129</v>
+        <v>1123</v>
       </c>
       <c r="E139" s="6" t="s">
         <v>582</v>
@@ -10254,7 +10311,7 @@
         <v>581</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>1130</v>
+        <v>1124</v>
       </c>
       <c r="E140" s="8" t="s">
         <v>625</v>
@@ -10286,7 +10343,7 @@
         <v>581</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>1131</v>
+        <v>1125</v>
       </c>
       <c r="E141" s="8" t="s">
         <v>628</v>
@@ -10318,7 +10375,7 @@
         <v>581</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>1132</v>
+        <v>1126</v>
       </c>
       <c r="E142" s="8" t="s">
         <v>586</v>
@@ -10350,7 +10407,7 @@
         <v>594</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>1159</v>
+        <v>1152</v>
       </c>
       <c r="E143" s="8" t="s">
         <v>593</v>
@@ -10385,7 +10442,7 @@
         <v>595</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>1133</v>
+        <v>1127</v>
       </c>
       <c r="E144" s="8" t="s">
         <v>596</v>
@@ -10417,7 +10474,7 @@
         <v>595</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>1134</v>
+        <v>1128</v>
       </c>
       <c r="E145" s="8" t="s">
         <v>600</v>
@@ -10481,7 +10538,7 @@
         <v>595</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E147" s="8" t="s">
         <v>609</v>
@@ -10513,7 +10570,7 @@
         <v>595</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>1134</v>
+        <v>1128</v>
       </c>
       <c r="E148" s="8" t="s">
         <v>612</v>
@@ -10812,7 +10869,7 @@
         <v>665</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>1135</v>
+        <v>1129</v>
       </c>
       <c r="E158" s="8" t="s">
         <v>694</v>
@@ -10877,7 +10934,7 @@
         <v>665</v>
       </c>
       <c r="D160" s="8" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="E160" s="8" t="s">
         <v>675</v>
@@ -10909,7 +10966,7 @@
         <v>665</v>
       </c>
       <c r="D161" s="8" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E161" s="8" t="s">
         <v>679</v>
@@ -10941,7 +10998,7 @@
         <v>665</v>
       </c>
       <c r="D162" s="8" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E162" s="8" t="s">
         <v>683</v>
@@ -10973,7 +11030,7 @@
         <v>665</v>
       </c>
       <c r="D163" s="8" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E163" s="8" t="s">
         <v>687</v>
@@ -11005,7 +11062,7 @@
         <v>665</v>
       </c>
       <c r="D164" s="8" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="E164" s="8" t="s">
         <v>691</v>
@@ -11037,7 +11094,7 @@
         <v>699</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>1160</v>
+        <v>1153</v>
       </c>
       <c r="E165" s="8" t="s">
         <v>700</v>
@@ -11066,7 +11123,7 @@
         <v>699</v>
       </c>
       <c r="D166" s="8" t="s">
-        <v>1136</v>
+        <v>1130</v>
       </c>
       <c r="E166" s="8" t="s">
         <v>704</v>
@@ -11098,7 +11155,7 @@
         <v>699</v>
       </c>
       <c r="D167" s="8" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E167" s="8" t="s">
         <v>707</v>
@@ -11130,7 +11187,7 @@
         <v>699</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="E168" s="8" t="s">
         <v>710</v>
@@ -11191,7 +11248,7 @@
         <v>713</v>
       </c>
       <c r="D170" s="8" t="s">
-        <v>1137</v>
+        <v>1131</v>
       </c>
       <c r="E170" s="8" t="s">
         <v>718</v>
@@ -11223,7 +11280,7 @@
         <v>713</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>1138</v>
+        <v>1132</v>
       </c>
       <c r="E171" s="8" t="s">
         <v>722</v>
@@ -11255,7 +11312,7 @@
         <v>713</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>1139</v>
+        <v>1133</v>
       </c>
       <c r="E172" s="8" t="s">
         <v>726</v>
@@ -11287,7 +11344,7 @@
         <v>713</v>
       </c>
       <c r="D173" s="8" t="s">
-        <v>1140</v>
+        <v>1134</v>
       </c>
       <c r="E173" s="10" t="s">
         <v>731</v>
@@ -11336,7 +11393,7 @@
         <v>735</v>
       </c>
       <c r="D174" s="8" t="s">
-        <v>1141</v>
+        <v>1135</v>
       </c>
       <c r="E174" s="14" t="s">
         <v>748</v>
@@ -11414,7 +11471,7 @@
         <v>736</v>
       </c>
       <c r="D176" s="8" t="s">
-        <v>1161</v>
+        <v>1154</v>
       </c>
       <c r="E176" s="8" t="s">
         <v>741</v>
@@ -11554,7 +11611,7 @@
         <v>753</v>
       </c>
       <c r="D180" s="8" t="s">
-        <v>1142</v>
+        <v>1136</v>
       </c>
       <c r="E180" s="8" t="s">
         <v>764</v>
@@ -11586,7 +11643,7 @@
         <v>753</v>
       </c>
       <c r="D181" s="8" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="E181" s="8" t="s">
         <v>768</v>
@@ -11618,7 +11675,7 @@
         <v>753</v>
       </c>
       <c r="D182" s="8" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="E182" s="8" t="s">
         <v>768</v>
@@ -11651,7 +11708,7 @@
         <v>753</v>
       </c>
       <c r="D183" s="8" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="E183" s="8" t="s">
         <v>768</v>
@@ -11684,7 +11741,7 @@
         <v>753</v>
       </c>
       <c r="D184" s="8" t="s">
-        <v>1143</v>
+        <v>1137</v>
       </c>
       <c r="E184" s="8" t="s">
         <v>776</v>
@@ -11716,7 +11773,7 @@
         <v>779</v>
       </c>
       <c r="D185" s="8" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="E185" s="6" t="s">
         <v>786</v>
@@ -11748,7 +11805,7 @@
         <v>784</v>
       </c>
       <c r="D186" s="8" t="s">
-        <v>1144</v>
+        <v>1138</v>
       </c>
       <c r="E186" s="6" t="s">
         <v>785</v>
@@ -11879,7 +11936,7 @@
         <v>805</v>
       </c>
       <c r="D190" s="8" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="E190" s="8" t="s">
         <v>806</v>
@@ -11911,7 +11968,7 @@
         <v>805</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>1145</v>
+        <v>1139</v>
       </c>
       <c r="E191" s="8" t="s">
         <v>809</v>
@@ -11943,7 +12000,7 @@
         <v>805</v>
       </c>
       <c r="D192" s="8" t="s">
-        <v>1146</v>
+        <v>1140</v>
       </c>
       <c r="E192" s="8" t="s">
         <v>814</v>
@@ -11975,7 +12032,7 @@
         <v>805</v>
       </c>
       <c r="D193" s="8" t="s">
-        <v>1147</v>
+        <v>1141</v>
       </c>
       <c r="E193" s="8" t="s">
         <v>826</v>
@@ -12007,7 +12064,7 @@
         <v>805</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>1162</v>
+        <v>1155</v>
       </c>
       <c r="E194" s="8" t="s">
         <v>820</v>
@@ -12042,7 +12099,7 @@
         <v>805</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>1148</v>
+        <v>1142</v>
       </c>
       <c r="E195" s="8" t="s">
         <v>823</v>
@@ -12074,7 +12131,7 @@
         <v>805</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>1149</v>
+        <v>1143</v>
       </c>
       <c r="E196" s="8" t="s">
         <v>830</v>
@@ -12106,7 +12163,7 @@
         <v>805</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>1150</v>
+        <v>1144</v>
       </c>
       <c r="E197" s="8" t="s">
         <v>837</v>
@@ -12138,7 +12195,7 @@
         <v>805</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>1151</v>
+        <v>1145</v>
       </c>
       <c r="E198" s="8" t="s">
         <v>838</v>
@@ -12170,7 +12227,7 @@
         <v>805</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>1152</v>
+        <v>1146</v>
       </c>
       <c r="E199" s="8" t="s">
         <v>842</v>
@@ -12202,7 +12259,7 @@
         <v>805</v>
       </c>
       <c r="D200" s="8" t="s">
-        <v>1163</v>
+        <v>1156</v>
       </c>
       <c r="E200" s="8" t="s">
         <v>846</v>
@@ -12234,7 +12291,7 @@
         <v>805</v>
       </c>
       <c r="D201" s="8" t="s">
-        <v>1164</v>
+        <v>1157</v>
       </c>
       <c r="E201" s="8" t="s">
         <v>850</v>
@@ -12266,7 +12323,7 @@
         <v>805</v>
       </c>
       <c r="D202" s="8" t="s">
-        <v>1153</v>
+        <v>1147</v>
       </c>
       <c r="E202" s="8" t="s">
         <v>855</v>
@@ -12298,7 +12355,7 @@
         <v>805</v>
       </c>
       <c r="D203" s="8" t="s">
-        <v>1150</v>
+        <v>1144</v>
       </c>
       <c r="E203" s="8" t="s">
         <v>862</v>
@@ -12423,7 +12480,7 @@
         <v>874</v>
       </c>
       <c r="D207" s="8" t="s">
-        <v>1154</v>
+        <v>1148</v>
       </c>
       <c r="E207" s="8" t="s">
         <v>879</v>
@@ -12455,7 +12512,7 @@
         <v>875</v>
       </c>
       <c r="D208" s="8" t="s">
-        <v>1155</v>
+        <v>1149</v>
       </c>
       <c r="E208" s="8" t="s">
         <v>876</v>
@@ -12487,7 +12544,7 @@
         <v>885</v>
       </c>
       <c r="D209" s="8" t="s">
-        <v>1156</v>
+        <v>1150</v>
       </c>
       <c r="E209" s="8" t="s">
         <v>886</v>

</xml_diff>

<commit_message>
started assignment section under learning resource...
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3951" uniqueCount="1212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3952" uniqueCount="1213">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5412,12 +5412,16 @@
   <si>
     <t>After deleted loader is moving on for long time</t>
   </si>
+  <si>
+    <t>fn_TagmetadataToLearningResource</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5888,25 +5892,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="A120" sqref="A120"/>
+    <sheetView tabSelected="1" topLeftCell="F126" workbookViewId="0">
+      <selection activeCell="K126" sqref="K126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5703125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.5703125" style="8" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.85546875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.5703125" style="6" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="41.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26" style="6" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" style="6" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="52.7109375" style="8" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="16.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="8" width="16.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="6" width="31.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="6" width="33.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="41.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="6" width="26.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="6" width="11.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="8" width="52.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -9666,8 +9670,8 @@
       <c r="I120" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="K120" s="8" t="s">
-        <v>911</v>
+      <c r="K120" t="s">
+        <v>1012</v>
       </c>
       <c r="L120" s="20" t="s">
         <v>948</v>
@@ -9701,8 +9705,8 @@
       <c r="J121" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K121" s="6" t="s">
-        <v>911</v>
+      <c r="K121" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="122" spans="1:12" ht="270" x14ac:dyDescent="0.25">
@@ -9770,8 +9774,8 @@
       <c r="J123" s="8" t="s">
         <v>972</v>
       </c>
-      <c r="K123" s="8" t="s">
-        <v>911</v>
+      <c r="K123" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="124" spans="1:12" ht="345" x14ac:dyDescent="0.25">
@@ -9800,8 +9804,8 @@
       <c r="I124" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="K124" s="8" t="s">
-        <v>911</v>
+      <c r="K124" t="s">
+        <v>1012</v>
       </c>
       <c r="L124" s="20" t="s">
         <v>1200</v>
@@ -9835,8 +9839,8 @@
       <c r="I125" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="K125" s="8" t="s">
-        <v>911</v>
+      <c r="K125" t="s">
+        <v>1012</v>
       </c>
       <c r="L125" s="20" t="s">
         <v>948</v>
@@ -9870,8 +9874,8 @@
       <c r="J126" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K126" s="6" t="s">
-        <v>911</v>
+      <c r="K126" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="127" spans="1:12" ht="270" x14ac:dyDescent="0.25">
@@ -9903,8 +9907,8 @@
       <c r="J127" s="8" t="s">
         <v>972</v>
       </c>
-      <c r="K127" s="8" t="s">
-        <v>911</v>
+      <c r="K127" t="s">
+        <v>1012</v>
       </c>
       <c r="L127" s="20" t="s">
         <v>974</v>
@@ -9954,7 +9958,7 @@
         <v>498</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>1199</v>
+        <v>1212</v>
       </c>
       <c r="E129" s="8" t="s">
         <v>521</v>
@@ -10004,7 +10008,7 @@
       <c r="I130" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="K130" s="20" t="s">
+      <c r="L130" s="20" t="s">
         <v>951</v>
       </c>
     </row>
@@ -12584,17 +12588,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working on resource section....
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3952" uniqueCount="1213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3951" uniqueCount="1213">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5065,12 +5065,6 @@
     <t>fA_AddRemarkforstudent'sFeedbackofView</t>
   </si>
   <si>
-    <t>fi_FunctionalityofLearningResources</t>
-  </si>
-  <si>
-    <t>fi_FunctionalityofPlayContent</t>
-  </si>
-  <si>
     <t>fi_ValidationsForMandatoryFieldsOnSaveAssessmentWindowofAssessmentGeneration</t>
   </si>
   <si>
@@ -5105,15 +5099,6 @@
   </si>
   <si>
     <t>fn_ViewAverageScoreofSelectedSubject</t>
-  </si>
-  <si>
-    <t>fi_ValidationsForMandatoryFieldsofPopupwindow</t>
-  </si>
-  <si>
-    <t>fi_FunctionalityToDeleteLearningResourcesByClickingOn'No'InConfirmationPopupofTotalnumber</t>
-  </si>
-  <si>
-    <t>fi_FunctionalityToofPlayedresource</t>
   </si>
   <si>
     <t>fi_FunctionalityToofLearningresource</t>
@@ -5415,13 +5400,27 @@
   <si>
     <t>fn_TagmetadataToLearningResource</t>
   </si>
+  <si>
+    <t>fn_ValidationsForMandatoryFieldsonAssignPopupwindow</t>
+  </si>
+  <si>
+    <t>fn_DeleteLearningResources</t>
+  </si>
+  <si>
+    <t>fn_DeleteResourcesByClickingOnNoInConfirmation</t>
+  </si>
+  <si>
+    <t>fn_PlayContent</t>
+  </si>
+  <si>
+    <t>fn_SavePlayedresource</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5892,25 +5891,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F126" workbookViewId="0">
-      <selection activeCell="K126" sqref="K126"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="18.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="16.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="8" width="16.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="6" width="31.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="6" width="33.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="41.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="6" width="26.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="6" width="11.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="8" width="52.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.5703125" style="8" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.85546875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.5703125" style="6" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="41.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26" style="6" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" style="6" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="52.7109375" style="8" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -8507,7 +8506,7 @@
         <v>347</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>352</v>
@@ -8539,7 +8538,7 @@
         <v>347</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>1151</v>
+        <v>1146</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>355</v>
@@ -8571,7 +8570,7 @@
         <v>347</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>1158</v>
+        <v>1153</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>360</v>
@@ -8603,7 +8602,7 @@
         <v>347</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>1159</v>
+        <v>1154</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>364</v>
@@ -8635,7 +8634,7 @@
         <v>368</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>1160</v>
+        <v>1155</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>370</v>
@@ -8667,7 +8666,7 @@
         <v>368</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>1161</v>
+        <v>1156</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>374</v>
@@ -8697,7 +8696,7 @@
         <v>377</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>1162</v>
+        <v>1157</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>382</v>
@@ -8726,7 +8725,7 @@
         <v>381</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>1163</v>
+        <v>1158</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>384</v>
@@ -8758,7 +8757,7 @@
         <v>381</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>1164</v>
+        <v>1159</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>386</v>
@@ -8790,7 +8789,7 @@
         <v>381</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>1165</v>
+        <v>1160</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>390</v>
@@ -8822,7 +8821,7 @@
         <v>381</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>1166</v>
+        <v>1161</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>394</v>
@@ -8854,7 +8853,7 @@
         <v>381</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>1167</v>
+        <v>1162</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>398</v>
@@ -8886,7 +8885,7 @@
         <v>381</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>1168</v>
+        <v>1163</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>403</v>
@@ -8918,7 +8917,7 @@
         <v>381</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>1169</v>
+        <v>1164</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>407</v>
@@ -8950,7 +8949,7 @@
         <v>414</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>412</v>
@@ -8982,7 +8981,7 @@
         <v>414</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>1171</v>
+        <v>1166</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>416</v>
@@ -9014,7 +9013,7 @@
         <v>425</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>1172</v>
+        <v>1167</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>424</v>
@@ -9046,7 +9045,7 @@
         <v>422</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>1173</v>
+        <v>1168</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>427</v>
@@ -9078,7 +9077,7 @@
         <v>422</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>1174</v>
+        <v>1169</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>429</v>
@@ -9099,7 +9098,7 @@
         <v>1012</v>
       </c>
       <c r="L101" s="8" t="s">
-        <v>1175</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="195" x14ac:dyDescent="0.25">
@@ -9113,7 +9112,7 @@
         <v>422</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>436</v>
@@ -9145,7 +9144,7 @@
         <v>422</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>1177</v>
+        <v>1172</v>
       </c>
       <c r="E103" s="8" t="s">
         <v>438</v>
@@ -9174,7 +9173,7 @@
         <v>442</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>1178</v>
+        <v>1173</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>443</v>
@@ -9206,7 +9205,7 @@
         <v>442</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>1179</v>
+        <v>1174</v>
       </c>
       <c r="E105" s="8" t="s">
         <v>446</v>
@@ -9238,7 +9237,7 @@
         <v>442</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>1180</v>
+        <v>1175</v>
       </c>
       <c r="E106" s="8" t="s">
         <v>451</v>
@@ -9270,7 +9269,7 @@
         <v>442</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>1181</v>
+        <v>1176</v>
       </c>
       <c r="E107" s="8" t="s">
         <v>455</v>
@@ -9299,7 +9298,7 @@
         <v>458</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>1182</v>
+        <v>1177</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>460</v>
@@ -9328,7 +9327,7 @@
         <v>458</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>1183</v>
+        <v>1178</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>620</v>
@@ -9357,7 +9356,7 @@
         <v>458</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>1184</v>
+        <v>1179</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>621</v>
@@ -9386,7 +9385,7 @@
         <v>464</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>465</v>
@@ -9412,10 +9411,10 @@
         <v>411</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>1188</v>
+        <v>1183</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>1187</v>
+        <v>1182</v>
       </c>
       <c r="E112" s="8"/>
       <c r="G112" s="2"/>
@@ -9435,7 +9434,7 @@
         <v>468</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>1186</v>
+        <v>1181</v>
       </c>
       <c r="E113" s="8" t="s">
         <v>471</v>
@@ -9464,7 +9463,7 @@
         <v>472</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>1189</v>
+        <v>1184</v>
       </c>
       <c r="E114" s="8" t="s">
         <v>474</v>
@@ -9493,7 +9492,7 @@
         <v>481</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>1190</v>
+        <v>1185</v>
       </c>
       <c r="E115" s="8" t="s">
         <v>424</v>
@@ -9525,7 +9524,7 @@
         <v>477</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>1191</v>
+        <v>1186</v>
       </c>
       <c r="E116" s="8" t="s">
         <v>478</v>
@@ -9557,7 +9556,7 @@
         <v>486</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>1192</v>
+        <v>1187</v>
       </c>
       <c r="E117" s="8" t="s">
         <v>487</v>
@@ -9589,7 +9588,7 @@
         <v>490</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>1193</v>
+        <v>1188</v>
       </c>
       <c r="E118" s="8" t="s">
         <v>491</v>
@@ -9621,7 +9620,7 @@
         <v>490</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>1194</v>
+        <v>1189</v>
       </c>
       <c r="E119" s="8" t="s">
         <v>495</v>
@@ -9653,7 +9652,7 @@
         <v>498</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>1195</v>
+        <v>1190</v>
       </c>
       <c r="E120" s="8" t="s">
         <v>500</v>
@@ -9688,7 +9687,7 @@
         <v>498</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>1196</v>
+        <v>1191</v>
       </c>
       <c r="E121" s="8" t="s">
         <v>505</v>
@@ -9720,7 +9719,7 @@
         <v>498</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>1197</v>
+        <v>1192</v>
       </c>
       <c r="E122" s="8" t="s">
         <v>508</v>
@@ -9756,7 +9755,7 @@
         <v>498</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>1198</v>
+        <v>1193</v>
       </c>
       <c r="E123" s="8" t="s">
         <v>513</v>
@@ -9789,7 +9788,7 @@
         <v>498</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>1199</v>
+        <v>1194</v>
       </c>
       <c r="E124" s="8" t="s">
         <v>521</v>
@@ -9808,7 +9807,7 @@
         <v>1012</v>
       </c>
       <c r="L124" s="20" t="s">
-        <v>1200</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="125" spans="1:12" ht="315" x14ac:dyDescent="0.25">
@@ -9819,22 +9818,22 @@
         <v>411</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>1202</v>
+        <v>1197</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>1203</v>
+        <v>1198</v>
       </c>
       <c r="E125" s="8" t="s">
+        <v>1199</v>
+      </c>
+      <c r="F125" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G125" s="2" t="s">
         <v>1204</v>
       </c>
-      <c r="F125" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G125" s="2" t="s">
-        <v>1209</v>
-      </c>
       <c r="H125" s="2" t="s">
-        <v>1205</v>
+        <v>1200</v>
       </c>
       <c r="I125" s="2" t="s">
         <v>502</v>
@@ -9857,7 +9856,7 @@
         <v>498</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>1206</v>
+        <v>1201</v>
       </c>
       <c r="E126" s="8" t="s">
         <v>505</v>
@@ -9889,7 +9888,7 @@
         <v>498</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>1207</v>
+        <v>1202</v>
       </c>
       <c r="E127" s="8" t="s">
         <v>508</v>
@@ -9898,7 +9897,7 @@
         <v>38</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>1208</v>
+        <v>1203</v>
       </c>
       <c r="H127" s="2"/>
       <c r="I127" s="2" t="s">
@@ -9925,7 +9924,7 @@
         <v>498</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>1210</v>
+        <v>1205</v>
       </c>
       <c r="E128" s="8" t="s">
         <v>513</v>
@@ -9943,8 +9942,8 @@
       <c r="J128" s="8" t="s">
         <v>972</v>
       </c>
-      <c r="K128" s="8" t="s">
-        <v>911</v>
+      <c r="K128" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="129" spans="1:12" ht="345" x14ac:dyDescent="0.25">
@@ -9958,7 +9957,7 @@
         <v>498</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>1212</v>
+        <v>1207</v>
       </c>
       <c r="E129" s="8" t="s">
         <v>521</v>
@@ -9977,7 +9976,7 @@
         <v>911</v>
       </c>
       <c r="L129" s="20" t="s">
-        <v>1200</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="130" spans="1:12" ht="375" x14ac:dyDescent="0.25">
@@ -9991,7 +9990,7 @@
         <v>540</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>1201</v>
+        <v>1196</v>
       </c>
       <c r="E130" s="8" t="s">
         <v>543</v>
@@ -10023,7 +10022,7 @@
         <v>540</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>1117</v>
+        <v>1208</v>
       </c>
       <c r="E131" s="8" t="s">
         <v>548</v>
@@ -10041,8 +10040,8 @@
       <c r="J131" s="8" t="s">
         <v>972</v>
       </c>
-      <c r="K131" s="8" t="s">
-        <v>911</v>
+      <c r="K131" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="132" spans="1:12" ht="165" x14ac:dyDescent="0.25">
@@ -10056,7 +10055,7 @@
         <v>552</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>1103</v>
+        <v>1209</v>
       </c>
       <c r="E132" s="8" t="s">
         <v>553</v>
@@ -10073,11 +10072,11 @@
       <c r="J132" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K132" s="8" t="s">
-        <v>911</v>
+      <c r="K132" t="s">
+        <v>1012</v>
       </c>
       <c r="L132" s="20" t="s">
-        <v>1211</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="133" spans="1:12" ht="165" x14ac:dyDescent="0.25">
@@ -10091,7 +10090,7 @@
         <v>552</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>1118</v>
+        <v>1210</v>
       </c>
       <c r="E133" s="8" t="s">
         <v>557</v>
@@ -10108,8 +10107,8 @@
       <c r="J133" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K133" s="8" t="s">
-        <v>911</v>
+      <c r="K133" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="134" spans="1:12" ht="150" x14ac:dyDescent="0.25">
@@ -10123,7 +10122,7 @@
         <v>561</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>1104</v>
+        <v>1211</v>
       </c>
       <c r="E134" s="8" t="s">
         <v>562</v>
@@ -10140,8 +10139,8 @@
       <c r="J134" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K134" s="8" t="s">
-        <v>911</v>
+      <c r="K134" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="135" spans="1:12" ht="195" x14ac:dyDescent="0.25">
@@ -10155,7 +10154,7 @@
         <v>561</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>1119</v>
+        <v>1212</v>
       </c>
       <c r="E135" s="8" t="s">
         <v>565</v>
@@ -10172,8 +10171,8 @@
       <c r="J135" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K135" s="8" t="s">
-        <v>911</v>
+      <c r="K135" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="136" spans="1:12" ht="195" x14ac:dyDescent="0.25">
@@ -10187,7 +10186,7 @@
         <v>561</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>1120</v>
+        <v>1115</v>
       </c>
       <c r="E136" s="8" t="s">
         <v>568</v>
@@ -10219,7 +10218,7 @@
         <v>561</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>1121</v>
+        <v>1116</v>
       </c>
       <c r="E137" s="8" t="s">
         <v>572</v>
@@ -10251,7 +10250,7 @@
         <v>561</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>1122</v>
+        <v>1117</v>
       </c>
       <c r="E138" s="8" t="s">
         <v>576</v>
@@ -10283,7 +10282,7 @@
         <v>581</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>1123</v>
+        <v>1118</v>
       </c>
       <c r="E139" s="6" t="s">
         <v>582</v>
@@ -10315,7 +10314,7 @@
         <v>581</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>1124</v>
+        <v>1119</v>
       </c>
       <c r="E140" s="8" t="s">
         <v>625</v>
@@ -10347,7 +10346,7 @@
         <v>581</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>1125</v>
+        <v>1120</v>
       </c>
       <c r="E141" s="8" t="s">
         <v>628</v>
@@ -10379,7 +10378,7 @@
         <v>581</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>1126</v>
+        <v>1121</v>
       </c>
       <c r="E142" s="8" t="s">
         <v>586</v>
@@ -10411,7 +10410,7 @@
         <v>594</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>1152</v>
+        <v>1147</v>
       </c>
       <c r="E143" s="8" t="s">
         <v>593</v>
@@ -10446,7 +10445,7 @@
         <v>595</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>1127</v>
+        <v>1122</v>
       </c>
       <c r="E144" s="8" t="s">
         <v>596</v>
@@ -10478,7 +10477,7 @@
         <v>595</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>1128</v>
+        <v>1123</v>
       </c>
       <c r="E145" s="8" t="s">
         <v>600</v>
@@ -10542,7 +10541,7 @@
         <v>595</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="E147" s="8" t="s">
         <v>609</v>
@@ -10574,7 +10573,7 @@
         <v>595</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>1128</v>
+        <v>1123</v>
       </c>
       <c r="E148" s="8" t="s">
         <v>612</v>
@@ -10873,7 +10872,7 @@
         <v>665</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>1129</v>
+        <v>1124</v>
       </c>
       <c r="E158" s="8" t="s">
         <v>694</v>
@@ -10938,7 +10937,7 @@
         <v>665</v>
       </c>
       <c r="D160" s="8" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="E160" s="8" t="s">
         <v>675</v>
@@ -10970,7 +10969,7 @@
         <v>665</v>
       </c>
       <c r="D161" s="8" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="E161" s="8" t="s">
         <v>679</v>
@@ -11002,7 +11001,7 @@
         <v>665</v>
       </c>
       <c r="D162" s="8" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="E162" s="8" t="s">
         <v>683</v>
@@ -11034,7 +11033,7 @@
         <v>665</v>
       </c>
       <c r="D163" s="8" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="E163" s="8" t="s">
         <v>687</v>
@@ -11066,7 +11065,7 @@
         <v>665</v>
       </c>
       <c r="D164" s="8" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="E164" s="8" t="s">
         <v>691</v>
@@ -11098,7 +11097,7 @@
         <v>699</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>1153</v>
+        <v>1148</v>
       </c>
       <c r="E165" s="8" t="s">
         <v>700</v>
@@ -11127,7 +11126,7 @@
         <v>699</v>
       </c>
       <c r="D166" s="8" t="s">
-        <v>1130</v>
+        <v>1125</v>
       </c>
       <c r="E166" s="8" t="s">
         <v>704</v>
@@ -11159,7 +11158,7 @@
         <v>699</v>
       </c>
       <c r="D167" s="8" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="E167" s="8" t="s">
         <v>707</v>
@@ -11191,7 +11190,7 @@
         <v>699</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="E168" s="8" t="s">
         <v>710</v>
@@ -11252,7 +11251,7 @@
         <v>713</v>
       </c>
       <c r="D170" s="8" t="s">
-        <v>1131</v>
+        <v>1126</v>
       </c>
       <c r="E170" s="8" t="s">
         <v>718</v>
@@ -11284,7 +11283,7 @@
         <v>713</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>1132</v>
+        <v>1127</v>
       </c>
       <c r="E171" s="8" t="s">
         <v>722</v>
@@ -11316,7 +11315,7 @@
         <v>713</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>1133</v>
+        <v>1128</v>
       </c>
       <c r="E172" s="8" t="s">
         <v>726</v>
@@ -11348,7 +11347,7 @@
         <v>713</v>
       </c>
       <c r="D173" s="8" t="s">
-        <v>1134</v>
+        <v>1129</v>
       </c>
       <c r="E173" s="10" t="s">
         <v>731</v>
@@ -11397,7 +11396,7 @@
         <v>735</v>
       </c>
       <c r="D174" s="8" t="s">
-        <v>1135</v>
+        <v>1130</v>
       </c>
       <c r="E174" s="14" t="s">
         <v>748</v>
@@ -11475,7 +11474,7 @@
         <v>736</v>
       </c>
       <c r="D176" s="8" t="s">
-        <v>1154</v>
+        <v>1149</v>
       </c>
       <c r="E176" s="8" t="s">
         <v>741</v>
@@ -11615,7 +11614,7 @@
         <v>753</v>
       </c>
       <c r="D180" s="8" t="s">
-        <v>1136</v>
+        <v>1131</v>
       </c>
       <c r="E180" s="8" t="s">
         <v>764</v>
@@ -11647,7 +11646,7 @@
         <v>753</v>
       </c>
       <c r="D181" s="8" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="E181" s="8" t="s">
         <v>768</v>
@@ -11679,7 +11678,7 @@
         <v>753</v>
       </c>
       <c r="D182" s="8" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="E182" s="8" t="s">
         <v>768</v>
@@ -11712,7 +11711,7 @@
         <v>753</v>
       </c>
       <c r="D183" s="8" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="E183" s="8" t="s">
         <v>768</v>
@@ -11745,7 +11744,7 @@
         <v>753</v>
       </c>
       <c r="D184" s="8" t="s">
-        <v>1137</v>
+        <v>1132</v>
       </c>
       <c r="E184" s="8" t="s">
         <v>776</v>
@@ -11777,7 +11776,7 @@
         <v>779</v>
       </c>
       <c r="D185" s="8" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="E185" s="6" t="s">
         <v>786</v>
@@ -11809,7 +11808,7 @@
         <v>784</v>
       </c>
       <c r="D186" s="8" t="s">
-        <v>1138</v>
+        <v>1133</v>
       </c>
       <c r="E186" s="6" t="s">
         <v>785</v>
@@ -11940,7 +11939,7 @@
         <v>805</v>
       </c>
       <c r="D190" s="8" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="E190" s="8" t="s">
         <v>806</v>
@@ -11972,7 +11971,7 @@
         <v>805</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>1139</v>
+        <v>1134</v>
       </c>
       <c r="E191" s="8" t="s">
         <v>809</v>
@@ -12004,7 +12003,7 @@
         <v>805</v>
       </c>
       <c r="D192" s="8" t="s">
-        <v>1140</v>
+        <v>1135</v>
       </c>
       <c r="E192" s="8" t="s">
         <v>814</v>
@@ -12036,7 +12035,7 @@
         <v>805</v>
       </c>
       <c r="D193" s="8" t="s">
-        <v>1141</v>
+        <v>1136</v>
       </c>
       <c r="E193" s="8" t="s">
         <v>826</v>
@@ -12068,7 +12067,7 @@
         <v>805</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>1155</v>
+        <v>1150</v>
       </c>
       <c r="E194" s="8" t="s">
         <v>820</v>
@@ -12103,7 +12102,7 @@
         <v>805</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>1142</v>
+        <v>1137</v>
       </c>
       <c r="E195" s="8" t="s">
         <v>823</v>
@@ -12135,7 +12134,7 @@
         <v>805</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>1143</v>
+        <v>1138</v>
       </c>
       <c r="E196" s="8" t="s">
         <v>830</v>
@@ -12167,7 +12166,7 @@
         <v>805</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>1144</v>
+        <v>1139</v>
       </c>
       <c r="E197" s="8" t="s">
         <v>837</v>
@@ -12199,7 +12198,7 @@
         <v>805</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>1145</v>
+        <v>1140</v>
       </c>
       <c r="E198" s="8" t="s">
         <v>838</v>
@@ -12231,7 +12230,7 @@
         <v>805</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>1146</v>
+        <v>1141</v>
       </c>
       <c r="E199" s="8" t="s">
         <v>842</v>
@@ -12263,7 +12262,7 @@
         <v>805</v>
       </c>
       <c r="D200" s="8" t="s">
-        <v>1156</v>
+        <v>1151</v>
       </c>
       <c r="E200" s="8" t="s">
         <v>846</v>
@@ -12295,7 +12294,7 @@
         <v>805</v>
       </c>
       <c r="D201" s="8" t="s">
-        <v>1157</v>
+        <v>1152</v>
       </c>
       <c r="E201" s="8" t="s">
         <v>850</v>
@@ -12327,7 +12326,7 @@
         <v>805</v>
       </c>
       <c r="D202" s="8" t="s">
-        <v>1147</v>
+        <v>1142</v>
       </c>
       <c r="E202" s="8" t="s">
         <v>855</v>
@@ -12359,7 +12358,7 @@
         <v>805</v>
       </c>
       <c r="D203" s="8" t="s">
-        <v>1144</v>
+        <v>1139</v>
       </c>
       <c r="E203" s="8" t="s">
         <v>862</v>
@@ -12484,7 +12483,7 @@
         <v>874</v>
       </c>
       <c r="D207" s="8" t="s">
-        <v>1148</v>
+        <v>1143</v>
       </c>
       <c r="E207" s="8" t="s">
         <v>879</v>
@@ -12516,7 +12515,7 @@
         <v>875</v>
       </c>
       <c r="D208" s="8" t="s">
-        <v>1149</v>
+        <v>1144</v>
       </c>
       <c r="E208" s="8" t="s">
         <v>876</v>
@@ -12548,7 +12547,7 @@
         <v>885</v>
       </c>
       <c r="D209" s="8" t="s">
-        <v>1150</v>
+        <v>1145</v>
       </c>
       <c r="E209" s="8" t="s">
         <v>886</v>
@@ -12588,17 +12587,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="31.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="37.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
started question bank section.....
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3951" uniqueCount="1213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3952" uniqueCount="1215">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5101,30 +5101,6 @@
     <t>fn_ViewAverageScoreofSelectedSubject</t>
   </si>
   <si>
-    <t>fi_FunctionalityToofLearningresource</t>
-  </si>
-  <si>
-    <t>fi_FunctionalityToRemoveofLearningresource</t>
-  </si>
-  <si>
-    <t>fi_FunctionalityToofLessonplayer</t>
-  </si>
-  <si>
-    <t>fi_ViewofAllquestions</t>
-  </si>
-  <si>
-    <t>fi_ViewofRecommendedquestions</t>
-  </si>
-  <si>
-    <t>fi_ViewofCreatedquestions</t>
-  </si>
-  <si>
-    <t>fi_PreviewofRespectivequestion</t>
-  </si>
-  <si>
-    <t>fi_ValidationForMandatoryFieldsofAssessmentwindow</t>
-  </si>
-  <si>
     <t>fi_CancelofAssessmentwindow</t>
   </si>
   <si>
@@ -5195,9 +5171,6 @@
   </si>
   <si>
     <t>fn_DisplayPracticeTestDetails</t>
-  </si>
-  <si>
-    <t>fi_FunctionalityOfAssessmentGenerationCorrespondingToTheQuestions</t>
   </si>
   <si>
     <t>f-_TeacherIsNotAllowedToRemoveTheTestAfterSubmissionFromTheStudent</t>
@@ -5414,6 +5387,39 @@
   </si>
   <si>
     <t>fn_SavePlayedresource</t>
+  </si>
+  <si>
+    <t>fn_BookmarkLearningresource</t>
+  </si>
+  <si>
+    <t>fn_RemoveLearningresource</t>
+  </si>
+  <si>
+    <t>fn_AddLessontoLessonplayer</t>
+  </si>
+  <si>
+    <t>fn_ViewAllquestions</t>
+  </si>
+  <si>
+    <t>fn_ViewRecommendedquestions</t>
+  </si>
+  <si>
+    <t>fn_ViewMyquestions</t>
+  </si>
+  <si>
+    <t>fn_PreviewRespectivequestion</t>
+  </si>
+  <si>
+    <t>fn_AssessmentGeneration</t>
+  </si>
+  <si>
+    <t>fn_ValidationForMandatoryFieldsonAssessmentwindow</t>
+  </si>
+  <si>
+    <t>fn_CancelAssessmentwindow</t>
+  </si>
+  <si>
+    <t>fn_RandomAssessmentGeneration</t>
   </si>
 </sst>
 </file>
@@ -5891,8 +5897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="A135" sqref="A135"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="D146" sqref="D146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8538,7 +8544,7 @@
         <v>347</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>1146</v>
+        <v>1138</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>355</v>
@@ -8570,7 +8576,7 @@
         <v>347</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>1153</v>
+        <v>1144</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>360</v>
@@ -8602,7 +8608,7 @@
         <v>347</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>1154</v>
+        <v>1145</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>364</v>
@@ -8634,7 +8640,7 @@
         <v>368</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>1155</v>
+        <v>1146</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>370</v>
@@ -8666,7 +8672,7 @@
         <v>368</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>1156</v>
+        <v>1147</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>374</v>
@@ -8696,7 +8702,7 @@
         <v>377</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>1157</v>
+        <v>1148</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>382</v>
@@ -8725,7 +8731,7 @@
         <v>381</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>1158</v>
+        <v>1149</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>384</v>
@@ -8757,7 +8763,7 @@
         <v>381</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>1159</v>
+        <v>1150</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>386</v>
@@ -8789,7 +8795,7 @@
         <v>381</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>1160</v>
+        <v>1151</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>390</v>
@@ -8821,7 +8827,7 @@
         <v>381</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>1161</v>
+        <v>1152</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>394</v>
@@ -8853,7 +8859,7 @@
         <v>381</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>1162</v>
+        <v>1153</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>398</v>
@@ -8885,7 +8891,7 @@
         <v>381</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>1163</v>
+        <v>1154</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>403</v>
@@ -8917,7 +8923,7 @@
         <v>381</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>1164</v>
+        <v>1155</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>407</v>
@@ -8949,7 +8955,7 @@
         <v>414</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>1165</v>
+        <v>1156</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>412</v>
@@ -8981,7 +8987,7 @@
         <v>414</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>1166</v>
+        <v>1157</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>416</v>
@@ -9013,7 +9019,7 @@
         <v>425</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>1167</v>
+        <v>1158</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>424</v>
@@ -9045,7 +9051,7 @@
         <v>422</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>1168</v>
+        <v>1159</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>427</v>
@@ -9077,7 +9083,7 @@
         <v>422</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>1169</v>
+        <v>1160</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>429</v>
@@ -9098,7 +9104,7 @@
         <v>1012</v>
       </c>
       <c r="L101" s="8" t="s">
-        <v>1170</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="195" x14ac:dyDescent="0.25">
@@ -9112,7 +9118,7 @@
         <v>422</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>1171</v>
+        <v>1162</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>436</v>
@@ -9144,7 +9150,7 @@
         <v>422</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>1172</v>
+        <v>1163</v>
       </c>
       <c r="E103" s="8" t="s">
         <v>438</v>
@@ -9173,7 +9179,7 @@
         <v>442</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>1173</v>
+        <v>1164</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>443</v>
@@ -9205,7 +9211,7 @@
         <v>442</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>1174</v>
+        <v>1165</v>
       </c>
       <c r="E105" s="8" t="s">
         <v>446</v>
@@ -9237,7 +9243,7 @@
         <v>442</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>1175</v>
+        <v>1166</v>
       </c>
       <c r="E106" s="8" t="s">
         <v>451</v>
@@ -9269,7 +9275,7 @@
         <v>442</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>1176</v>
+        <v>1167</v>
       </c>
       <c r="E107" s="8" t="s">
         <v>455</v>
@@ -9298,7 +9304,7 @@
         <v>458</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>1177</v>
+        <v>1168</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>460</v>
@@ -9327,7 +9333,7 @@
         <v>458</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>1178</v>
+        <v>1169</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>620</v>
@@ -9356,7 +9362,7 @@
         <v>458</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>1179</v>
+        <v>1170</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>621</v>
@@ -9385,7 +9391,7 @@
         <v>464</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>1180</v>
+        <v>1171</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>465</v>
@@ -9411,10 +9417,10 @@
         <v>411</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>1183</v>
+        <v>1174</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>1182</v>
+        <v>1173</v>
       </c>
       <c r="E112" s="8"/>
       <c r="G112" s="2"/>
@@ -9434,7 +9440,7 @@
         <v>468</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>1181</v>
+        <v>1172</v>
       </c>
       <c r="E113" s="8" t="s">
         <v>471</v>
@@ -9463,7 +9469,7 @@
         <v>472</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>1184</v>
+        <v>1175</v>
       </c>
       <c r="E114" s="8" t="s">
         <v>474</v>
@@ -9492,7 +9498,7 @@
         <v>481</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>1185</v>
+        <v>1176</v>
       </c>
       <c r="E115" s="8" t="s">
         <v>424</v>
@@ -9524,7 +9530,7 @@
         <v>477</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>1186</v>
+        <v>1177</v>
       </c>
       <c r="E116" s="8" t="s">
         <v>478</v>
@@ -9556,7 +9562,7 @@
         <v>486</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>1187</v>
+        <v>1178</v>
       </c>
       <c r="E117" s="8" t="s">
         <v>487</v>
@@ -9588,7 +9594,7 @@
         <v>490</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>1188</v>
+        <v>1179</v>
       </c>
       <c r="E118" s="8" t="s">
         <v>491</v>
@@ -9620,7 +9626,7 @@
         <v>490</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>1189</v>
+        <v>1180</v>
       </c>
       <c r="E119" s="8" t="s">
         <v>495</v>
@@ -9652,7 +9658,7 @@
         <v>498</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>1190</v>
+        <v>1181</v>
       </c>
       <c r="E120" s="8" t="s">
         <v>500</v>
@@ -9687,7 +9693,7 @@
         <v>498</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>1191</v>
+        <v>1182</v>
       </c>
       <c r="E121" s="8" t="s">
         <v>505</v>
@@ -9719,7 +9725,7 @@
         <v>498</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>1192</v>
+        <v>1183</v>
       </c>
       <c r="E122" s="8" t="s">
         <v>508</v>
@@ -9755,7 +9761,7 @@
         <v>498</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>1193</v>
+        <v>1184</v>
       </c>
       <c r="E123" s="8" t="s">
         <v>513</v>
@@ -9788,7 +9794,7 @@
         <v>498</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>1194</v>
+        <v>1185</v>
       </c>
       <c r="E124" s="8" t="s">
         <v>521</v>
@@ -9807,7 +9813,7 @@
         <v>1012</v>
       </c>
       <c r="L124" s="20" t="s">
-        <v>1195</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="125" spans="1:12" ht="315" x14ac:dyDescent="0.25">
@@ -9818,22 +9824,22 @@
         <v>411</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>1197</v>
+        <v>1188</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>1198</v>
+        <v>1189</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>1199</v>
+        <v>1190</v>
       </c>
       <c r="F125" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>1204</v>
+        <v>1195</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>1200</v>
+        <v>1191</v>
       </c>
       <c r="I125" s="2" t="s">
         <v>502</v>
@@ -9856,7 +9862,7 @@
         <v>498</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>1201</v>
+        <v>1192</v>
       </c>
       <c r="E126" s="8" t="s">
         <v>505</v>
@@ -9888,7 +9894,7 @@
         <v>498</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>1202</v>
+        <v>1193</v>
       </c>
       <c r="E127" s="8" t="s">
         <v>508</v>
@@ -9897,7 +9903,7 @@
         <v>38</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>1203</v>
+        <v>1194</v>
       </c>
       <c r="H127" s="2"/>
       <c r="I127" s="2" t="s">
@@ -9924,7 +9930,7 @@
         <v>498</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>1205</v>
+        <v>1196</v>
       </c>
       <c r="E128" s="8" t="s">
         <v>513</v>
@@ -9957,7 +9963,7 @@
         <v>498</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>1207</v>
+        <v>1198</v>
       </c>
       <c r="E129" s="8" t="s">
         <v>521</v>
@@ -9976,7 +9982,7 @@
         <v>911</v>
       </c>
       <c r="L129" s="20" t="s">
-        <v>1195</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="130" spans="1:12" ht="375" x14ac:dyDescent="0.25">
@@ -9990,7 +9996,7 @@
         <v>540</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>1196</v>
+        <v>1187</v>
       </c>
       <c r="E130" s="8" t="s">
         <v>543</v>
@@ -10022,7 +10028,7 @@
         <v>540</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>1208</v>
+        <v>1199</v>
       </c>
       <c r="E131" s="8" t="s">
         <v>548</v>
@@ -10055,7 +10061,7 @@
         <v>552</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>1209</v>
+        <v>1200</v>
       </c>
       <c r="E132" s="8" t="s">
         <v>553</v>
@@ -10076,7 +10082,7 @@
         <v>1012</v>
       </c>
       <c r="L132" s="20" t="s">
-        <v>1206</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="133" spans="1:12" ht="165" x14ac:dyDescent="0.25">
@@ -10090,7 +10096,7 @@
         <v>552</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>1210</v>
+        <v>1201</v>
       </c>
       <c r="E133" s="8" t="s">
         <v>557</v>
@@ -10122,7 +10128,7 @@
         <v>561</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>1211</v>
+        <v>1202</v>
       </c>
       <c r="E134" s="8" t="s">
         <v>562</v>
@@ -10154,7 +10160,7 @@
         <v>561</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>1212</v>
+        <v>1203</v>
       </c>
       <c r="E135" s="8" t="s">
         <v>565</v>
@@ -10186,7 +10192,7 @@
         <v>561</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>1115</v>
+        <v>1204</v>
       </c>
       <c r="E136" s="8" t="s">
         <v>568</v>
@@ -10218,7 +10224,7 @@
         <v>561</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>1116</v>
+        <v>1205</v>
       </c>
       <c r="E137" s="8" t="s">
         <v>572</v>
@@ -10250,7 +10256,7 @@
         <v>561</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>1117</v>
+        <v>1206</v>
       </c>
       <c r="E138" s="8" t="s">
         <v>576</v>
@@ -10282,7 +10288,7 @@
         <v>581</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>1118</v>
+        <v>1207</v>
       </c>
       <c r="E139" s="6" t="s">
         <v>582</v>
@@ -10314,7 +10320,7 @@
         <v>581</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>1119</v>
+        <v>1208</v>
       </c>
       <c r="E140" s="8" t="s">
         <v>625</v>
@@ -10346,7 +10352,7 @@
         <v>581</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>1120</v>
+        <v>1209</v>
       </c>
       <c r="E141" s="8" t="s">
         <v>628</v>
@@ -10378,7 +10384,7 @@
         <v>581</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>1121</v>
+        <v>1210</v>
       </c>
       <c r="E142" s="8" t="s">
         <v>586</v>
@@ -10410,7 +10416,7 @@
         <v>594</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>1147</v>
+        <v>1211</v>
       </c>
       <c r="E143" s="8" t="s">
         <v>593</v>
@@ -10445,7 +10451,7 @@
         <v>595</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>1122</v>
+        <v>1212</v>
       </c>
       <c r="E144" s="8" t="s">
         <v>596</v>
@@ -10477,7 +10483,7 @@
         <v>595</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>1123</v>
+        <v>1213</v>
       </c>
       <c r="E145" s="8" t="s">
         <v>600</v>
@@ -10508,6 +10514,9 @@
       <c r="C146" s="8" t="s">
         <v>595</v>
       </c>
+      <c r="D146" s="8" t="s">
+        <v>1214</v>
+      </c>
       <c r="E146" s="8" t="s">
         <v>604</v>
       </c>
@@ -10573,7 +10582,7 @@
         <v>595</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>1123</v>
+        <v>1115</v>
       </c>
       <c r="E148" s="8" t="s">
         <v>612</v>
@@ -10872,7 +10881,7 @@
         <v>665</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>1124</v>
+        <v>1116</v>
       </c>
       <c r="E158" s="8" t="s">
         <v>694</v>
@@ -11097,7 +11106,7 @@
         <v>699</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>1148</v>
+        <v>1139</v>
       </c>
       <c r="E165" s="8" t="s">
         <v>700</v>
@@ -11126,7 +11135,7 @@
         <v>699</v>
       </c>
       <c r="D166" s="8" t="s">
-        <v>1125</v>
+        <v>1117</v>
       </c>
       <c r="E166" s="8" t="s">
         <v>704</v>
@@ -11251,7 +11260,7 @@
         <v>713</v>
       </c>
       <c r="D170" s="8" t="s">
-        <v>1126</v>
+        <v>1118</v>
       </c>
       <c r="E170" s="8" t="s">
         <v>718</v>
@@ -11283,7 +11292,7 @@
         <v>713</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>1127</v>
+        <v>1119</v>
       </c>
       <c r="E171" s="8" t="s">
         <v>722</v>
@@ -11315,7 +11324,7 @@
         <v>713</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>1128</v>
+        <v>1120</v>
       </c>
       <c r="E172" s="8" t="s">
         <v>726</v>
@@ -11347,7 +11356,7 @@
         <v>713</v>
       </c>
       <c r="D173" s="8" t="s">
-        <v>1129</v>
+        <v>1121</v>
       </c>
       <c r="E173" s="10" t="s">
         <v>731</v>
@@ -11396,7 +11405,7 @@
         <v>735</v>
       </c>
       <c r="D174" s="8" t="s">
-        <v>1130</v>
+        <v>1122</v>
       </c>
       <c r="E174" s="14" t="s">
         <v>748</v>
@@ -11474,7 +11483,7 @@
         <v>736</v>
       </c>
       <c r="D176" s="8" t="s">
-        <v>1149</v>
+        <v>1140</v>
       </c>
       <c r="E176" s="8" t="s">
         <v>741</v>
@@ -11614,7 +11623,7 @@
         <v>753</v>
       </c>
       <c r="D180" s="8" t="s">
-        <v>1131</v>
+        <v>1123</v>
       </c>
       <c r="E180" s="8" t="s">
         <v>764</v>
@@ -11744,7 +11753,7 @@
         <v>753</v>
       </c>
       <c r="D184" s="8" t="s">
-        <v>1132</v>
+        <v>1124</v>
       </c>
       <c r="E184" s="8" t="s">
         <v>776</v>
@@ -11808,7 +11817,7 @@
         <v>784</v>
       </c>
       <c r="D186" s="8" t="s">
-        <v>1133</v>
+        <v>1125</v>
       </c>
       <c r="E186" s="6" t="s">
         <v>785</v>
@@ -11971,7 +11980,7 @@
         <v>805</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>1134</v>
+        <v>1126</v>
       </c>
       <c r="E191" s="8" t="s">
         <v>809</v>
@@ -12003,7 +12012,7 @@
         <v>805</v>
       </c>
       <c r="D192" s="8" t="s">
-        <v>1135</v>
+        <v>1127</v>
       </c>
       <c r="E192" s="8" t="s">
         <v>814</v>
@@ -12035,7 +12044,7 @@
         <v>805</v>
       </c>
       <c r="D193" s="8" t="s">
-        <v>1136</v>
+        <v>1128</v>
       </c>
       <c r="E193" s="8" t="s">
         <v>826</v>
@@ -12067,7 +12076,7 @@
         <v>805</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>1150</v>
+        <v>1141</v>
       </c>
       <c r="E194" s="8" t="s">
         <v>820</v>
@@ -12102,7 +12111,7 @@
         <v>805</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>1137</v>
+        <v>1129</v>
       </c>
       <c r="E195" s="8" t="s">
         <v>823</v>
@@ -12134,7 +12143,7 @@
         <v>805</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>1138</v>
+        <v>1130</v>
       </c>
       <c r="E196" s="8" t="s">
         <v>830</v>
@@ -12166,7 +12175,7 @@
         <v>805</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>1139</v>
+        <v>1131</v>
       </c>
       <c r="E197" s="8" t="s">
         <v>837</v>
@@ -12198,7 +12207,7 @@
         <v>805</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>1140</v>
+        <v>1132</v>
       </c>
       <c r="E198" s="8" t="s">
         <v>838</v>
@@ -12230,7 +12239,7 @@
         <v>805</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>1141</v>
+        <v>1133</v>
       </c>
       <c r="E199" s="8" t="s">
         <v>842</v>
@@ -12262,7 +12271,7 @@
         <v>805</v>
       </c>
       <c r="D200" s="8" t="s">
-        <v>1151</v>
+        <v>1142</v>
       </c>
       <c r="E200" s="8" t="s">
         <v>846</v>
@@ -12294,7 +12303,7 @@
         <v>805</v>
       </c>
       <c r="D201" s="8" t="s">
-        <v>1152</v>
+        <v>1143</v>
       </c>
       <c r="E201" s="8" t="s">
         <v>850</v>
@@ -12326,7 +12335,7 @@
         <v>805</v>
       </c>
       <c r="D202" s="8" t="s">
-        <v>1142</v>
+        <v>1134</v>
       </c>
       <c r="E202" s="8" t="s">
         <v>855</v>
@@ -12358,7 +12367,7 @@
         <v>805</v>
       </c>
       <c r="D203" s="8" t="s">
-        <v>1139</v>
+        <v>1131</v>
       </c>
       <c r="E203" s="8" t="s">
         <v>862</v>
@@ -12483,7 +12492,7 @@
         <v>874</v>
       </c>
       <c r="D207" s="8" t="s">
-        <v>1143</v>
+        <v>1135</v>
       </c>
       <c r="E207" s="8" t="s">
         <v>879</v>
@@ -12515,7 +12524,7 @@
         <v>875</v>
       </c>
       <c r="D208" s="8" t="s">
-        <v>1144</v>
+        <v>1136</v>
       </c>
       <c r="E208" s="8" t="s">
         <v>876</v>
@@ -12547,7 +12556,7 @@
         <v>885</v>
       </c>
       <c r="D209" s="8" t="s">
-        <v>1145</v>
+        <v>1137</v>
       </c>
       <c r="E209" s="8" t="s">
         <v>886</v>

</xml_diff>

<commit_message>
create test section is done...
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3952" uniqueCount="1215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3961" uniqueCount="1227">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5065,30 +5065,6 @@
     <t>fA_AddRemarkforstudent'sFeedbackofView</t>
   </si>
   <si>
-    <t>fi_ValidationsForMandatoryFieldsOnSaveAssessmentWindowofAssessmentGeneration</t>
-  </si>
-  <si>
-    <t>f-_FunctionalityofEditsection</t>
-  </si>
-  <si>
-    <t>f-_FunctionalityofDeletesection</t>
-  </si>
-  <si>
-    <t>f-_FunctionalityToSearchSpecificQuestionWithAdvancedofQuestionBank</t>
-  </si>
-  <si>
-    <t>f-_FunctionalityToSearchSpecificQuestionFromLeftofQuestionBank</t>
-  </si>
-  <si>
-    <t>f-_FunctionalityToTryoutAofQuestionBank</t>
-  </si>
-  <si>
-    <t>f-_FunctionalityToDeleteTestofNobutton</t>
-  </si>
-  <si>
-    <t>f-_TeacherIsNotAbleofRecommendedtests</t>
-  </si>
-  <si>
     <t>fv_ValidationToofTimefields</t>
   </si>
   <si>
@@ -5101,15 +5077,6 @@
     <t>fn_ViewAverageScoreofSelectedSubject</t>
   </si>
   <si>
-    <t>fi_CancelofAssessmentwindow</t>
-  </si>
-  <si>
-    <t>f-_ForofMandatoryfield</t>
-  </si>
-  <si>
-    <t>f-_FunctionalityofDeletetest</t>
-  </si>
-  <si>
     <t>f-_FunctionalityToAssignofAGroup</t>
   </si>
   <si>
@@ -5171,9 +5138,6 @@
   </si>
   <si>
     <t>fn_DisplayPracticeTestDetails</t>
-  </si>
-  <si>
-    <t>f-_TeacherIsNotAllowedToRemoveTheTestAfterSubmissionFromTheStudent</t>
   </si>
   <si>
     <t>fL_ViewLessonsPlannedForTheWeek</t>
@@ -5420,6 +5384,82 @@
   </si>
   <si>
     <t>fn_RandomAssessmentGeneration</t>
+  </si>
+  <si>
+    <t>fn_ValidationsForMandatoryFieldsOnRandomAssessmentGeneration</t>
+  </si>
+  <si>
+    <t>fn_CancelRandomAssessmentwindow</t>
+  </si>
+  <si>
+    <t>fn_ViewAllTests</t>
+  </si>
+  <si>
+    <t>fn_ViewAllRecommendedTests</t>
+  </si>
+  <si>
+    <t>fn_ViewAllMyTests</t>
+  </si>
+  <si>
+    <t>fn_SearchTest</t>
+  </si>
+  <si>
+    <t>1. No.of submissions block getting disappeared after selecting type
+2.Enhancement: Generate button shows dropdown sign, it need to remove</t>
+  </si>
+  <si>
+    <t>fn_SearchInvalidTest</t>
+  </si>
+  <si>
+    <t>fn_PreviewTest</t>
+  </si>
+  <si>
+    <t>fn_PrintTest</t>
+  </si>
+  <si>
+    <t>fn_PrintAnswerBooklet</t>
+  </si>
+  <si>
+    <t>fn_CreateTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. after adding questions to a section , other added section does not show Add question icon
+2. While adding questions on Question Bank page, select no. of questions by checkbox and click Add to Section now it should redirect to section page, but here it let user to click again on add to section button and it doubles no of questions and showing wrong no of questions selected
+3. After added questions for default section third section gets disappeared
+4. After adding a question in any section if add question in other section then last added question checkbox is disabled with checked status and counted </t>
+  </si>
+  <si>
+    <t>fn_ValidationforMandatoryfieldinCreateTest</t>
+  </si>
+  <si>
+    <t>fn_AddMoreSections</t>
+  </si>
+  <si>
+    <t>fn_EditSection</t>
+  </si>
+  <si>
+    <t>fn_DeleteSection</t>
+  </si>
+  <si>
+    <t>fn_SearchSpecificQuestionWithAdvancedofQuestionBank</t>
+  </si>
+  <si>
+    <t>fn_SearchSpecificQuestionFromLeftofQuestionBank</t>
+  </si>
+  <si>
+    <t>fn_TryoutAQuestionBank</t>
+  </si>
+  <si>
+    <t>fn_RemoveSubmittedTest</t>
+  </si>
+  <si>
+    <t>fn_DeleteTest</t>
+  </si>
+  <si>
+    <t>fn_DeleteTestbyNobutton</t>
+  </si>
+  <si>
+    <t>fn_DeleteRecommendedTests</t>
   </si>
 </sst>
 </file>
@@ -5897,8 +5937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="D146" sqref="D146"/>
+    <sheetView tabSelected="1" topLeftCell="C168" workbookViewId="0">
+      <selection activeCell="D168" sqref="D168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8512,7 +8552,7 @@
         <v>347</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>1114</v>
+        <v>1106</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>352</v>
@@ -8544,7 +8584,7 @@
         <v>347</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>1138</v>
+        <v>1127</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>355</v>
@@ -8576,7 +8616,7 @@
         <v>347</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>1144</v>
+        <v>1132</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>360</v>
@@ -8608,7 +8648,7 @@
         <v>347</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>1145</v>
+        <v>1133</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>364</v>
@@ -8640,7 +8680,7 @@
         <v>368</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>1146</v>
+        <v>1134</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>370</v>
@@ -8672,7 +8712,7 @@
         <v>368</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>1147</v>
+        <v>1135</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>374</v>
@@ -8702,7 +8742,7 @@
         <v>377</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>1148</v>
+        <v>1136</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>382</v>
@@ -8731,7 +8771,7 @@
         <v>381</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>1149</v>
+        <v>1137</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>384</v>
@@ -8763,7 +8803,7 @@
         <v>381</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>1150</v>
+        <v>1138</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>386</v>
@@ -8795,7 +8835,7 @@
         <v>381</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>1151</v>
+        <v>1139</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>390</v>
@@ -8827,7 +8867,7 @@
         <v>381</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>1152</v>
+        <v>1140</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>394</v>
@@ -8859,7 +8899,7 @@
         <v>381</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>1153</v>
+        <v>1141</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>398</v>
@@ -8891,7 +8931,7 @@
         <v>381</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>1154</v>
+        <v>1142</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>403</v>
@@ -8923,7 +8963,7 @@
         <v>381</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>1155</v>
+        <v>1143</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>407</v>
@@ -8955,7 +8995,7 @@
         <v>414</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>1156</v>
+        <v>1144</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>412</v>
@@ -8987,7 +9027,7 @@
         <v>414</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>1157</v>
+        <v>1145</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>416</v>
@@ -9019,7 +9059,7 @@
         <v>425</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>1158</v>
+        <v>1146</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>424</v>
@@ -9051,7 +9091,7 @@
         <v>422</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>1159</v>
+        <v>1147</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>427</v>
@@ -9083,7 +9123,7 @@
         <v>422</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>1160</v>
+        <v>1148</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>429</v>
@@ -9104,7 +9144,7 @@
         <v>1012</v>
       </c>
       <c r="L101" s="8" t="s">
-        <v>1161</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="195" x14ac:dyDescent="0.25">
@@ -9118,7 +9158,7 @@
         <v>422</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>1162</v>
+        <v>1150</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>436</v>
@@ -9150,7 +9190,7 @@
         <v>422</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>1163</v>
+        <v>1151</v>
       </c>
       <c r="E103" s="8" t="s">
         <v>438</v>
@@ -9179,7 +9219,7 @@
         <v>442</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>1164</v>
+        <v>1152</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>443</v>
@@ -9211,7 +9251,7 @@
         <v>442</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>1165</v>
+        <v>1153</v>
       </c>
       <c r="E105" s="8" t="s">
         <v>446</v>
@@ -9243,7 +9283,7 @@
         <v>442</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>1166</v>
+        <v>1154</v>
       </c>
       <c r="E106" s="8" t="s">
         <v>451</v>
@@ -9275,7 +9315,7 @@
         <v>442</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>1167</v>
+        <v>1155</v>
       </c>
       <c r="E107" s="8" t="s">
         <v>455</v>
@@ -9304,7 +9344,7 @@
         <v>458</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>1168</v>
+        <v>1156</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>460</v>
@@ -9333,7 +9373,7 @@
         <v>458</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>1169</v>
+        <v>1157</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>620</v>
@@ -9362,7 +9402,7 @@
         <v>458</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>1170</v>
+        <v>1158</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>621</v>
@@ -9391,7 +9431,7 @@
         <v>464</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>1171</v>
+        <v>1159</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>465</v>
@@ -9417,10 +9457,10 @@
         <v>411</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>1174</v>
+        <v>1162</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>1173</v>
+        <v>1161</v>
       </c>
       <c r="E112" s="8"/>
       <c r="G112" s="2"/>
@@ -9440,7 +9480,7 @@
         <v>468</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>1172</v>
+        <v>1160</v>
       </c>
       <c r="E113" s="8" t="s">
         <v>471</v>
@@ -9469,7 +9509,7 @@
         <v>472</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>1175</v>
+        <v>1163</v>
       </c>
       <c r="E114" s="8" t="s">
         <v>474</v>
@@ -9498,7 +9538,7 @@
         <v>481</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>1176</v>
+        <v>1164</v>
       </c>
       <c r="E115" s="8" t="s">
         <v>424</v>
@@ -9530,7 +9570,7 @@
         <v>477</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>1177</v>
+        <v>1165</v>
       </c>
       <c r="E116" s="8" t="s">
         <v>478</v>
@@ -9562,7 +9602,7 @@
         <v>486</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>1178</v>
+        <v>1166</v>
       </c>
       <c r="E117" s="8" t="s">
         <v>487</v>
@@ -9594,7 +9634,7 @@
         <v>490</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>1179</v>
+        <v>1167</v>
       </c>
       <c r="E118" s="8" t="s">
         <v>491</v>
@@ -9626,7 +9666,7 @@
         <v>490</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>1180</v>
+        <v>1168</v>
       </c>
       <c r="E119" s="8" t="s">
         <v>495</v>
@@ -9658,7 +9698,7 @@
         <v>498</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>1181</v>
+        <v>1169</v>
       </c>
       <c r="E120" s="8" t="s">
         <v>500</v>
@@ -9693,7 +9733,7 @@
         <v>498</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>1182</v>
+        <v>1170</v>
       </c>
       <c r="E121" s="8" t="s">
         <v>505</v>
@@ -9725,7 +9765,7 @@
         <v>498</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>1183</v>
+        <v>1171</v>
       </c>
       <c r="E122" s="8" t="s">
         <v>508</v>
@@ -9761,7 +9801,7 @@
         <v>498</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>1184</v>
+        <v>1172</v>
       </c>
       <c r="E123" s="8" t="s">
         <v>513</v>
@@ -9794,7 +9834,7 @@
         <v>498</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>1185</v>
+        <v>1173</v>
       </c>
       <c r="E124" s="8" t="s">
         <v>521</v>
@@ -9813,7 +9853,7 @@
         <v>1012</v>
       </c>
       <c r="L124" s="20" t="s">
-        <v>1186</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="125" spans="1:12" ht="315" x14ac:dyDescent="0.25">
@@ -9824,22 +9864,22 @@
         <v>411</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>1188</v>
+        <v>1176</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>1189</v>
+        <v>1177</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>1190</v>
+        <v>1178</v>
       </c>
       <c r="F125" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>1195</v>
+        <v>1183</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>1191</v>
+        <v>1179</v>
       </c>
       <c r="I125" s="2" t="s">
         <v>502</v>
@@ -9862,7 +9902,7 @@
         <v>498</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>1192</v>
+        <v>1180</v>
       </c>
       <c r="E126" s="8" t="s">
         <v>505</v>
@@ -9894,7 +9934,7 @@
         <v>498</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>1193</v>
+        <v>1181</v>
       </c>
       <c r="E127" s="8" t="s">
         <v>508</v>
@@ -9903,7 +9943,7 @@
         <v>38</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>1194</v>
+        <v>1182</v>
       </c>
       <c r="H127" s="2"/>
       <c r="I127" s="2" t="s">
@@ -9930,7 +9970,7 @@
         <v>498</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>1196</v>
+        <v>1184</v>
       </c>
       <c r="E128" s="8" t="s">
         <v>513</v>
@@ -9963,7 +10003,7 @@
         <v>498</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>1198</v>
+        <v>1186</v>
       </c>
       <c r="E129" s="8" t="s">
         <v>521</v>
@@ -9982,7 +10022,7 @@
         <v>911</v>
       </c>
       <c r="L129" s="20" t="s">
-        <v>1186</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="130" spans="1:12" ht="375" x14ac:dyDescent="0.25">
@@ -9996,7 +10036,7 @@
         <v>540</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>1187</v>
+        <v>1175</v>
       </c>
       <c r="E130" s="8" t="s">
         <v>543</v>
@@ -10028,7 +10068,7 @@
         <v>540</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>1199</v>
+        <v>1187</v>
       </c>
       <c r="E131" s="8" t="s">
         <v>548</v>
@@ -10061,7 +10101,7 @@
         <v>552</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>1200</v>
+        <v>1188</v>
       </c>
       <c r="E132" s="8" t="s">
         <v>553</v>
@@ -10082,7 +10122,7 @@
         <v>1012</v>
       </c>
       <c r="L132" s="20" t="s">
-        <v>1197</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="133" spans="1:12" ht="165" x14ac:dyDescent="0.25">
@@ -10096,7 +10136,7 @@
         <v>552</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>1201</v>
+        <v>1189</v>
       </c>
       <c r="E133" s="8" t="s">
         <v>557</v>
@@ -10128,7 +10168,7 @@
         <v>561</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>1202</v>
+        <v>1190</v>
       </c>
       <c r="E134" s="8" t="s">
         <v>562</v>
@@ -10160,7 +10200,7 @@
         <v>561</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>1203</v>
+        <v>1191</v>
       </c>
       <c r="E135" s="8" t="s">
         <v>565</v>
@@ -10192,7 +10232,7 @@
         <v>561</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>1204</v>
+        <v>1192</v>
       </c>
       <c r="E136" s="8" t="s">
         <v>568</v>
@@ -10209,8 +10249,8 @@
       <c r="J136" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K136" s="8" t="s">
-        <v>911</v>
+      <c r="K136" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="137" spans="1:12" ht="225" x14ac:dyDescent="0.25">
@@ -10224,7 +10264,7 @@
         <v>561</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>1205</v>
+        <v>1193</v>
       </c>
       <c r="E137" s="8" t="s">
         <v>572</v>
@@ -10241,8 +10281,8 @@
       <c r="J137" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K137" s="8" t="s">
-        <v>911</v>
+      <c r="K137" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="138" spans="1:12" ht="225" x14ac:dyDescent="0.25">
@@ -10256,7 +10296,7 @@
         <v>561</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>1206</v>
+        <v>1194</v>
       </c>
       <c r="E138" s="8" t="s">
         <v>576</v>
@@ -10273,8 +10313,8 @@
       <c r="J138" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K138" s="8" t="s">
-        <v>911</v>
+      <c r="K138" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="139" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -10288,7 +10328,7 @@
         <v>581</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>1207</v>
+        <v>1195</v>
       </c>
       <c r="E139" s="6" t="s">
         <v>582</v>
@@ -10305,8 +10345,8 @@
       <c r="J139" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K139" s="8" t="s">
-        <v>911</v>
+      <c r="K139" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="140" spans="1:12" ht="150" x14ac:dyDescent="0.25">
@@ -10320,7 +10360,7 @@
         <v>581</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>1208</v>
+        <v>1196</v>
       </c>
       <c r="E140" s="8" t="s">
         <v>625</v>
@@ -10337,8 +10377,8 @@
       <c r="J140" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K140" s="8" t="s">
-        <v>911</v>
+      <c r="K140" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="141" spans="1:12" ht="150" x14ac:dyDescent="0.25">
@@ -10352,7 +10392,7 @@
         <v>581</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>1209</v>
+        <v>1197</v>
       </c>
       <c r="E141" s="8" t="s">
         <v>628</v>
@@ -10369,8 +10409,8 @@
       <c r="J141" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K141" s="8" t="s">
-        <v>911</v>
+      <c r="K141" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="142" spans="1:12" ht="150" x14ac:dyDescent="0.25">
@@ -10384,7 +10424,7 @@
         <v>581</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>1210</v>
+        <v>1198</v>
       </c>
       <c r="E142" s="8" t="s">
         <v>586</v>
@@ -10401,8 +10441,8 @@
       <c r="J142" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K142" s="8" t="s">
-        <v>911</v>
+      <c r="K142" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="143" spans="1:12" ht="195" x14ac:dyDescent="0.25">
@@ -10416,7 +10456,7 @@
         <v>594</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>1211</v>
+        <v>1199</v>
       </c>
       <c r="E143" s="8" t="s">
         <v>593</v>
@@ -10433,11 +10473,11 @@
       <c r="J143" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K143" s="8" t="s">
-        <v>911</v>
-      </c>
-      <c r="L143" s="8" t="s">
-        <v>973</v>
+      <c r="K143" t="s">
+        <v>1012</v>
+      </c>
+      <c r="L143" s="20" t="s">
+        <v>1209</v>
       </c>
     </row>
     <row r="144" spans="1:12" ht="180" x14ac:dyDescent="0.25">
@@ -10451,7 +10491,7 @@
         <v>595</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>1212</v>
+        <v>1200</v>
       </c>
       <c r="E144" s="8" t="s">
         <v>596</v>
@@ -10468,8 +10508,8 @@
       <c r="J144" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K144" s="8" t="s">
-        <v>911</v>
+      <c r="K144" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="145" spans="1:12" ht="165" x14ac:dyDescent="0.25">
@@ -10483,7 +10523,7 @@
         <v>595</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>1213</v>
+        <v>1201</v>
       </c>
       <c r="E145" s="8" t="s">
         <v>600</v>
@@ -10500,8 +10540,8 @@
       <c r="J145" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K145" s="8" t="s">
-        <v>911</v>
+      <c r="K145" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="146" spans="1:12" ht="330" x14ac:dyDescent="0.25">
@@ -10515,7 +10555,7 @@
         <v>595</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>1214</v>
+        <v>1202</v>
       </c>
       <c r="E146" s="8" t="s">
         <v>604</v>
@@ -10532,8 +10572,8 @@
       <c r="J146" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K146" s="8" t="s">
-        <v>911</v>
+      <c r="K146" t="s">
+        <v>1012</v>
       </c>
       <c r="L146" s="8" t="s">
         <v>953</v>
@@ -10550,7 +10590,7 @@
         <v>595</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>1103</v>
+        <v>1203</v>
       </c>
       <c r="E147" s="8" t="s">
         <v>609</v>
@@ -10567,8 +10607,8 @@
       <c r="J147" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K147" s="8" t="s">
-        <v>911</v>
+      <c r="K147" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="148" spans="1:12" ht="165" x14ac:dyDescent="0.25">
@@ -10582,7 +10622,7 @@
         <v>595</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>1115</v>
+        <v>1204</v>
       </c>
       <c r="E148" s="8" t="s">
         <v>612</v>
@@ -10599,8 +10639,8 @@
       <c r="J148" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K148" s="8" t="s">
-        <v>911</v>
+      <c r="K148" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="149" spans="1:12" ht="120" x14ac:dyDescent="0.25">
@@ -10613,6 +10653,9 @@
       <c r="C149" s="6" t="s">
         <v>617</v>
       </c>
+      <c r="D149" s="8" t="s">
+        <v>1205</v>
+      </c>
       <c r="E149" s="6" t="s">
         <v>635</v>
       </c>
@@ -10628,8 +10671,8 @@
       <c r="J149" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K149" s="8" t="s">
-        <v>911</v>
+      <c r="K149" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="150" spans="1:12" ht="150" x14ac:dyDescent="0.25">
@@ -10642,6 +10685,9 @@
       <c r="C150" s="6" t="s">
         <v>617</v>
       </c>
+      <c r="D150" s="8" t="s">
+        <v>1206</v>
+      </c>
       <c r="E150" s="8" t="s">
         <v>638</v>
       </c>
@@ -10657,8 +10703,8 @@
       <c r="J150" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K150" s="8" t="s">
-        <v>911</v>
+      <c r="K150" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="151" spans="1:12" ht="150" x14ac:dyDescent="0.25">
@@ -10671,6 +10717,9 @@
       <c r="C151" s="6" t="s">
         <v>617</v>
       </c>
+      <c r="D151" s="8" t="s">
+        <v>1207</v>
+      </c>
       <c r="E151" s="6" t="s">
         <v>641</v>
       </c>
@@ -10686,8 +10735,8 @@
       <c r="J151" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K151" s="8" t="s">
-        <v>911</v>
+      <c r="K151" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="152" spans="1:12" ht="150" x14ac:dyDescent="0.25">
@@ -10700,6 +10749,9 @@
       <c r="C152" s="6" t="s">
         <v>617</v>
       </c>
+      <c r="D152" s="8" t="s">
+        <v>1208</v>
+      </c>
       <c r="E152" s="8" t="s">
         <v>645</v>
       </c>
@@ -10729,6 +10781,9 @@
       <c r="C153" s="6" t="s">
         <v>617</v>
       </c>
+      <c r="D153" s="8" t="s">
+        <v>1210</v>
+      </c>
       <c r="E153" s="8" t="s">
         <v>649</v>
       </c>
@@ -10744,8 +10799,8 @@
       <c r="J153" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K153" s="8" t="s">
-        <v>911</v>
+      <c r="K153" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="154" spans="1:12" ht="150" x14ac:dyDescent="0.25">
@@ -10758,6 +10813,9 @@
       <c r="C154" s="6" t="s">
         <v>617</v>
       </c>
+      <c r="D154" s="8" t="s">
+        <v>1211</v>
+      </c>
       <c r="E154" s="8" t="s">
         <v>653</v>
       </c>
@@ -10773,8 +10831,8 @@
       <c r="J154" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K154" s="8" t="s">
-        <v>911</v>
+      <c r="K154" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="155" spans="1:12" ht="150" x14ac:dyDescent="0.25">
@@ -10787,6 +10845,9 @@
       <c r="C155" s="6" t="s">
         <v>617</v>
       </c>
+      <c r="D155" s="8" t="s">
+        <v>1212</v>
+      </c>
       <c r="E155" s="8" t="s">
         <v>657</v>
       </c>
@@ -10802,8 +10863,8 @@
       <c r="J155" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K155" s="8" t="s">
-        <v>911</v>
+      <c r="K155" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="156" spans="1:12" ht="150" x14ac:dyDescent="0.25">
@@ -10816,6 +10877,9 @@
       <c r="C156" s="6" t="s">
         <v>617</v>
       </c>
+      <c r="D156" s="8" t="s">
+        <v>1213</v>
+      </c>
       <c r="E156" s="8" t="s">
         <v>661</v>
       </c>
@@ -10831,8 +10895,8 @@
       <c r="J156" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K156" s="8" t="s">
-        <v>911</v>
+      <c r="K156" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="157" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
@@ -10846,7 +10910,7 @@
         <v>665</v>
       </c>
       <c r="D157" s="8" t="s">
-        <v>1000</v>
+        <v>1214</v>
       </c>
       <c r="E157" s="8" t="s">
         <v>666</v>
@@ -10867,7 +10931,7 @@
         <v>909</v>
       </c>
       <c r="L157" s="20" t="s">
-        <v>954</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="158" spans="1:12" ht="195" x14ac:dyDescent="0.25">
@@ -10881,7 +10945,7 @@
         <v>665</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>1116</v>
+        <v>1216</v>
       </c>
       <c r="E158" s="8" t="s">
         <v>694</v>
@@ -10913,6 +10977,9 @@
       <c r="C159" s="6" t="s">
         <v>665</v>
       </c>
+      <c r="D159" s="8" t="s">
+        <v>1217</v>
+      </c>
       <c r="E159" s="8" t="s">
         <v>671</v>
       </c>
@@ -10946,7 +11013,7 @@
         <v>665</v>
       </c>
       <c r="D160" s="8" t="s">
-        <v>1104</v>
+        <v>1218</v>
       </c>
       <c r="E160" s="8" t="s">
         <v>675</v>
@@ -10978,7 +11045,7 @@
         <v>665</v>
       </c>
       <c r="D161" s="8" t="s">
-        <v>1105</v>
+        <v>1219</v>
       </c>
       <c r="E161" s="8" t="s">
         <v>679</v>
@@ -11010,7 +11077,7 @@
         <v>665</v>
       </c>
       <c r="D162" s="8" t="s">
-        <v>1106</v>
+        <v>1220</v>
       </c>
       <c r="E162" s="8" t="s">
         <v>683</v>
@@ -11042,7 +11109,7 @@
         <v>665</v>
       </c>
       <c r="D163" s="8" t="s">
-        <v>1107</v>
+        <v>1221</v>
       </c>
       <c r="E163" s="8" t="s">
         <v>687</v>
@@ -11074,7 +11141,7 @@
         <v>665</v>
       </c>
       <c r="D164" s="8" t="s">
-        <v>1108</v>
+        <v>1222</v>
       </c>
       <c r="E164" s="8" t="s">
         <v>691</v>
@@ -11106,7 +11173,7 @@
         <v>699</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>1139</v>
+        <v>1223</v>
       </c>
       <c r="E165" s="8" t="s">
         <v>700</v>
@@ -11135,7 +11202,7 @@
         <v>699</v>
       </c>
       <c r="D166" s="8" t="s">
-        <v>1117</v>
+        <v>1224</v>
       </c>
       <c r="E166" s="8" t="s">
         <v>704</v>
@@ -11167,7 +11234,7 @@
         <v>699</v>
       </c>
       <c r="D167" s="8" t="s">
-        <v>1109</v>
+        <v>1225</v>
       </c>
       <c r="E167" s="8" t="s">
         <v>707</v>
@@ -11199,7 +11266,7 @@
         <v>699</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>1110</v>
+        <v>1226</v>
       </c>
       <c r="E168" s="8" t="s">
         <v>710</v>
@@ -11260,7 +11327,7 @@
         <v>713</v>
       </c>
       <c r="D170" s="8" t="s">
-        <v>1118</v>
+        <v>1107</v>
       </c>
       <c r="E170" s="8" t="s">
         <v>718</v>
@@ -11292,7 +11359,7 @@
         <v>713</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>1119</v>
+        <v>1108</v>
       </c>
       <c r="E171" s="8" t="s">
         <v>722</v>
@@ -11324,7 +11391,7 @@
         <v>713</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>1120</v>
+        <v>1109</v>
       </c>
       <c r="E172" s="8" t="s">
         <v>726</v>
@@ -11356,7 +11423,7 @@
         <v>713</v>
       </c>
       <c r="D173" s="8" t="s">
-        <v>1121</v>
+        <v>1110</v>
       </c>
       <c r="E173" s="10" t="s">
         <v>731</v>
@@ -11405,7 +11472,7 @@
         <v>735</v>
       </c>
       <c r="D174" s="8" t="s">
-        <v>1122</v>
+        <v>1111</v>
       </c>
       <c r="E174" s="14" t="s">
         <v>748</v>
@@ -11483,7 +11550,7 @@
         <v>736</v>
       </c>
       <c r="D176" s="8" t="s">
-        <v>1140</v>
+        <v>1128</v>
       </c>
       <c r="E176" s="8" t="s">
         <v>741</v>
@@ -11623,7 +11690,7 @@
         <v>753</v>
       </c>
       <c r="D180" s="8" t="s">
-        <v>1123</v>
+        <v>1112</v>
       </c>
       <c r="E180" s="8" t="s">
         <v>764</v>
@@ -11655,7 +11722,7 @@
         <v>753</v>
       </c>
       <c r="D181" s="8" t="s">
-        <v>1111</v>
+        <v>1103</v>
       </c>
       <c r="E181" s="8" t="s">
         <v>768</v>
@@ -11687,7 +11754,7 @@
         <v>753</v>
       </c>
       <c r="D182" s="8" t="s">
-        <v>1111</v>
+        <v>1103</v>
       </c>
       <c r="E182" s="8" t="s">
         <v>768</v>
@@ -11720,7 +11787,7 @@
         <v>753</v>
       </c>
       <c r="D183" s="8" t="s">
-        <v>1111</v>
+        <v>1103</v>
       </c>
       <c r="E183" s="8" t="s">
         <v>768</v>
@@ -11753,7 +11820,7 @@
         <v>753</v>
       </c>
       <c r="D184" s="8" t="s">
-        <v>1124</v>
+        <v>1113</v>
       </c>
       <c r="E184" s="8" t="s">
         <v>776</v>
@@ -11785,7 +11852,7 @@
         <v>779</v>
       </c>
       <c r="D185" s="8" t="s">
-        <v>1112</v>
+        <v>1104</v>
       </c>
       <c r="E185" s="6" t="s">
         <v>786</v>
@@ -11817,7 +11884,7 @@
         <v>784</v>
       </c>
       <c r="D186" s="8" t="s">
-        <v>1125</v>
+        <v>1114</v>
       </c>
       <c r="E186" s="6" t="s">
         <v>785</v>
@@ -11948,7 +12015,7 @@
         <v>805</v>
       </c>
       <c r="D190" s="8" t="s">
-        <v>1113</v>
+        <v>1105</v>
       </c>
       <c r="E190" s="8" t="s">
         <v>806</v>
@@ -11980,7 +12047,7 @@
         <v>805</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>1126</v>
+        <v>1115</v>
       </c>
       <c r="E191" s="8" t="s">
         <v>809</v>
@@ -12012,7 +12079,7 @@
         <v>805</v>
       </c>
       <c r="D192" s="8" t="s">
-        <v>1127</v>
+        <v>1116</v>
       </c>
       <c r="E192" s="8" t="s">
         <v>814</v>
@@ -12044,7 +12111,7 @@
         <v>805</v>
       </c>
       <c r="D193" s="8" t="s">
-        <v>1128</v>
+        <v>1117</v>
       </c>
       <c r="E193" s="8" t="s">
         <v>826</v>
@@ -12076,7 +12143,7 @@
         <v>805</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>1141</v>
+        <v>1129</v>
       </c>
       <c r="E194" s="8" t="s">
         <v>820</v>
@@ -12111,7 +12178,7 @@
         <v>805</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>1129</v>
+        <v>1118</v>
       </c>
       <c r="E195" s="8" t="s">
         <v>823</v>
@@ -12143,7 +12210,7 @@
         <v>805</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>1130</v>
+        <v>1119</v>
       </c>
       <c r="E196" s="8" t="s">
         <v>830</v>
@@ -12175,7 +12242,7 @@
         <v>805</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>1131</v>
+        <v>1120</v>
       </c>
       <c r="E197" s="8" t="s">
         <v>837</v>
@@ -12207,7 +12274,7 @@
         <v>805</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>1132</v>
+        <v>1121</v>
       </c>
       <c r="E198" s="8" t="s">
         <v>838</v>
@@ -12239,7 +12306,7 @@
         <v>805</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>1133</v>
+        <v>1122</v>
       </c>
       <c r="E199" s="8" t="s">
         <v>842</v>
@@ -12271,7 +12338,7 @@
         <v>805</v>
       </c>
       <c r="D200" s="8" t="s">
-        <v>1142</v>
+        <v>1130</v>
       </c>
       <c r="E200" s="8" t="s">
         <v>846</v>
@@ -12303,7 +12370,7 @@
         <v>805</v>
       </c>
       <c r="D201" s="8" t="s">
-        <v>1143</v>
+        <v>1131</v>
       </c>
       <c r="E201" s="8" t="s">
         <v>850</v>
@@ -12335,7 +12402,7 @@
         <v>805</v>
       </c>
       <c r="D202" s="8" t="s">
-        <v>1134</v>
+        <v>1123</v>
       </c>
       <c r="E202" s="8" t="s">
         <v>855</v>
@@ -12367,7 +12434,7 @@
         <v>805</v>
       </c>
       <c r="D203" s="8" t="s">
-        <v>1131</v>
+        <v>1120</v>
       </c>
       <c r="E203" s="8" t="s">
         <v>862</v>
@@ -12492,7 +12559,7 @@
         <v>874</v>
       </c>
       <c r="D207" s="8" t="s">
-        <v>1135</v>
+        <v>1124</v>
       </c>
       <c r="E207" s="8" t="s">
         <v>879</v>
@@ -12524,7 +12591,7 @@
         <v>875</v>
       </c>
       <c r="D208" s="8" t="s">
-        <v>1136</v>
+        <v>1125</v>
       </c>
       <c r="E208" s="8" t="s">
         <v>876</v>
@@ -12556,7 +12623,7 @@
         <v>885</v>
       </c>
       <c r="D209" s="8" t="s">
-        <v>1137</v>
+        <v>1126</v>
       </c>
       <c r="E209" s="8" t="s">
         <v>886</v>

</xml_diff>

<commit_message>
started Calendar section(Add Event)...
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3975" uniqueCount="1231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3972" uniqueCount="1236">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5065,34 +5065,13 @@
     <t>fA_AddRemarkforstudent'sFeedbackofView</t>
   </si>
   <si>
-    <t>fv_ValidationToofTimefields</t>
-  </si>
-  <si>
     <t>fP_ViewofPlannedLessons</t>
   </si>
   <si>
-    <t>fe_ManageAssignmentIsofCalendarsection</t>
-  </si>
-  <si>
     <t>fn_ViewAverageScoreofSelectedSubject</t>
   </si>
   <si>
-    <t>fv_ValidationsofMandatoryfields</t>
-  </si>
-  <si>
-    <t>fv_CancelofEventpopup</t>
-  </si>
-  <si>
     <t>ft_ViewofLessonplan</t>
-  </si>
-  <si>
-    <t>fe_ViewAllTheLessonPlansofYouTeacher)</t>
-  </si>
-  <si>
-    <t>fe_ViewAllTheofSpecifieddates</t>
-  </si>
-  <si>
-    <t>fe_ViewAllTheActivitiesOfLearningofSpecifieddates</t>
   </si>
   <si>
     <t>fe_ViewTheofStudent'slearning</t>
@@ -5475,13 +5454,51 @@
   <si>
     <t>No students present: Fail</t>
   </si>
+  <si>
+    <t>fn_AddAllDayEvent</t>
+  </si>
+  <si>
+    <t>fn_AddSpecificHourEvent</t>
+  </si>
+  <si>
+    <t>fn_ValidationsforMandatoryfields</t>
+  </si>
+  <si>
+    <t>1. On Teacher Dashboard, under Calendar section, click on Add Event
+2. Enter/Select all fields except Title and click on Save button
+3.  Enter/Select all fields except Description and click on Save button
+4. Select From Date &amp; Time greater than current date &amp; time and To Date &amp; Time less than current date &amp; time then click on Save button</t>
+  </si>
+  <si>
+    <t>fn_ValidationifFromTimeGreaterthanCurrntandTotimeLessthanCurrnt</t>
+  </si>
+  <si>
+    <t>fn_ValidationifFromTimeLessthanCurrntandTotimeGreaterthanCurrnt</t>
+  </si>
+  <si>
+    <t>fn_ValidationifToDateLessthanFromDate</t>
+  </si>
+  <si>
+    <t>fn_CancelAddEventPopup</t>
+  </si>
+  <si>
+    <t>fn_VisibilityofManageAssignments</t>
+  </si>
+  <si>
+    <t>fn_ViewAllLessonPlansbyTeacher</t>
+  </si>
+  <si>
+    <t>fn_ViewAllActivitiesforSpecifieddates</t>
+  </si>
+  <si>
+    <t>fe_ViewAllLearningMaterialsforSpecifieddates</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5952,25 +5969,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F167" workbookViewId="0">
-      <selection activeCell="K167" sqref="K167"/>
+    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
+      <selection activeCell="D185" sqref="D185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="18.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="16.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="8" width="16.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="6" width="31.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="6" width="33.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="41.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="6" width="26.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="6" width="11.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="8" width="52.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.5703125" style="8" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.85546875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.5703125" style="6" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="41.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26" style="6" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" style="6" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="52.7109375" style="8" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -8567,7 +8584,7 @@
         <v>347</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>352</v>
@@ -8599,7 +8616,7 @@
         <v>347</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>1122</v>
+        <v>1115</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>355</v>
@@ -8631,7 +8648,7 @@
         <v>347</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>1127</v>
+        <v>1120</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>360</v>
@@ -8663,7 +8680,7 @@
         <v>347</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>1128</v>
+        <v>1121</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>364</v>
@@ -8695,7 +8712,7 @@
         <v>368</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>1129</v>
+        <v>1122</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>370</v>
@@ -8727,7 +8744,7 @@
         <v>368</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>1130</v>
+        <v>1123</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>374</v>
@@ -8757,7 +8774,7 @@
         <v>377</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>1131</v>
+        <v>1124</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>382</v>
@@ -8786,7 +8803,7 @@
         <v>381</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>1132</v>
+        <v>1125</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>384</v>
@@ -8818,7 +8835,7 @@
         <v>381</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>1133</v>
+        <v>1126</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>386</v>
@@ -8850,7 +8867,7 @@
         <v>381</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>1134</v>
+        <v>1127</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>390</v>
@@ -8882,7 +8899,7 @@
         <v>381</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>1135</v>
+        <v>1128</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>394</v>
@@ -8914,7 +8931,7 @@
         <v>381</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>1136</v>
+        <v>1129</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>398</v>
@@ -8946,7 +8963,7 @@
         <v>381</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>1137</v>
+        <v>1130</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>403</v>
@@ -8978,7 +8995,7 @@
         <v>381</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>1138</v>
+        <v>1131</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>407</v>
@@ -9010,7 +9027,7 @@
         <v>414</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>1139</v>
+        <v>1132</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>412</v>
@@ -9042,7 +9059,7 @@
         <v>414</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>1140</v>
+        <v>1133</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>416</v>
@@ -9074,7 +9091,7 @@
         <v>425</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>1141</v>
+        <v>1134</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>424</v>
@@ -9106,7 +9123,7 @@
         <v>422</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>1142</v>
+        <v>1135</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>427</v>
@@ -9138,7 +9155,7 @@
         <v>422</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>1143</v>
+        <v>1136</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>429</v>
@@ -9159,7 +9176,7 @@
         <v>1012</v>
       </c>
       <c r="L101" s="8" t="s">
-        <v>1144</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="195" x14ac:dyDescent="0.25">
@@ -9173,7 +9190,7 @@
         <v>422</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>1145</v>
+        <v>1138</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>436</v>
@@ -9205,7 +9222,7 @@
         <v>422</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>1146</v>
+        <v>1139</v>
       </c>
       <c r="E103" s="8" t="s">
         <v>438</v>
@@ -9234,7 +9251,7 @@
         <v>442</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>1147</v>
+        <v>1140</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>443</v>
@@ -9266,7 +9283,7 @@
         <v>442</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>1148</v>
+        <v>1141</v>
       </c>
       <c r="E105" s="8" t="s">
         <v>446</v>
@@ -9298,7 +9315,7 @@
         <v>442</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>1149</v>
+        <v>1142</v>
       </c>
       <c r="E106" s="8" t="s">
         <v>451</v>
@@ -9330,7 +9347,7 @@
         <v>442</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>1150</v>
+        <v>1143</v>
       </c>
       <c r="E107" s="8" t="s">
         <v>455</v>
@@ -9359,7 +9376,7 @@
         <v>458</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>1151</v>
+        <v>1144</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>460</v>
@@ -9388,7 +9405,7 @@
         <v>458</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>1152</v>
+        <v>1145</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>620</v>
@@ -9417,7 +9434,7 @@
         <v>458</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>1153</v>
+        <v>1146</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>621</v>
@@ -9446,7 +9463,7 @@
         <v>464</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>1154</v>
+        <v>1147</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>465</v>
@@ -9472,10 +9489,10 @@
         <v>411</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>1157</v>
+        <v>1150</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>1156</v>
+        <v>1149</v>
       </c>
       <c r="E112" s="8"/>
       <c r="G112" s="2"/>
@@ -9495,7 +9512,7 @@
         <v>468</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>1155</v>
+        <v>1148</v>
       </c>
       <c r="E113" s="8" t="s">
         <v>471</v>
@@ -9524,7 +9541,7 @@
         <v>472</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>1158</v>
+        <v>1151</v>
       </c>
       <c r="E114" s="8" t="s">
         <v>474</v>
@@ -9553,7 +9570,7 @@
         <v>481</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>1159</v>
+        <v>1152</v>
       </c>
       <c r="E115" s="8" t="s">
         <v>424</v>
@@ -9585,7 +9602,7 @@
         <v>477</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>1160</v>
+        <v>1153</v>
       </c>
       <c r="E116" s="8" t="s">
         <v>478</v>
@@ -9617,7 +9634,7 @@
         <v>486</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>1161</v>
+        <v>1154</v>
       </c>
       <c r="E117" s="8" t="s">
         <v>487</v>
@@ -9649,7 +9666,7 @@
         <v>490</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>1162</v>
+        <v>1155</v>
       </c>
       <c r="E118" s="8" t="s">
         <v>491</v>
@@ -9681,7 +9698,7 @@
         <v>490</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>1163</v>
+        <v>1156</v>
       </c>
       <c r="E119" s="8" t="s">
         <v>495</v>
@@ -9713,7 +9730,7 @@
         <v>498</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>1164</v>
+        <v>1157</v>
       </c>
       <c r="E120" s="8" t="s">
         <v>500</v>
@@ -9748,7 +9765,7 @@
         <v>498</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>1165</v>
+        <v>1158</v>
       </c>
       <c r="E121" s="8" t="s">
         <v>505</v>
@@ -9780,7 +9797,7 @@
         <v>498</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>1166</v>
+        <v>1159</v>
       </c>
       <c r="E122" s="8" t="s">
         <v>508</v>
@@ -9816,7 +9833,7 @@
         <v>498</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>1167</v>
+        <v>1160</v>
       </c>
       <c r="E123" s="8" t="s">
         <v>513</v>
@@ -9849,7 +9866,7 @@
         <v>498</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>1168</v>
+        <v>1161</v>
       </c>
       <c r="E124" s="8" t="s">
         <v>521</v>
@@ -9868,7 +9885,7 @@
         <v>1012</v>
       </c>
       <c r="L124" s="20" t="s">
-        <v>1169</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="125" spans="1:12" ht="315" x14ac:dyDescent="0.25">
@@ -9879,22 +9896,22 @@
         <v>411</v>
       </c>
       <c r="C125" s="8" t="s">
+        <v>1164</v>
+      </c>
+      <c r="D125" s="8" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E125" s="8" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F125" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G125" s="2" t="s">
         <v>1171</v>
       </c>
-      <c r="D125" s="8" t="s">
-        <v>1172</v>
-      </c>
-      <c r="E125" s="8" t="s">
-        <v>1173</v>
-      </c>
-      <c r="F125" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G125" s="2" t="s">
-        <v>1178</v>
-      </c>
       <c r="H125" s="2" t="s">
-        <v>1174</v>
+        <v>1167</v>
       </c>
       <c r="I125" s="2" t="s">
         <v>502</v>
@@ -9917,7 +9934,7 @@
         <v>498</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>1175</v>
+        <v>1168</v>
       </c>
       <c r="E126" s="8" t="s">
         <v>505</v>
@@ -9949,7 +9966,7 @@
         <v>498</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>1176</v>
+        <v>1169</v>
       </c>
       <c r="E127" s="8" t="s">
         <v>508</v>
@@ -9958,7 +9975,7 @@
         <v>38</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>1177</v>
+        <v>1170</v>
       </c>
       <c r="H127" s="2"/>
       <c r="I127" s="2" t="s">
@@ -9985,7 +10002,7 @@
         <v>498</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>1179</v>
+        <v>1172</v>
       </c>
       <c r="E128" s="8" t="s">
         <v>513</v>
@@ -10018,7 +10035,7 @@
         <v>498</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>1181</v>
+        <v>1174</v>
       </c>
       <c r="E129" s="8" t="s">
         <v>521</v>
@@ -10037,7 +10054,7 @@
         <v>911</v>
       </c>
       <c r="L129" s="20" t="s">
-        <v>1169</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="130" spans="1:12" ht="375" x14ac:dyDescent="0.25">
@@ -10051,7 +10068,7 @@
         <v>540</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>1170</v>
+        <v>1163</v>
       </c>
       <c r="E130" s="8" t="s">
         <v>543</v>
@@ -10083,7 +10100,7 @@
         <v>540</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>1182</v>
+        <v>1175</v>
       </c>
       <c r="E131" s="8" t="s">
         <v>548</v>
@@ -10116,7 +10133,7 @@
         <v>552</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>1183</v>
+        <v>1176</v>
       </c>
       <c r="E132" s="8" t="s">
         <v>553</v>
@@ -10137,7 +10154,7 @@
         <v>1012</v>
       </c>
       <c r="L132" s="20" t="s">
-        <v>1180</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="133" spans="1:12" ht="165" x14ac:dyDescent="0.25">
@@ -10151,7 +10168,7 @@
         <v>552</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>1184</v>
+        <v>1177</v>
       </c>
       <c r="E133" s="8" t="s">
         <v>557</v>
@@ -10183,7 +10200,7 @@
         <v>561</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>1185</v>
+        <v>1178</v>
       </c>
       <c r="E134" s="8" t="s">
         <v>562</v>
@@ -10215,7 +10232,7 @@
         <v>561</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>1186</v>
+        <v>1179</v>
       </c>
       <c r="E135" s="8" t="s">
         <v>565</v>
@@ -10247,7 +10264,7 @@
         <v>561</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>1187</v>
+        <v>1180</v>
       </c>
       <c r="E136" s="8" t="s">
         <v>568</v>
@@ -10279,7 +10296,7 @@
         <v>561</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>1188</v>
+        <v>1181</v>
       </c>
       <c r="E137" s="8" t="s">
         <v>572</v>
@@ -10311,7 +10328,7 @@
         <v>561</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>1189</v>
+        <v>1182</v>
       </c>
       <c r="E138" s="8" t="s">
         <v>576</v>
@@ -10343,7 +10360,7 @@
         <v>581</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>1190</v>
+        <v>1183</v>
       </c>
       <c r="E139" s="6" t="s">
         <v>582</v>
@@ -10375,7 +10392,7 @@
         <v>581</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>1191</v>
+        <v>1184</v>
       </c>
       <c r="E140" s="8" t="s">
         <v>625</v>
@@ -10407,7 +10424,7 @@
         <v>581</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>1192</v>
+        <v>1185</v>
       </c>
       <c r="E141" s="8" t="s">
         <v>628</v>
@@ -10439,7 +10456,7 @@
         <v>581</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>1193</v>
+        <v>1186</v>
       </c>
       <c r="E142" s="8" t="s">
         <v>586</v>
@@ -10471,7 +10488,7 @@
         <v>594</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>1194</v>
+        <v>1187</v>
       </c>
       <c r="E143" s="8" t="s">
         <v>593</v>
@@ -10492,7 +10509,7 @@
         <v>1012</v>
       </c>
       <c r="L143" s="20" t="s">
-        <v>1204</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="144" spans="1:12" ht="180" x14ac:dyDescent="0.25">
@@ -10506,7 +10523,7 @@
         <v>595</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>1195</v>
+        <v>1188</v>
       </c>
       <c r="E144" s="8" t="s">
         <v>596</v>
@@ -10538,7 +10555,7 @@
         <v>595</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>1196</v>
+        <v>1189</v>
       </c>
       <c r="E145" s="8" t="s">
         <v>600</v>
@@ -10570,7 +10587,7 @@
         <v>595</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>1197</v>
+        <v>1190</v>
       </c>
       <c r="E146" s="8" t="s">
         <v>604</v>
@@ -10605,7 +10622,7 @@
         <v>595</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>1198</v>
+        <v>1191</v>
       </c>
       <c r="E147" s="8" t="s">
         <v>609</v>
@@ -10637,7 +10654,7 @@
         <v>595</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>1199</v>
+        <v>1192</v>
       </c>
       <c r="E148" s="8" t="s">
         <v>612</v>
@@ -10669,7 +10686,7 @@
         <v>617</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>1200</v>
+        <v>1193</v>
       </c>
       <c r="E149" s="6" t="s">
         <v>635</v>
@@ -10701,7 +10718,7 @@
         <v>617</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>1201</v>
+        <v>1194</v>
       </c>
       <c r="E150" s="8" t="s">
         <v>638</v>
@@ -10733,7 +10750,7 @@
         <v>617</v>
       </c>
       <c r="D151" s="8" t="s">
-        <v>1202</v>
+        <v>1195</v>
       </c>
       <c r="E151" s="6" t="s">
         <v>641</v>
@@ -10765,7 +10782,7 @@
         <v>617</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>1203</v>
+        <v>1196</v>
       </c>
       <c r="E152" s="8" t="s">
         <v>645</v>
@@ -10797,7 +10814,7 @@
         <v>617</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>1205</v>
+        <v>1198</v>
       </c>
       <c r="E153" s="8" t="s">
         <v>649</v>
@@ -10829,7 +10846,7 @@
         <v>617</v>
       </c>
       <c r="D154" s="8" t="s">
-        <v>1206</v>
+        <v>1199</v>
       </c>
       <c r="E154" s="8" t="s">
         <v>653</v>
@@ -10861,7 +10878,7 @@
         <v>617</v>
       </c>
       <c r="D155" s="8" t="s">
-        <v>1207</v>
+        <v>1200</v>
       </c>
       <c r="E155" s="8" t="s">
         <v>657</v>
@@ -10893,7 +10910,7 @@
         <v>617</v>
       </c>
       <c r="D156" s="8" t="s">
-        <v>1208</v>
+        <v>1201</v>
       </c>
       <c r="E156" s="8" t="s">
         <v>661</v>
@@ -10925,7 +10942,7 @@
         <v>665</v>
       </c>
       <c r="D157" s="8" t="s">
-        <v>1209</v>
+        <v>1202</v>
       </c>
       <c r="E157" s="8" t="s">
         <v>666</v>
@@ -10942,11 +10959,11 @@
       <c r="I157" s="2" t="s">
         <v>669</v>
       </c>
-      <c r="K157" s="20" t="s">
-        <v>909</v>
+      <c r="K157" t="s">
+        <v>1012</v>
       </c>
       <c r="L157" s="20" t="s">
-        <v>1210</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="158" spans="1:12" ht="195" x14ac:dyDescent="0.25">
@@ -10960,7 +10977,7 @@
         <v>665</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>1211</v>
+        <v>1204</v>
       </c>
       <c r="E158" s="8" t="s">
         <v>694</v>
@@ -10993,7 +11010,7 @@
         <v>665</v>
       </c>
       <c r="D159" s="8" t="s">
-        <v>1212</v>
+        <v>1205</v>
       </c>
       <c r="E159" s="8" t="s">
         <v>671</v>
@@ -11028,7 +11045,7 @@
         <v>665</v>
       </c>
       <c r="D160" s="8" t="s">
-        <v>1213</v>
+        <v>1206</v>
       </c>
       <c r="E160" s="8" t="s">
         <v>675</v>
@@ -11060,7 +11077,7 @@
         <v>665</v>
       </c>
       <c r="D161" s="8" t="s">
-        <v>1214</v>
+        <v>1207</v>
       </c>
       <c r="E161" s="8" t="s">
         <v>679</v>
@@ -11092,7 +11109,7 @@
         <v>665</v>
       </c>
       <c r="D162" s="8" t="s">
-        <v>1215</v>
+        <v>1208</v>
       </c>
       <c r="E162" s="8" t="s">
         <v>683</v>
@@ -11109,8 +11126,8 @@
       <c r="J162" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K162" s="8" t="s">
-        <v>911</v>
+      <c r="K162" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="163" spans="1:27" ht="285" x14ac:dyDescent="0.25">
@@ -11124,7 +11141,7 @@
         <v>665</v>
       </c>
       <c r="D163" s="8" t="s">
-        <v>1216</v>
+        <v>1209</v>
       </c>
       <c r="E163" s="8" t="s">
         <v>687</v>
@@ -11141,8 +11158,8 @@
       <c r="J163" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K163" s="8" t="s">
-        <v>911</v>
+      <c r="K163" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="164" spans="1:27" ht="315" x14ac:dyDescent="0.25">
@@ -11156,7 +11173,7 @@
         <v>665</v>
       </c>
       <c r="D164" s="8" t="s">
-        <v>1217</v>
+        <v>1210</v>
       </c>
       <c r="E164" s="8" t="s">
         <v>691</v>
@@ -11173,8 +11190,8 @@
       <c r="J164" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K164" s="8" t="s">
-        <v>911</v>
+      <c r="K164" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="165" spans="1:27" ht="150" x14ac:dyDescent="0.25">
@@ -11188,7 +11205,7 @@
         <v>699</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>1218</v>
+        <v>1211</v>
       </c>
       <c r="E165" s="8" t="s">
         <v>700</v>
@@ -11220,7 +11237,7 @@
         <v>699</v>
       </c>
       <c r="D166" s="8" t="s">
-        <v>1219</v>
+        <v>1212</v>
       </c>
       <c r="E166" s="8" t="s">
         <v>704</v>
@@ -11252,7 +11269,7 @@
         <v>699</v>
       </c>
       <c r="D167" s="8" t="s">
-        <v>1220</v>
+        <v>1213</v>
       </c>
       <c r="E167" s="8" t="s">
         <v>707</v>
@@ -11284,7 +11301,7 @@
         <v>699</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>1221</v>
+        <v>1214</v>
       </c>
       <c r="E168" s="8" t="s">
         <v>710</v>
@@ -11316,7 +11333,7 @@
         <v>713</v>
       </c>
       <c r="D169" s="8" t="s">
-        <v>1222</v>
+        <v>1215</v>
       </c>
       <c r="E169" s="8" t="s">
         <v>714</v>
@@ -11334,10 +11351,10 @@
         <v>964</v>
       </c>
       <c r="K169" t="s">
-        <v>1230</v>
+        <v>1223</v>
       </c>
       <c r="L169" s="20" t="s">
-        <v>1223</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="170" spans="1:27" ht="225" x14ac:dyDescent="0.25">
@@ -11351,7 +11368,7 @@
         <v>713</v>
       </c>
       <c r="D170" s="8" t="s">
-        <v>1224</v>
+        <v>1217</v>
       </c>
       <c r="E170" s="8" t="s">
         <v>718</v>
@@ -11368,8 +11385,8 @@
       <c r="J170" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K170" s="6" t="s">
-        <v>911</v>
+      <c r="K170" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="171" spans="1:27" ht="270" x14ac:dyDescent="0.25">
@@ -11383,7 +11400,7 @@
         <v>713</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>1225</v>
+        <v>1218</v>
       </c>
       <c r="E171" s="8" t="s">
         <v>722</v>
@@ -11400,8 +11417,8 @@
       <c r="J171" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K171" s="6" t="s">
-        <v>911</v>
+      <c r="K171" t="s">
+        <v>1223</v>
       </c>
     </row>
     <row r="172" spans="1:27" ht="285.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11415,7 +11432,7 @@
         <v>713</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>1226</v>
+        <v>1219</v>
       </c>
       <c r="E172" s="8" t="s">
         <v>726</v>
@@ -11432,8 +11449,8 @@
       <c r="J172" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K172" s="6" t="s">
-        <v>911</v>
+      <c r="K172" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="173" spans="1:27" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11447,7 +11464,7 @@
         <v>713</v>
       </c>
       <c r="D173" s="8" t="s">
-        <v>1227</v>
+        <v>1220</v>
       </c>
       <c r="E173" s="10" t="s">
         <v>731</v>
@@ -11465,8 +11482,8 @@
       <c r="J173" s="23" t="s">
         <v>964</v>
       </c>
-      <c r="K173" s="23" t="s">
-        <v>911</v>
+      <c r="K173" t="s">
+        <v>1012</v>
       </c>
       <c r="L173" s="23"/>
       <c r="M173" s="11"/>
@@ -11496,7 +11513,7 @@
         <v>735</v>
       </c>
       <c r="D174" s="8" t="s">
-        <v>1228</v>
+        <v>1221</v>
       </c>
       <c r="E174" s="14" t="s">
         <v>748</v>
@@ -11545,7 +11562,7 @@
         <v>753</v>
       </c>
       <c r="D175" s="8" t="s">
-        <v>1001</v>
+        <v>1224</v>
       </c>
       <c r="E175" s="8" t="s">
         <v>754</v>
@@ -11580,7 +11597,7 @@
         <v>753</v>
       </c>
       <c r="D176" s="8" t="s">
-        <v>1002</v>
+        <v>1225</v>
       </c>
       <c r="E176" s="8" t="s">
         <v>759</v>
@@ -11618,7 +11635,7 @@
         <v>753</v>
       </c>
       <c r="D177" s="8" t="s">
-        <v>1107</v>
+        <v>1226</v>
       </c>
       <c r="E177" s="8" t="s">
         <v>764</v>
@@ -11639,7 +11656,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="178" spans="1:12" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:12" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="6" t="s">
         <v>763</v>
       </c>
@@ -11650,7 +11667,7 @@
         <v>753</v>
       </c>
       <c r="D178" s="8" t="s">
-        <v>1103</v>
+        <v>1228</v>
       </c>
       <c r="E178" s="8" t="s">
         <v>768</v>
@@ -11659,7 +11676,7 @@
         <v>38</v>
       </c>
       <c r="G178" s="13" t="s">
-        <v>765</v>
+        <v>1227</v>
       </c>
       <c r="I178" s="2" t="s">
         <v>766</v>
@@ -11682,7 +11699,7 @@
         <v>753</v>
       </c>
       <c r="D179" s="8" t="s">
-        <v>1103</v>
+        <v>1229</v>
       </c>
       <c r="E179" s="8" t="s">
         <v>768</v>
@@ -11715,7 +11732,7 @@
         <v>753</v>
       </c>
       <c r="D180" s="8" t="s">
-        <v>1103</v>
+        <v>1230</v>
       </c>
       <c r="E180" s="8" t="s">
         <v>768</v>
@@ -11748,7 +11765,7 @@
         <v>753</v>
       </c>
       <c r="D181" s="8" t="s">
-        <v>1108</v>
+        <v>1231</v>
       </c>
       <c r="E181" s="8" t="s">
         <v>776</v>
@@ -11780,7 +11797,7 @@
         <v>805</v>
       </c>
       <c r="D182" s="8" t="s">
-        <v>1105</v>
+        <v>1232</v>
       </c>
       <c r="E182" s="8" t="s">
         <v>806</v>
@@ -11801,7 +11818,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="183" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="6" t="s">
         <v>780</v>
       </c>
@@ -11812,7 +11829,7 @@
         <v>805</v>
       </c>
       <c r="D183" s="8" t="s">
-        <v>1110</v>
+        <v>1233</v>
       </c>
       <c r="E183" s="8" t="s">
         <v>809</v>
@@ -11844,7 +11861,7 @@
         <v>805</v>
       </c>
       <c r="D184" s="8" t="s">
-        <v>1111</v>
+        <v>1234</v>
       </c>
       <c r="E184" s="8" t="s">
         <v>814</v>
@@ -11876,7 +11893,7 @@
         <v>805</v>
       </c>
       <c r="D185" s="8" t="s">
-        <v>1112</v>
+        <v>1235</v>
       </c>
       <c r="E185" s="8" t="s">
         <v>826</v>
@@ -11908,7 +11925,7 @@
         <v>805</v>
       </c>
       <c r="D186" s="8" t="s">
-        <v>1124</v>
+        <v>1117</v>
       </c>
       <c r="E186" s="8" t="s">
         <v>820</v>
@@ -11943,7 +11960,7 @@
         <v>805</v>
       </c>
       <c r="D187" s="8" t="s">
-        <v>1113</v>
+        <v>1106</v>
       </c>
       <c r="E187" s="8" t="s">
         <v>823</v>
@@ -11975,7 +11992,7 @@
         <v>805</v>
       </c>
       <c r="D188" s="8" t="s">
-        <v>1114</v>
+        <v>1107</v>
       </c>
       <c r="E188" s="8" t="s">
         <v>830</v>
@@ -12007,7 +12024,7 @@
         <v>805</v>
       </c>
       <c r="D189" s="8" t="s">
-        <v>1115</v>
+        <v>1108</v>
       </c>
       <c r="E189" s="8" t="s">
         <v>837</v>
@@ -12039,7 +12056,7 @@
         <v>805</v>
       </c>
       <c r="D190" s="8" t="s">
-        <v>1116</v>
+        <v>1109</v>
       </c>
       <c r="E190" s="8" t="s">
         <v>838</v>
@@ -12071,7 +12088,7 @@
         <v>805</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>1117</v>
+        <v>1110</v>
       </c>
       <c r="E191" s="8" t="s">
         <v>842</v>
@@ -12103,7 +12120,7 @@
         <v>805</v>
       </c>
       <c r="D192" s="8" t="s">
-        <v>1125</v>
+        <v>1118</v>
       </c>
       <c r="E192" s="8" t="s">
         <v>846</v>
@@ -12135,7 +12152,7 @@
         <v>805</v>
       </c>
       <c r="D193" s="8" t="s">
-        <v>1126</v>
+        <v>1119</v>
       </c>
       <c r="E193" s="8" t="s">
         <v>850</v>
@@ -12167,7 +12184,7 @@
         <v>805</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>1118</v>
+        <v>1111</v>
       </c>
       <c r="E194" s="8" t="s">
         <v>855</v>
@@ -12199,7 +12216,7 @@
         <v>805</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>1115</v>
+        <v>1108</v>
       </c>
       <c r="E195" s="8" t="s">
         <v>862</v>
@@ -12324,7 +12341,7 @@
         <v>874</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>1119</v>
+        <v>1112</v>
       </c>
       <c r="E199" s="8" t="s">
         <v>879</v>
@@ -12356,7 +12373,7 @@
         <v>875</v>
       </c>
       <c r="D200" s="8" t="s">
-        <v>1120</v>
+        <v>1113</v>
       </c>
       <c r="E200" s="8" t="s">
         <v>876</v>
@@ -12388,7 +12405,7 @@
         <v>885</v>
       </c>
       <c r="D201" s="8" t="s">
-        <v>1121</v>
+        <v>1114</v>
       </c>
       <c r="E201" s="8" t="s">
         <v>886</v>
@@ -12438,7 +12455,7 @@
         <v>970</v>
       </c>
       <c r="M202" t="s">
-        <v>1229</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="203" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12452,7 +12469,7 @@
         <v>736</v>
       </c>
       <c r="D203" s="8" t="s">
-        <v>1123</v>
+        <v>1116</v>
       </c>
       <c r="E203" s="8" t="s">
         <v>741</v>
@@ -12476,7 +12493,7 @@
         <v>969</v>
       </c>
       <c r="M203" t="s">
-        <v>1229</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="204" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12511,7 +12528,7 @@
         <v>960</v>
       </c>
       <c r="M204" t="s">
-        <v>1229</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="205" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12525,7 +12542,7 @@
         <v>779</v>
       </c>
       <c r="D205" s="8" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="E205" s="6" t="s">
         <v>786</v>
@@ -12546,7 +12563,7 @@
         <v>911</v>
       </c>
       <c r="M205" t="s">
-        <v>1229</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="206" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12560,7 +12577,7 @@
         <v>784</v>
       </c>
       <c r="D206" s="8" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="E206" s="6" t="s">
         <v>785</v>
@@ -12581,7 +12598,7 @@
         <v>911</v>
       </c>
       <c r="M206" t="s">
-        <v>1229</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="207" spans="1:13" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12616,7 +12633,7 @@
         <v>961</v>
       </c>
       <c r="M207" t="s">
-        <v>1229</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="208" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12651,7 +12668,7 @@
         <v>961</v>
       </c>
       <c r="M208" t="s">
-        <v>1229</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="209" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12689,7 +12706,7 @@
         <v>961</v>
       </c>
       <c r="M209" t="s">
-        <v>1229</v>
+        <v>1222</v>
       </c>
     </row>
   </sheetData>
@@ -12708,17 +12725,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="31.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="37.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Worked on Assignment section under manage assignment section..
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3972" uniqueCount="1236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3974" uniqueCount="1239">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5074,24 +5074,6 @@
     <t>ft_ViewofLessonplan</t>
   </si>
   <si>
-    <t>fe_ViewTheofStudent'slearning</t>
-  </si>
-  <si>
-    <t>fe_ViewAllTheTestsWithinofDaterange</t>
-  </si>
-  <si>
-    <t>fe_ViewofSubmissiondetails</t>
-  </si>
-  <si>
-    <t>fe_SaveRemarkFeedbackForTheofTestactivity)</t>
-  </si>
-  <si>
-    <t>fe_ViewofTestreport</t>
-  </si>
-  <si>
-    <t>fe_ViewAllTheAssignmentsWithinofDaterange</t>
-  </si>
-  <si>
     <t>f _MarksEntryLinkofInheader</t>
   </si>
   <si>
@@ -5105,15 +5087,6 @@
   </si>
   <si>
     <t>fL_ViewLessonsPlannedForTheWeek</t>
-  </si>
-  <si>
-    <t>fe_ViewTheStudentResourceMarkingReport</t>
-  </si>
-  <si>
-    <t>fe_EvaluateTheRespectiveTest</t>
-  </si>
-  <si>
-    <t>fe_UploadingWorksheet</t>
   </si>
   <si>
     <t>fn_ViewOverallPerformanceandStudentSubmissionStatusReport</t>
@@ -5491,7 +5464,43 @@
     <t>fn_ViewAllActivitiesforSpecifieddates</t>
   </si>
   <si>
-    <t>fe_ViewAllLearningMaterialsforSpecifieddates</t>
+    <t>fn_ViewAllLearningMaterialsforSpecifieddates</t>
+  </si>
+  <si>
+    <t>fn_ViewStudentResourceMarkingReport</t>
+  </si>
+  <si>
+    <t>fn_ViewStudentsLearning</t>
+  </si>
+  <si>
+    <t>fn_ViewTestsforSpecifiedDaterange</t>
+  </si>
+  <si>
+    <t>fn_ViewStudentSubmissiondetails</t>
+  </si>
+  <si>
+    <t>fn_SaveRemarkFeedbackofTest</t>
+  </si>
+  <si>
+    <t>fn_ViewTestReport</t>
+  </si>
+  <si>
+    <t>fn_EvaluateRespectiveTest</t>
+  </si>
+  <si>
+    <t>fn_UploadingWorksheet</t>
+  </si>
+  <si>
+    <t>fn_ViewAssignmentsWithinSpecifiedDaterange</t>
+  </si>
+  <si>
+    <t>fn_ViewAssignmentSubmissionDetails</t>
+  </si>
+  <si>
+    <t>fn_ViewAssignmentSubmissionsandResponses</t>
+  </si>
+  <si>
+    <t>fn_DownloadAssignmentSubmittedResources</t>
   </si>
 </sst>
 </file>
@@ -5969,8 +5978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
-      <selection activeCell="D185" sqref="D185"/>
+    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
+      <selection activeCell="D197" sqref="D197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8616,7 +8625,7 @@
         <v>347</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>1115</v>
+        <v>1109</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>355</v>
@@ -8648,7 +8657,7 @@
         <v>347</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>1120</v>
+        <v>1111</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>360</v>
@@ -8680,7 +8689,7 @@
         <v>347</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>1121</v>
+        <v>1112</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>364</v>
@@ -8712,7 +8721,7 @@
         <v>368</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>1122</v>
+        <v>1113</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>370</v>
@@ -8744,7 +8753,7 @@
         <v>368</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>1123</v>
+        <v>1114</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>374</v>
@@ -8774,7 +8783,7 @@
         <v>377</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>1124</v>
+        <v>1115</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>382</v>
@@ -8803,7 +8812,7 @@
         <v>381</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>1125</v>
+        <v>1116</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>384</v>
@@ -8835,7 +8844,7 @@
         <v>381</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>1126</v>
+        <v>1117</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>386</v>
@@ -8867,7 +8876,7 @@
         <v>381</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>1127</v>
+        <v>1118</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>390</v>
@@ -8899,7 +8908,7 @@
         <v>381</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>1128</v>
+        <v>1119</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>394</v>
@@ -8931,7 +8940,7 @@
         <v>381</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>1129</v>
+        <v>1120</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>398</v>
@@ -8963,7 +8972,7 @@
         <v>381</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>1130</v>
+        <v>1121</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>403</v>
@@ -8995,7 +9004,7 @@
         <v>381</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>1131</v>
+        <v>1122</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>407</v>
@@ -9027,7 +9036,7 @@
         <v>414</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>1132</v>
+        <v>1123</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>412</v>
@@ -9059,7 +9068,7 @@
         <v>414</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>1133</v>
+        <v>1124</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>416</v>
@@ -9091,7 +9100,7 @@
         <v>425</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>1134</v>
+        <v>1125</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>424</v>
@@ -9123,7 +9132,7 @@
         <v>422</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>1135</v>
+        <v>1126</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>427</v>
@@ -9155,7 +9164,7 @@
         <v>422</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>1136</v>
+        <v>1127</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>429</v>
@@ -9176,7 +9185,7 @@
         <v>1012</v>
       </c>
       <c r="L101" s="8" t="s">
-        <v>1137</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="195" x14ac:dyDescent="0.25">
@@ -9190,7 +9199,7 @@
         <v>422</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>1138</v>
+        <v>1129</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>436</v>
@@ -9222,7 +9231,7 @@
         <v>422</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>1139</v>
+        <v>1130</v>
       </c>
       <c r="E103" s="8" t="s">
         <v>438</v>
@@ -9251,7 +9260,7 @@
         <v>442</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>1140</v>
+        <v>1131</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>443</v>
@@ -9283,7 +9292,7 @@
         <v>442</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>1141</v>
+        <v>1132</v>
       </c>
       <c r="E105" s="8" t="s">
         <v>446</v>
@@ -9315,7 +9324,7 @@
         <v>442</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>1142</v>
+        <v>1133</v>
       </c>
       <c r="E106" s="8" t="s">
         <v>451</v>
@@ -9347,7 +9356,7 @@
         <v>442</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>1143</v>
+        <v>1134</v>
       </c>
       <c r="E107" s="8" t="s">
         <v>455</v>
@@ -9376,7 +9385,7 @@
         <v>458</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>1144</v>
+        <v>1135</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>460</v>
@@ -9405,7 +9414,7 @@
         <v>458</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>1145</v>
+        <v>1136</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>620</v>
@@ -9434,7 +9443,7 @@
         <v>458</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>1146</v>
+        <v>1137</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>621</v>
@@ -9463,7 +9472,7 @@
         <v>464</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>1147</v>
+        <v>1138</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>465</v>
@@ -9489,10 +9498,10 @@
         <v>411</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>1150</v>
+        <v>1141</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>1149</v>
+        <v>1140</v>
       </c>
       <c r="E112" s="8"/>
       <c r="G112" s="2"/>
@@ -9512,7 +9521,7 @@
         <v>468</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>1148</v>
+        <v>1139</v>
       </c>
       <c r="E113" s="8" t="s">
         <v>471</v>
@@ -9541,7 +9550,7 @@
         <v>472</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>1151</v>
+        <v>1142</v>
       </c>
       <c r="E114" s="8" t="s">
         <v>474</v>
@@ -9570,7 +9579,7 @@
         <v>481</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>1152</v>
+        <v>1143</v>
       </c>
       <c r="E115" s="8" t="s">
         <v>424</v>
@@ -9602,7 +9611,7 @@
         <v>477</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>1153</v>
+        <v>1144</v>
       </c>
       <c r="E116" s="8" t="s">
         <v>478</v>
@@ -9634,7 +9643,7 @@
         <v>486</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>1154</v>
+        <v>1145</v>
       </c>
       <c r="E117" s="8" t="s">
         <v>487</v>
@@ -9666,7 +9675,7 @@
         <v>490</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>1155</v>
+        <v>1146</v>
       </c>
       <c r="E118" s="8" t="s">
         <v>491</v>
@@ -9698,7 +9707,7 @@
         <v>490</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>1156</v>
+        <v>1147</v>
       </c>
       <c r="E119" s="8" t="s">
         <v>495</v>
@@ -9730,7 +9739,7 @@
         <v>498</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>1157</v>
+        <v>1148</v>
       </c>
       <c r="E120" s="8" t="s">
         <v>500</v>
@@ -9765,7 +9774,7 @@
         <v>498</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>1158</v>
+        <v>1149</v>
       </c>
       <c r="E121" s="8" t="s">
         <v>505</v>
@@ -9797,7 +9806,7 @@
         <v>498</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>1159</v>
+        <v>1150</v>
       </c>
       <c r="E122" s="8" t="s">
         <v>508</v>
@@ -9833,7 +9842,7 @@
         <v>498</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>1160</v>
+        <v>1151</v>
       </c>
       <c r="E123" s="8" t="s">
         <v>513</v>
@@ -9866,7 +9875,7 @@
         <v>498</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>1161</v>
+        <v>1152</v>
       </c>
       <c r="E124" s="8" t="s">
         <v>521</v>
@@ -9885,7 +9894,7 @@
         <v>1012</v>
       </c>
       <c r="L124" s="20" t="s">
-        <v>1162</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="125" spans="1:12" ht="315" x14ac:dyDescent="0.25">
@@ -9896,22 +9905,22 @@
         <v>411</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>1164</v>
+        <v>1155</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>1165</v>
+        <v>1156</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>1166</v>
+        <v>1157</v>
       </c>
       <c r="F125" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>1171</v>
+        <v>1162</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>1167</v>
+        <v>1158</v>
       </c>
       <c r="I125" s="2" t="s">
         <v>502</v>
@@ -9934,7 +9943,7 @@
         <v>498</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>1168</v>
+        <v>1159</v>
       </c>
       <c r="E126" s="8" t="s">
         <v>505</v>
@@ -9966,7 +9975,7 @@
         <v>498</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>1169</v>
+        <v>1160</v>
       </c>
       <c r="E127" s="8" t="s">
         <v>508</v>
@@ -9975,7 +9984,7 @@
         <v>38</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>1170</v>
+        <v>1161</v>
       </c>
       <c r="H127" s="2"/>
       <c r="I127" s="2" t="s">
@@ -10002,7 +10011,7 @@
         <v>498</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>1172</v>
+        <v>1163</v>
       </c>
       <c r="E128" s="8" t="s">
         <v>513</v>
@@ -10035,7 +10044,7 @@
         <v>498</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>1174</v>
+        <v>1165</v>
       </c>
       <c r="E129" s="8" t="s">
         <v>521</v>
@@ -10054,7 +10063,7 @@
         <v>911</v>
       </c>
       <c r="L129" s="20" t="s">
-        <v>1162</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="130" spans="1:12" ht="375" x14ac:dyDescent="0.25">
@@ -10068,7 +10077,7 @@
         <v>540</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>1163</v>
+        <v>1154</v>
       </c>
       <c r="E130" s="8" t="s">
         <v>543</v>
@@ -10100,7 +10109,7 @@
         <v>540</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>1175</v>
+        <v>1166</v>
       </c>
       <c r="E131" s="8" t="s">
         <v>548</v>
@@ -10133,7 +10142,7 @@
         <v>552</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>1176</v>
+        <v>1167</v>
       </c>
       <c r="E132" s="8" t="s">
         <v>553</v>
@@ -10154,7 +10163,7 @@
         <v>1012</v>
       </c>
       <c r="L132" s="20" t="s">
-        <v>1173</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="133" spans="1:12" ht="165" x14ac:dyDescent="0.25">
@@ -10168,7 +10177,7 @@
         <v>552</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>1177</v>
+        <v>1168</v>
       </c>
       <c r="E133" s="8" t="s">
         <v>557</v>
@@ -10200,7 +10209,7 @@
         <v>561</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>1178</v>
+        <v>1169</v>
       </c>
       <c r="E134" s="8" t="s">
         <v>562</v>
@@ -10232,7 +10241,7 @@
         <v>561</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>1179</v>
+        <v>1170</v>
       </c>
       <c r="E135" s="8" t="s">
         <v>565</v>
@@ -10264,7 +10273,7 @@
         <v>561</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>1180</v>
+        <v>1171</v>
       </c>
       <c r="E136" s="8" t="s">
         <v>568</v>
@@ -10296,7 +10305,7 @@
         <v>561</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>1181</v>
+        <v>1172</v>
       </c>
       <c r="E137" s="8" t="s">
         <v>572</v>
@@ -10328,7 +10337,7 @@
         <v>561</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>1182</v>
+        <v>1173</v>
       </c>
       <c r="E138" s="8" t="s">
         <v>576</v>
@@ -10360,7 +10369,7 @@
         <v>581</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>1183</v>
+        <v>1174</v>
       </c>
       <c r="E139" s="6" t="s">
         <v>582</v>
@@ -10392,7 +10401,7 @@
         <v>581</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>1184</v>
+        <v>1175</v>
       </c>
       <c r="E140" s="8" t="s">
         <v>625</v>
@@ -10424,7 +10433,7 @@
         <v>581</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>1185</v>
+        <v>1176</v>
       </c>
       <c r="E141" s="8" t="s">
         <v>628</v>
@@ -10456,7 +10465,7 @@
         <v>581</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>1186</v>
+        <v>1177</v>
       </c>
       <c r="E142" s="8" t="s">
         <v>586</v>
@@ -10488,7 +10497,7 @@
         <v>594</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>1187</v>
+        <v>1178</v>
       </c>
       <c r="E143" s="8" t="s">
         <v>593</v>
@@ -10509,7 +10518,7 @@
         <v>1012</v>
       </c>
       <c r="L143" s="20" t="s">
-        <v>1197</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="144" spans="1:12" ht="180" x14ac:dyDescent="0.25">
@@ -10523,7 +10532,7 @@
         <v>595</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>1188</v>
+        <v>1179</v>
       </c>
       <c r="E144" s="8" t="s">
         <v>596</v>
@@ -10555,7 +10564,7 @@
         <v>595</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>1189</v>
+        <v>1180</v>
       </c>
       <c r="E145" s="8" t="s">
         <v>600</v>
@@ -10587,7 +10596,7 @@
         <v>595</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>1190</v>
+        <v>1181</v>
       </c>
       <c r="E146" s="8" t="s">
         <v>604</v>
@@ -10622,7 +10631,7 @@
         <v>595</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>1191</v>
+        <v>1182</v>
       </c>
       <c r="E147" s="8" t="s">
         <v>609</v>
@@ -10654,7 +10663,7 @@
         <v>595</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>1192</v>
+        <v>1183</v>
       </c>
       <c r="E148" s="8" t="s">
         <v>612</v>
@@ -10686,7 +10695,7 @@
         <v>617</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>1193</v>
+        <v>1184</v>
       </c>
       <c r="E149" s="6" t="s">
         <v>635</v>
@@ -10718,7 +10727,7 @@
         <v>617</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>1194</v>
+        <v>1185</v>
       </c>
       <c r="E150" s="8" t="s">
         <v>638</v>
@@ -10750,7 +10759,7 @@
         <v>617</v>
       </c>
       <c r="D151" s="8" t="s">
-        <v>1195</v>
+        <v>1186</v>
       </c>
       <c r="E151" s="6" t="s">
         <v>641</v>
@@ -10782,7 +10791,7 @@
         <v>617</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>1196</v>
+        <v>1187</v>
       </c>
       <c r="E152" s="8" t="s">
         <v>645</v>
@@ -10814,7 +10823,7 @@
         <v>617</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>1198</v>
+        <v>1189</v>
       </c>
       <c r="E153" s="8" t="s">
         <v>649</v>
@@ -10846,7 +10855,7 @@
         <v>617</v>
       </c>
       <c r="D154" s="8" t="s">
-        <v>1199</v>
+        <v>1190</v>
       </c>
       <c r="E154" s="8" t="s">
         <v>653</v>
@@ -10878,7 +10887,7 @@
         <v>617</v>
       </c>
       <c r="D155" s="8" t="s">
-        <v>1200</v>
+        <v>1191</v>
       </c>
       <c r="E155" s="8" t="s">
         <v>657</v>
@@ -10910,7 +10919,7 @@
         <v>617</v>
       </c>
       <c r="D156" s="8" t="s">
-        <v>1201</v>
+        <v>1192</v>
       </c>
       <c r="E156" s="8" t="s">
         <v>661</v>
@@ -10942,7 +10951,7 @@
         <v>665</v>
       </c>
       <c r="D157" s="8" t="s">
-        <v>1202</v>
+        <v>1193</v>
       </c>
       <c r="E157" s="8" t="s">
         <v>666</v>
@@ -10963,7 +10972,7 @@
         <v>1012</v>
       </c>
       <c r="L157" s="20" t="s">
-        <v>1203</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="158" spans="1:12" ht="195" x14ac:dyDescent="0.25">
@@ -10977,7 +10986,7 @@
         <v>665</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>1204</v>
+        <v>1195</v>
       </c>
       <c r="E158" s="8" t="s">
         <v>694</v>
@@ -11010,7 +11019,7 @@
         <v>665</v>
       </c>
       <c r="D159" s="8" t="s">
-        <v>1205</v>
+        <v>1196</v>
       </c>
       <c r="E159" s="8" t="s">
         <v>671</v>
@@ -11045,7 +11054,7 @@
         <v>665</v>
       </c>
       <c r="D160" s="8" t="s">
-        <v>1206</v>
+        <v>1197</v>
       </c>
       <c r="E160" s="8" t="s">
         <v>675</v>
@@ -11077,7 +11086,7 @@
         <v>665</v>
       </c>
       <c r="D161" s="8" t="s">
-        <v>1207</v>
+        <v>1198</v>
       </c>
       <c r="E161" s="8" t="s">
         <v>679</v>
@@ -11109,7 +11118,7 @@
         <v>665</v>
       </c>
       <c r="D162" s="8" t="s">
-        <v>1208</v>
+        <v>1199</v>
       </c>
       <c r="E162" s="8" t="s">
         <v>683</v>
@@ -11141,7 +11150,7 @@
         <v>665</v>
       </c>
       <c r="D163" s="8" t="s">
-        <v>1209</v>
+        <v>1200</v>
       </c>
       <c r="E163" s="8" t="s">
         <v>687</v>
@@ -11173,7 +11182,7 @@
         <v>665</v>
       </c>
       <c r="D164" s="8" t="s">
-        <v>1210</v>
+        <v>1201</v>
       </c>
       <c r="E164" s="8" t="s">
         <v>691</v>
@@ -11205,7 +11214,7 @@
         <v>699</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>1211</v>
+        <v>1202</v>
       </c>
       <c r="E165" s="8" t="s">
         <v>700</v>
@@ -11237,7 +11246,7 @@
         <v>699</v>
       </c>
       <c r="D166" s="8" t="s">
-        <v>1212</v>
+        <v>1203</v>
       </c>
       <c r="E166" s="8" t="s">
         <v>704</v>
@@ -11269,7 +11278,7 @@
         <v>699</v>
       </c>
       <c r="D167" s="8" t="s">
-        <v>1213</v>
+        <v>1204</v>
       </c>
       <c r="E167" s="8" t="s">
         <v>707</v>
@@ -11301,7 +11310,7 @@
         <v>699</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>1214</v>
+        <v>1205</v>
       </c>
       <c r="E168" s="8" t="s">
         <v>710</v>
@@ -11333,7 +11342,7 @@
         <v>713</v>
       </c>
       <c r="D169" s="8" t="s">
-        <v>1215</v>
+        <v>1206</v>
       </c>
       <c r="E169" s="8" t="s">
         <v>714</v>
@@ -11351,10 +11360,10 @@
         <v>964</v>
       </c>
       <c r="K169" t="s">
-        <v>1223</v>
+        <v>1214</v>
       </c>
       <c r="L169" s="20" t="s">
-        <v>1216</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="170" spans="1:27" ht="225" x14ac:dyDescent="0.25">
@@ -11368,7 +11377,7 @@
         <v>713</v>
       </c>
       <c r="D170" s="8" t="s">
-        <v>1217</v>
+        <v>1208</v>
       </c>
       <c r="E170" s="8" t="s">
         <v>718</v>
@@ -11400,7 +11409,7 @@
         <v>713</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>1218</v>
+        <v>1209</v>
       </c>
       <c r="E171" s="8" t="s">
         <v>722</v>
@@ -11418,7 +11427,7 @@
         <v>964</v>
       </c>
       <c r="K171" t="s">
-        <v>1223</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="172" spans="1:27" ht="285.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11432,7 +11441,7 @@
         <v>713</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>1219</v>
+        <v>1210</v>
       </c>
       <c r="E172" s="8" t="s">
         <v>726</v>
@@ -11464,7 +11473,7 @@
         <v>713</v>
       </c>
       <c r="D173" s="8" t="s">
-        <v>1220</v>
+        <v>1211</v>
       </c>
       <c r="E173" s="10" t="s">
         <v>731</v>
@@ -11513,7 +11522,7 @@
         <v>735</v>
       </c>
       <c r="D174" s="8" t="s">
-        <v>1221</v>
+        <v>1212</v>
       </c>
       <c r="E174" s="14" t="s">
         <v>748</v>
@@ -11531,8 +11540,8 @@
       <c r="J174" s="24" t="s">
         <v>964</v>
       </c>
-      <c r="K174" s="24" t="s">
-        <v>911</v>
+      <c r="K174" t="s">
+        <v>1012</v>
       </c>
       <c r="L174" s="24"/>
       <c r="M174" s="16"/>
@@ -11562,7 +11571,7 @@
         <v>753</v>
       </c>
       <c r="D175" s="8" t="s">
-        <v>1224</v>
+        <v>1215</v>
       </c>
       <c r="E175" s="8" t="s">
         <v>754</v>
@@ -11582,8 +11591,8 @@
       <c r="J175" s="25" t="s">
         <v>964</v>
       </c>
-      <c r="K175" s="25" t="s">
-        <v>911</v>
+      <c r="K175" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="176" spans="1:27" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11597,7 +11606,7 @@
         <v>753</v>
       </c>
       <c r="D176" s="8" t="s">
-        <v>1225</v>
+        <v>1216</v>
       </c>
       <c r="E176" s="8" t="s">
         <v>759</v>
@@ -11635,7 +11644,7 @@
         <v>753</v>
       </c>
       <c r="D177" s="8" t="s">
-        <v>1226</v>
+        <v>1217</v>
       </c>
       <c r="E177" s="8" t="s">
         <v>764</v>
@@ -11667,7 +11676,7 @@
         <v>753</v>
       </c>
       <c r="D178" s="8" t="s">
-        <v>1228</v>
+        <v>1219</v>
       </c>
       <c r="E178" s="8" t="s">
         <v>768</v>
@@ -11676,7 +11685,7 @@
         <v>38</v>
       </c>
       <c r="G178" s="13" t="s">
-        <v>1227</v>
+        <v>1218</v>
       </c>
       <c r="I178" s="2" t="s">
         <v>766</v>
@@ -11699,7 +11708,7 @@
         <v>753</v>
       </c>
       <c r="D179" s="8" t="s">
-        <v>1229</v>
+        <v>1220</v>
       </c>
       <c r="E179" s="8" t="s">
         <v>768</v>
@@ -11732,7 +11741,7 @@
         <v>753</v>
       </c>
       <c r="D180" s="8" t="s">
-        <v>1230</v>
+        <v>1221</v>
       </c>
       <c r="E180" s="8" t="s">
         <v>768</v>
@@ -11765,7 +11774,7 @@
         <v>753</v>
       </c>
       <c r="D181" s="8" t="s">
-        <v>1231</v>
+        <v>1222</v>
       </c>
       <c r="E181" s="8" t="s">
         <v>776</v>
@@ -11797,7 +11806,7 @@
         <v>805</v>
       </c>
       <c r="D182" s="8" t="s">
-        <v>1232</v>
+        <v>1223</v>
       </c>
       <c r="E182" s="8" t="s">
         <v>806</v>
@@ -11829,7 +11838,7 @@
         <v>805</v>
       </c>
       <c r="D183" s="8" t="s">
-        <v>1233</v>
+        <v>1224</v>
       </c>
       <c r="E183" s="8" t="s">
         <v>809</v>
@@ -11861,7 +11870,7 @@
         <v>805</v>
       </c>
       <c r="D184" s="8" t="s">
-        <v>1234</v>
+        <v>1225</v>
       </c>
       <c r="E184" s="8" t="s">
         <v>814</v>
@@ -11893,7 +11902,7 @@
         <v>805</v>
       </c>
       <c r="D185" s="8" t="s">
-        <v>1235</v>
+        <v>1226</v>
       </c>
       <c r="E185" s="8" t="s">
         <v>826</v>
@@ -11925,7 +11934,7 @@
         <v>805</v>
       </c>
       <c r="D186" s="8" t="s">
-        <v>1117</v>
+        <v>1227</v>
       </c>
       <c r="E186" s="8" t="s">
         <v>820</v>
@@ -11960,7 +11969,7 @@
         <v>805</v>
       </c>
       <c r="D187" s="8" t="s">
-        <v>1106</v>
+        <v>1228</v>
       </c>
       <c r="E187" s="8" t="s">
         <v>823</v>
@@ -11992,7 +12001,7 @@
         <v>805</v>
       </c>
       <c r="D188" s="8" t="s">
-        <v>1107</v>
+        <v>1229</v>
       </c>
       <c r="E188" s="8" t="s">
         <v>830</v>
@@ -12024,7 +12033,7 @@
         <v>805</v>
       </c>
       <c r="D189" s="8" t="s">
-        <v>1108</v>
+        <v>1230</v>
       </c>
       <c r="E189" s="8" t="s">
         <v>837</v>
@@ -12056,7 +12065,7 @@
         <v>805</v>
       </c>
       <c r="D190" s="8" t="s">
-        <v>1109</v>
+        <v>1231</v>
       </c>
       <c r="E190" s="8" t="s">
         <v>838</v>
@@ -12088,7 +12097,7 @@
         <v>805</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>1110</v>
+        <v>1232</v>
       </c>
       <c r="E191" s="8" t="s">
         <v>842</v>
@@ -12120,7 +12129,7 @@
         <v>805</v>
       </c>
       <c r="D192" s="8" t="s">
-        <v>1118</v>
+        <v>1233</v>
       </c>
       <c r="E192" s="8" t="s">
         <v>846</v>
@@ -12152,7 +12161,7 @@
         <v>805</v>
       </c>
       <c r="D193" s="8" t="s">
-        <v>1119</v>
+        <v>1234</v>
       </c>
       <c r="E193" s="8" t="s">
         <v>850</v>
@@ -12184,7 +12193,7 @@
         <v>805</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>1111</v>
+        <v>1235</v>
       </c>
       <c r="E194" s="8" t="s">
         <v>855</v>
@@ -12216,7 +12225,7 @@
         <v>805</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>1108</v>
+        <v>1236</v>
       </c>
       <c r="E195" s="8" t="s">
         <v>862</v>
@@ -12247,6 +12256,9 @@
       <c r="C196" s="8" t="s">
         <v>805</v>
       </c>
+      <c r="D196" s="8" t="s">
+        <v>1237</v>
+      </c>
       <c r="E196" s="8" t="s">
         <v>863</v>
       </c>
@@ -12276,6 +12288,9 @@
       <c r="C197" s="8" t="s">
         <v>805</v>
       </c>
+      <c r="D197" s="8" t="s">
+        <v>1238</v>
+      </c>
       <c r="E197" s="8" t="s">
         <v>867</v>
       </c>
@@ -12341,7 +12356,7 @@
         <v>874</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>1112</v>
+        <v>1106</v>
       </c>
       <c r="E199" s="8" t="s">
         <v>879</v>
@@ -12373,7 +12388,7 @@
         <v>875</v>
       </c>
       <c r="D200" s="8" t="s">
-        <v>1113</v>
+        <v>1107</v>
       </c>
       <c r="E200" s="8" t="s">
         <v>876</v>
@@ -12405,7 +12420,7 @@
         <v>885</v>
       </c>
       <c r="D201" s="8" t="s">
-        <v>1114</v>
+        <v>1108</v>
       </c>
       <c r="E201" s="8" t="s">
         <v>886</v>
@@ -12455,7 +12470,7 @@
         <v>970</v>
       </c>
       <c r="M202" t="s">
-        <v>1222</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="203" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12469,7 +12484,7 @@
         <v>736</v>
       </c>
       <c r="D203" s="8" t="s">
-        <v>1116</v>
+        <v>1110</v>
       </c>
       <c r="E203" s="8" t="s">
         <v>741</v>
@@ -12493,7 +12508,7 @@
         <v>969</v>
       </c>
       <c r="M203" t="s">
-        <v>1222</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="204" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12528,7 +12543,7 @@
         <v>960</v>
       </c>
       <c r="M204" t="s">
-        <v>1222</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="205" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12563,7 +12578,7 @@
         <v>911</v>
       </c>
       <c r="M205" t="s">
-        <v>1222</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="206" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12598,7 +12613,7 @@
         <v>911</v>
       </c>
       <c r="M206" t="s">
-        <v>1222</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="207" spans="1:13" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12633,7 +12648,7 @@
         <v>961</v>
       </c>
       <c r="M207" t="s">
-        <v>1222</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="208" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12668,7 +12683,7 @@
         <v>961</v>
       </c>
       <c r="M208" t="s">
-        <v>1222</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="209" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12706,7 +12721,7 @@
         <v>961</v>
       </c>
       <c r="M209" t="s">
-        <v>1222</v>
+        <v>1213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started marks entry section.......
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3974" uniqueCount="1239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3976" uniqueCount="1240">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5074,12 +5074,6 @@
     <t>ft_ViewofLessonplan</t>
   </si>
   <si>
-    <t>f _MarksEntryLinkofInheader</t>
-  </si>
-  <si>
-    <t>f _FunctionalityToGradeStudentsOnReadingSkillsWritingSkillsSpeakingSkillsAndListeningSkillsAndAlsoToEnterTheMarksScoredInofTermtest</t>
-  </si>
-  <si>
     <t>f _MarksEntryFeatureIsEnabledOnlyofClassteacher</t>
   </si>
   <si>
@@ -5501,6 +5495,15 @@
   </si>
   <si>
     <t>fn_DownloadAssignmentSubmittedResources</t>
+  </si>
+  <si>
+    <t>fn_StudentAssignmentMarkingReport</t>
+  </si>
+  <si>
+    <t>fn_VisibilityofMarksEntryLink</t>
+  </si>
+  <si>
+    <t>fn_GradeStudents</t>
   </si>
 </sst>
 </file>
@@ -5978,8 +5981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="D197" sqref="D197"/>
+    <sheetView tabSelected="1" topLeftCell="F199" workbookViewId="0">
+      <selection activeCell="K200" sqref="K200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8625,7 +8628,7 @@
         <v>347</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>355</v>
@@ -8657,7 +8660,7 @@
         <v>347</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>360</v>
@@ -8689,7 +8692,7 @@
         <v>347</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>364</v>
@@ -8721,7 +8724,7 @@
         <v>368</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>370</v>
@@ -8753,7 +8756,7 @@
         <v>368</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="E88" s="8" t="s">
         <v>374</v>
@@ -8783,7 +8786,7 @@
         <v>377</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>382</v>
@@ -8812,7 +8815,7 @@
         <v>381</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="E90" s="8" t="s">
         <v>384</v>
@@ -8844,7 +8847,7 @@
         <v>381</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>386</v>
@@ -8876,7 +8879,7 @@
         <v>381</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>390</v>
@@ -8908,7 +8911,7 @@
         <v>381</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="E93" s="8" t="s">
         <v>394</v>
@@ -8940,7 +8943,7 @@
         <v>381</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="E94" s="8" t="s">
         <v>398</v>
@@ -8972,7 +8975,7 @@
         <v>381</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="E95" s="8" t="s">
         <v>403</v>
@@ -9004,7 +9007,7 @@
         <v>381</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>407</v>
@@ -9036,7 +9039,7 @@
         <v>414</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="E97" s="8" t="s">
         <v>412</v>
@@ -9068,7 +9071,7 @@
         <v>414</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>416</v>
@@ -9100,7 +9103,7 @@
         <v>425</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="E99" s="8" t="s">
         <v>424</v>
@@ -9132,7 +9135,7 @@
         <v>422</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>427</v>
@@ -9164,7 +9167,7 @@
         <v>422</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>429</v>
@@ -9185,7 +9188,7 @@
         <v>1012</v>
       </c>
       <c r="L101" s="8" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="195" x14ac:dyDescent="0.25">
@@ -9199,7 +9202,7 @@
         <v>422</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="E102" s="8" t="s">
         <v>436</v>
@@ -9231,7 +9234,7 @@
         <v>422</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="E103" s="8" t="s">
         <v>438</v>
@@ -9260,7 +9263,7 @@
         <v>442</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>443</v>
@@ -9292,7 +9295,7 @@
         <v>442</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="E105" s="8" t="s">
         <v>446</v>
@@ -9324,7 +9327,7 @@
         <v>442</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="E106" s="8" t="s">
         <v>451</v>
@@ -9356,7 +9359,7 @@
         <v>442</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="E107" s="8" t="s">
         <v>455</v>
@@ -9385,7 +9388,7 @@
         <v>458</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>460</v>
@@ -9414,7 +9417,7 @@
         <v>458</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="E109" s="8" t="s">
         <v>620</v>
@@ -9443,7 +9446,7 @@
         <v>458</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="E110" s="8" t="s">
         <v>621</v>
@@ -9472,7 +9475,7 @@
         <v>464</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>465</v>
@@ -9498,10 +9501,10 @@
         <v>411</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="E112" s="8"/>
       <c r="G112" s="2"/>
@@ -9521,7 +9524,7 @@
         <v>468</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="E113" s="8" t="s">
         <v>471</v>
@@ -9550,7 +9553,7 @@
         <v>472</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="E114" s="8" t="s">
         <v>474</v>
@@ -9579,7 +9582,7 @@
         <v>481</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="E115" s="8" t="s">
         <v>424</v>
@@ -9611,7 +9614,7 @@
         <v>477</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="E116" s="8" t="s">
         <v>478</v>
@@ -9643,7 +9646,7 @@
         <v>486</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="E117" s="8" t="s">
         <v>487</v>
@@ -9675,7 +9678,7 @@
         <v>490</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="E118" s="8" t="s">
         <v>491</v>
@@ -9707,7 +9710,7 @@
         <v>490</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="E119" s="8" t="s">
         <v>495</v>
@@ -9739,7 +9742,7 @@
         <v>498</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="E120" s="8" t="s">
         <v>500</v>
@@ -9774,7 +9777,7 @@
         <v>498</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="E121" s="8" t="s">
         <v>505</v>
@@ -9806,7 +9809,7 @@
         <v>498</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="E122" s="8" t="s">
         <v>508</v>
@@ -9842,7 +9845,7 @@
         <v>498</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="E123" s="8" t="s">
         <v>513</v>
@@ -9875,7 +9878,7 @@
         <v>498</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="E124" s="8" t="s">
         <v>521</v>
@@ -9894,7 +9897,7 @@
         <v>1012</v>
       </c>
       <c r="L124" s="20" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="125" spans="1:12" ht="315" x14ac:dyDescent="0.25">
@@ -9905,22 +9908,22 @@
         <v>411</v>
       </c>
       <c r="C125" s="8" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D125" s="8" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E125" s="8" t="s">
         <v>1155</v>
       </c>
-      <c r="D125" s="8" t="s">
+      <c r="F125" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>1160</v>
+      </c>
+      <c r="H125" s="2" t="s">
         <v>1156</v>
-      </c>
-      <c r="E125" s="8" t="s">
-        <v>1157</v>
-      </c>
-      <c r="F125" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G125" s="2" t="s">
-        <v>1162</v>
-      </c>
-      <c r="H125" s="2" t="s">
-        <v>1158</v>
       </c>
       <c r="I125" s="2" t="s">
         <v>502</v>
@@ -9943,7 +9946,7 @@
         <v>498</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="E126" s="8" t="s">
         <v>505</v>
@@ -9975,7 +9978,7 @@
         <v>498</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="E127" s="8" t="s">
         <v>508</v>
@@ -9984,7 +9987,7 @@
         <v>38</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="H127" s="2"/>
       <c r="I127" s="2" t="s">
@@ -10011,7 +10014,7 @@
         <v>498</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="E128" s="8" t="s">
         <v>513</v>
@@ -10044,7 +10047,7 @@
         <v>498</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="E129" s="8" t="s">
         <v>521</v>
@@ -10063,7 +10066,7 @@
         <v>911</v>
       </c>
       <c r="L129" s="20" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="130" spans="1:12" ht="375" x14ac:dyDescent="0.25">
@@ -10077,7 +10080,7 @@
         <v>540</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="E130" s="8" t="s">
         <v>543</v>
@@ -10109,7 +10112,7 @@
         <v>540</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="E131" s="8" t="s">
         <v>548</v>
@@ -10142,7 +10145,7 @@
         <v>552</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="E132" s="8" t="s">
         <v>553</v>
@@ -10163,7 +10166,7 @@
         <v>1012</v>
       </c>
       <c r="L132" s="20" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="133" spans="1:12" ht="165" x14ac:dyDescent="0.25">
@@ -10177,7 +10180,7 @@
         <v>552</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="E133" s="8" t="s">
         <v>557</v>
@@ -10209,7 +10212,7 @@
         <v>561</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="E134" s="8" t="s">
         <v>562</v>
@@ -10241,7 +10244,7 @@
         <v>561</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="E135" s="8" t="s">
         <v>565</v>
@@ -10273,7 +10276,7 @@
         <v>561</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="E136" s="8" t="s">
         <v>568</v>
@@ -10305,7 +10308,7 @@
         <v>561</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="E137" s="8" t="s">
         <v>572</v>
@@ -10337,7 +10340,7 @@
         <v>561</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="E138" s="8" t="s">
         <v>576</v>
@@ -10369,7 +10372,7 @@
         <v>581</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="E139" s="6" t="s">
         <v>582</v>
@@ -10401,7 +10404,7 @@
         <v>581</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="E140" s="8" t="s">
         <v>625</v>
@@ -10433,7 +10436,7 @@
         <v>581</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="E141" s="8" t="s">
         <v>628</v>
@@ -10465,7 +10468,7 @@
         <v>581</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="E142" s="8" t="s">
         <v>586</v>
@@ -10497,7 +10500,7 @@
         <v>594</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="E143" s="8" t="s">
         <v>593</v>
@@ -10518,7 +10521,7 @@
         <v>1012</v>
       </c>
       <c r="L143" s="20" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="144" spans="1:12" ht="180" x14ac:dyDescent="0.25">
@@ -10532,7 +10535,7 @@
         <v>595</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="E144" s="8" t="s">
         <v>596</v>
@@ -10564,7 +10567,7 @@
         <v>595</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="E145" s="8" t="s">
         <v>600</v>
@@ -10596,7 +10599,7 @@
         <v>595</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="E146" s="8" t="s">
         <v>604</v>
@@ -10631,7 +10634,7 @@
         <v>595</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="E147" s="8" t="s">
         <v>609</v>
@@ -10663,7 +10666,7 @@
         <v>595</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="E148" s="8" t="s">
         <v>612</v>
@@ -10695,7 +10698,7 @@
         <v>617</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="E149" s="6" t="s">
         <v>635</v>
@@ -10727,7 +10730,7 @@
         <v>617</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="E150" s="8" t="s">
         <v>638</v>
@@ -10759,7 +10762,7 @@
         <v>617</v>
       </c>
       <c r="D151" s="8" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="E151" s="6" t="s">
         <v>641</v>
@@ -10791,7 +10794,7 @@
         <v>617</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="E152" s="8" t="s">
         <v>645</v>
@@ -10823,7 +10826,7 @@
         <v>617</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="E153" s="8" t="s">
         <v>649</v>
@@ -10855,7 +10858,7 @@
         <v>617</v>
       </c>
       <c r="D154" s="8" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E154" s="8" t="s">
         <v>653</v>
@@ -10887,7 +10890,7 @@
         <v>617</v>
       </c>
       <c r="D155" s="8" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="E155" s="8" t="s">
         <v>657</v>
@@ -10919,7 +10922,7 @@
         <v>617</v>
       </c>
       <c r="D156" s="8" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="E156" s="8" t="s">
         <v>661</v>
@@ -10951,7 +10954,7 @@
         <v>665</v>
       </c>
       <c r="D157" s="8" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="E157" s="8" t="s">
         <v>666</v>
@@ -10972,7 +10975,7 @@
         <v>1012</v>
       </c>
       <c r="L157" s="20" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="158" spans="1:12" ht="195" x14ac:dyDescent="0.25">
@@ -10986,7 +10989,7 @@
         <v>665</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="E158" s="8" t="s">
         <v>694</v>
@@ -11019,7 +11022,7 @@
         <v>665</v>
       </c>
       <c r="D159" s="8" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="E159" s="8" t="s">
         <v>671</v>
@@ -11054,7 +11057,7 @@
         <v>665</v>
       </c>
       <c r="D160" s="8" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="E160" s="8" t="s">
         <v>675</v>
@@ -11086,7 +11089,7 @@
         <v>665</v>
       </c>
       <c r="D161" s="8" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="E161" s="8" t="s">
         <v>679</v>
@@ -11118,7 +11121,7 @@
         <v>665</v>
       </c>
       <c r="D162" s="8" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="E162" s="8" t="s">
         <v>683</v>
@@ -11150,7 +11153,7 @@
         <v>665</v>
       </c>
       <c r="D163" s="8" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="E163" s="8" t="s">
         <v>687</v>
@@ -11182,7 +11185,7 @@
         <v>665</v>
       </c>
       <c r="D164" s="8" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="E164" s="8" t="s">
         <v>691</v>
@@ -11214,7 +11217,7 @@
         <v>699</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="E165" s="8" t="s">
         <v>700</v>
@@ -11246,7 +11249,7 @@
         <v>699</v>
       </c>
       <c r="D166" s="8" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="E166" s="8" t="s">
         <v>704</v>
@@ -11278,7 +11281,7 @@
         <v>699</v>
       </c>
       <c r="D167" s="8" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="E167" s="8" t="s">
         <v>707</v>
@@ -11310,7 +11313,7 @@
         <v>699</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="E168" s="8" t="s">
         <v>710</v>
@@ -11342,7 +11345,7 @@
         <v>713</v>
       </c>
       <c r="D169" s="8" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="E169" s="8" t="s">
         <v>714</v>
@@ -11360,10 +11363,10 @@
         <v>964</v>
       </c>
       <c r="K169" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="L169" s="20" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="170" spans="1:27" ht="225" x14ac:dyDescent="0.25">
@@ -11377,7 +11380,7 @@
         <v>713</v>
       </c>
       <c r="D170" s="8" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="E170" s="8" t="s">
         <v>718</v>
@@ -11409,7 +11412,7 @@
         <v>713</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="E171" s="8" t="s">
         <v>722</v>
@@ -11427,7 +11430,7 @@
         <v>964</v>
       </c>
       <c r="K171" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="172" spans="1:27" ht="285.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11441,7 +11444,7 @@
         <v>713</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="E172" s="8" t="s">
         <v>726</v>
@@ -11473,7 +11476,7 @@
         <v>713</v>
       </c>
       <c r="D173" s="8" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="E173" s="10" t="s">
         <v>731</v>
@@ -11522,7 +11525,7 @@
         <v>735</v>
       </c>
       <c r="D174" s="8" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="E174" s="14" t="s">
         <v>748</v>
@@ -11571,7 +11574,7 @@
         <v>753</v>
       </c>
       <c r="D175" s="8" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="E175" s="8" t="s">
         <v>754</v>
@@ -11606,7 +11609,7 @@
         <v>753</v>
       </c>
       <c r="D176" s="8" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="E176" s="8" t="s">
         <v>759</v>
@@ -11626,8 +11629,8 @@
       <c r="J176" s="25" t="s">
         <v>964</v>
       </c>
-      <c r="K176" s="25" t="s">
-        <v>911</v>
+      <c r="K176" t="s">
+        <v>1012</v>
       </c>
       <c r="L176" s="25" t="s">
         <v>968</v>
@@ -11644,7 +11647,7 @@
         <v>753</v>
       </c>
       <c r="D177" s="8" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="E177" s="8" t="s">
         <v>764</v>
@@ -11661,8 +11664,8 @@
       <c r="J177" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K177" s="6" t="s">
-        <v>911</v>
+      <c r="K177" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="178" spans="1:12" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11676,7 +11679,7 @@
         <v>753</v>
       </c>
       <c r="D178" s="8" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="E178" s="8" t="s">
         <v>768</v>
@@ -11685,7 +11688,7 @@
         <v>38</v>
       </c>
       <c r="G178" s="13" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="I178" s="2" t="s">
         <v>766</v>
@@ -11693,8 +11696,8 @@
       <c r="J178" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K178" s="6" t="s">
-        <v>911</v>
+      <c r="K178" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="179" spans="1:12" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11708,7 +11711,7 @@
         <v>753</v>
       </c>
       <c r="D179" s="8" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="E179" s="8" t="s">
         <v>768</v>
@@ -11726,8 +11729,8 @@
       <c r="J179" s="25" t="s">
         <v>964</v>
       </c>
-      <c r="K179" s="25" t="s">
-        <v>911</v>
+      <c r="K179" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="180" spans="1:12" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11741,7 +11744,7 @@
         <v>753</v>
       </c>
       <c r="D180" s="8" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="E180" s="8" t="s">
         <v>768</v>
@@ -11759,8 +11762,8 @@
       <c r="J180" s="25" t="s">
         <v>964</v>
       </c>
-      <c r="K180" s="25" t="s">
-        <v>911</v>
+      <c r="K180" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="181" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11774,7 +11777,7 @@
         <v>753</v>
       </c>
       <c r="D181" s="8" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="E181" s="8" t="s">
         <v>776</v>
@@ -11791,8 +11794,8 @@
       <c r="J181" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K181" s="25" t="s">
-        <v>911</v>
+      <c r="K181" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="182" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11806,7 +11809,7 @@
         <v>805</v>
       </c>
       <c r="D182" s="8" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="E182" s="8" t="s">
         <v>806</v>
@@ -11823,8 +11826,8 @@
       <c r="J182" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K182" s="27" t="s">
-        <v>911</v>
+      <c r="K182" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="183" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11838,7 +11841,7 @@
         <v>805</v>
       </c>
       <c r="D183" s="8" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="E183" s="8" t="s">
         <v>809</v>
@@ -11855,8 +11858,8 @@
       <c r="J183" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K183" s="27" t="s">
-        <v>911</v>
+      <c r="K183" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="184" spans="1:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11870,7 +11873,7 @@
         <v>805</v>
       </c>
       <c r="D184" s="8" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="E184" s="8" t="s">
         <v>814</v>
@@ -11887,8 +11890,8 @@
       <c r="J184" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K184" s="27" t="s">
-        <v>911</v>
+      <c r="K184" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="185" spans="1:12" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11902,7 +11905,7 @@
         <v>805</v>
       </c>
       <c r="D185" s="8" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="E185" s="8" t="s">
         <v>826</v>
@@ -11919,8 +11922,8 @@
       <c r="J185" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K185" s="27" t="s">
-        <v>911</v>
+      <c r="K185" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="186" spans="1:12" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11934,7 +11937,7 @@
         <v>805</v>
       </c>
       <c r="D186" s="8" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="E186" s="8" t="s">
         <v>820</v>
@@ -11951,8 +11954,8 @@
       <c r="J186" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K186" s="27" t="s">
-        <v>911</v>
+      <c r="K186" t="s">
+        <v>1012</v>
       </c>
       <c r="L186" s="8" t="s">
         <v>962</v>
@@ -11969,7 +11972,7 @@
         <v>805</v>
       </c>
       <c r="D187" s="8" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="E187" s="8" t="s">
         <v>823</v>
@@ -11986,8 +11989,8 @@
       <c r="J187" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K187" s="27" t="s">
-        <v>911</v>
+      <c r="K187" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="188" spans="1:12" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12001,7 +12004,7 @@
         <v>805</v>
       </c>
       <c r="D188" s="8" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E188" s="8" t="s">
         <v>830</v>
@@ -12018,8 +12021,8 @@
       <c r="J188" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K188" s="27" t="s">
-        <v>911</v>
+      <c r="K188" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="189" spans="1:12" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12033,7 +12036,7 @@
         <v>805</v>
       </c>
       <c r="D189" s="8" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="E189" s="8" t="s">
         <v>837</v>
@@ -12050,8 +12053,8 @@
       <c r="J189" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K189" s="27" t="s">
-        <v>911</v>
+      <c r="K189" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="190" spans="1:12" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12065,7 +12068,7 @@
         <v>805</v>
       </c>
       <c r="D190" s="8" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="E190" s="8" t="s">
         <v>838</v>
@@ -12082,8 +12085,8 @@
       <c r="J190" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K190" s="27" t="s">
-        <v>911</v>
+      <c r="K190" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="191" spans="1:12" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12097,7 +12100,7 @@
         <v>805</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="E191" s="8" t="s">
         <v>842</v>
@@ -12114,8 +12117,8 @@
       <c r="J191" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K191" s="27" t="s">
-        <v>911</v>
+      <c r="K191" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="192" spans="1:12" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12129,7 +12132,7 @@
         <v>805</v>
       </c>
       <c r="D192" s="8" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="E192" s="8" t="s">
         <v>846</v>
@@ -12161,7 +12164,7 @@
         <v>805</v>
       </c>
       <c r="D193" s="8" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="E193" s="8" t="s">
         <v>850</v>
@@ -12193,7 +12196,7 @@
         <v>805</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="E194" s="8" t="s">
         <v>855</v>
@@ -12210,8 +12213,8 @@
       <c r="J194" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K194" s="27" t="s">
-        <v>911</v>
+      <c r="K194" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="195" spans="1:13" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12225,7 +12228,7 @@
         <v>805</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="E195" s="8" t="s">
         <v>862</v>
@@ -12242,8 +12245,8 @@
       <c r="J195" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K195" s="27" t="s">
-        <v>911</v>
+      <c r="K195" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="196" spans="1:13" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12257,7 +12260,7 @@
         <v>805</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="E196" s="8" t="s">
         <v>863</v>
@@ -12289,7 +12292,7 @@
         <v>805</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="E197" s="8" t="s">
         <v>867</v>
@@ -12323,6 +12326,9 @@
       <c r="C198" s="8" t="s">
         <v>805</v>
       </c>
+      <c r="D198" s="8" t="s">
+        <v>1237</v>
+      </c>
       <c r="E198" s="8" t="s">
         <v>820</v>
       </c>
@@ -12345,7 +12351,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="199" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A199" s="6" t="s">
         <v>849</v>
       </c>
@@ -12356,7 +12362,7 @@
         <v>874</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>1106</v>
+        <v>1238</v>
       </c>
       <c r="E199" s="8" t="s">
         <v>879</v>
@@ -12373,8 +12379,8 @@
       <c r="J199" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K199" s="22" t="s">
-        <v>911</v>
+      <c r="K199" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="200" spans="1:13" ht="180" x14ac:dyDescent="0.25">
@@ -12388,7 +12394,7 @@
         <v>875</v>
       </c>
       <c r="D200" s="8" t="s">
-        <v>1107</v>
+        <v>1239</v>
       </c>
       <c r="E200" s="8" t="s">
         <v>876</v>
@@ -12405,8 +12411,8 @@
       <c r="J200" s="6" t="s">
         <v>964</v>
       </c>
-      <c r="K200" s="22" t="s">
-        <v>911</v>
+      <c r="K200" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="201" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12420,7 +12426,7 @@
         <v>885</v>
       </c>
       <c r="D201" s="8" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="E201" s="8" t="s">
         <v>886</v>
@@ -12439,6 +12445,9 @@
       </c>
       <c r="K201" s="22" t="s">
         <v>911</v>
+      </c>
+      <c r="M201" t="s">
+        <v>1211</v>
       </c>
     </row>
     <row r="202" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12470,7 +12479,7 @@
         <v>970</v>
       </c>
       <c r="M202" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="203" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12484,7 +12493,7 @@
         <v>736</v>
       </c>
       <c r="D203" s="8" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="E203" s="8" t="s">
         <v>741</v>
@@ -12508,7 +12517,7 @@
         <v>969</v>
       </c>
       <c r="M203" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="204" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12543,7 +12552,7 @@
         <v>960</v>
       </c>
       <c r="M204" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="205" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12578,7 +12587,7 @@
         <v>911</v>
       </c>
       <c r="M205" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="206" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12613,7 +12622,7 @@
         <v>911</v>
       </c>
       <c r="M206" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="207" spans="1:13" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12648,7 +12657,7 @@
         <v>961</v>
       </c>
       <c r="M207" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="208" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12683,7 +12692,7 @@
         <v>961</v>
       </c>
       <c r="M208" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="209" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12721,7 +12730,7 @@
         <v>961</v>
       </c>
       <c r="M209" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added IRetry Analyzer in testng to run only failed methods....
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3976" uniqueCount="1240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3978" uniqueCount="1242">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5505,12 +5505,20 @@
   <si>
     <t>fn_GradeStudents</t>
   </si>
+  <si>
+    <t>https://203.129.242.98/OxfordAdvantageUAT/Reports/AdminStudentReport.aspx?ar=1&amp;classid=RKQ80oM78lg=</t>
+  </si>
+  <si>
+    <t>1. Changing on Academic year in dropdown  loader moving continue and nothing happens
+2. Practice Test details window not getting opened and direct overall performance is coming</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5547,6 +5555,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5590,10 +5606,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5675,8 +5692,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5981,25 +6000,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F199" workbookViewId="0">
-      <selection activeCell="K200" sqref="K200"/>
+    <sheetView tabSelected="1" topLeftCell="H65" workbookViewId="0">
+      <selection activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5703125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.5703125" style="8" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.85546875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.5703125" style="6" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="41.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26" style="6" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" style="6" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="52.7109375" style="8" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="16.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="8" width="16.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="6" width="31.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="6" width="33.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="41.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="6" width="26.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="6" width="11.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="8" width="52.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -8710,7 +8729,10 @@
         <v>909</v>
       </c>
       <c r="L86" s="20" t="s">
-        <v>940</v>
+        <v>1241</v>
+      </c>
+      <c r="M86" s="29" t="s">
+        <v>1240</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -12734,8 +12756,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M86" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -12749,17 +12774,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finished marks entry section.......
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3978" uniqueCount="1242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3979" uniqueCount="1242">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5517,8 +5517,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6000,25 +5999,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H65" workbookViewId="0">
-      <selection activeCell="K65" sqref="K65"/>
+    <sheetView tabSelected="1" topLeftCell="G208" workbookViewId="0">
+      <selection activeCell="G211" sqref="G211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="18.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="16.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="8" width="16.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="6" width="31.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="6" width="33.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="41.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="6" width="26.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="6" width="11.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="8" width="52.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.5703125" style="8" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.85546875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.5703125" style="6" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="41.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26" style="6" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.42578125" style="6" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="52.7109375" style="8" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -6115,7 +6114,9 @@
       <c r="J6" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K6"/>
+      <c r="K6" t="s">
+        <v>1012</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -6145,7 +6146,9 @@
       <c r="J7" s="6" t="s">
         <v>972</v>
       </c>
-      <c r="K7"/>
+      <c r="K7" t="s">
+        <v>1012</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -12757,7 +12760,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M86" r:id="rId3"/>
+    <hyperlink ref="M86" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -12774,17 +12777,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="31.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="37.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
improved excel code to report....
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4169" uniqueCount="1183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4170" uniqueCount="1189">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5198,6 +5198,24 @@
   </si>
   <si>
     <t>No students are coming in select users section</t>
+  </si>
+  <si>
+    <t>fn_MarksEntryFeatureIsEnabledOnlyofClassteacher</t>
+  </si>
+  <si>
+    <t>fn_ViewLessonPlanForMonth</t>
+  </si>
+  <si>
+    <t>fn_ViewLessonPlanForWeek</t>
+  </si>
+  <si>
+    <t>fn_ViewLessonPlanForDay</t>
+  </si>
+  <si>
+    <t>fn_ViewPlannedLesson</t>
+  </si>
+  <si>
+    <t>fn_ViewofLessonplan</t>
   </si>
 </sst>
 </file>
@@ -12456,8 +12474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H32" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" topLeftCell="F33" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13681,7 +13699,7 @@
         <v>924</v>
       </c>
       <c r="K37" t="s">
-        <v>952</v>
+        <v>959</v>
       </c>
       <c r="L37" s="8" t="s">
         <v>936</v>
@@ -13716,7 +13734,7 @@
         <v>924</v>
       </c>
       <c r="K38" t="s">
-        <v>952</v>
+        <v>959</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18882,7 +18900,7 @@
         <v>862</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>1046</v>
+        <v>1183</v>
       </c>
       <c r="E197" s="8" t="s">
         <v>863</v>
@@ -18916,6 +18934,9 @@
       <c r="C198" s="8" t="s">
         <v>713</v>
       </c>
+      <c r="D198" s="8" t="s">
+        <v>1184</v>
+      </c>
       <c r="E198" s="8" t="s">
         <v>714</v>
       </c>
@@ -18949,7 +18970,7 @@
         <v>713</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>1048</v>
+        <v>1186</v>
       </c>
       <c r="E199" s="8" t="s">
         <v>718</v>
@@ -18987,7 +19008,7 @@
         <v>713</v>
       </c>
       <c r="D200" s="8" t="s">
-        <v>1039</v>
+        <v>1185</v>
       </c>
       <c r="E200" s="8" t="s">
         <v>722</v>
@@ -19022,7 +19043,7 @@
         <v>756</v>
       </c>
       <c r="D201" s="8" t="s">
-        <v>1043</v>
+        <v>1187</v>
       </c>
       <c r="E201" s="6" t="s">
         <v>763</v>
@@ -19057,7 +19078,7 @@
         <v>761</v>
       </c>
       <c r="D202" s="8" t="s">
-        <v>1045</v>
+        <v>1188</v>
       </c>
       <c r="E202" s="6" t="s">
         <v>762</v>

</xml_diff>

<commit_message>
improved login module script...
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4170" uniqueCount="1189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4181" uniqueCount="1189">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5222,7 +5222,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5701,25 +5702,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA209"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="H148" workbookViewId="0">
+      <selection activeCell="K148" sqref="K148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5703125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.5703125" style="8" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.85546875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.5703125" style="6" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="41.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26" style="6" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" style="6" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="52.7109375" style="8" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="16.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="8" width="16.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="6" width="31.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="6" width="33.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="41.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="6" width="26.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="6" width="11.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="8" width="52.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -9764,7 +9765,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="345" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" ht="345" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>533</v>
       </c>
@@ -9797,7 +9798,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="130" spans="1:12" ht="375" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" ht="375" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
         <v>537</v>
       </c>
@@ -9829,7 +9830,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="131" spans="1:12" ht="330" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" ht="330" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>543</v>
       </c>
@@ -9862,7 +9863,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="132" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" ht="165" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
         <v>546</v>
       </c>
@@ -9896,8 +9897,11 @@
       <c r="L132" s="20" t="s">
         <v>1102</v>
       </c>
-    </row>
-    <row r="133" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+      <c r="N132" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" ht="165" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>548</v>
       </c>
@@ -9929,7 +9933,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="134" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
         <v>554</v>
       </c>
@@ -9961,7 +9965,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="135" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" ht="195" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
         <v>557</v>
       </c>
@@ -9993,7 +9997,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="136" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" ht="195" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
         <v>562</v>
       </c>
@@ -10025,7 +10029,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="137" spans="1:12" ht="225" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" ht="225" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
         <v>566</v>
       </c>
@@ -10057,7 +10061,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="138" spans="1:12" ht="225" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" ht="225" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
         <v>569</v>
       </c>
@@ -10089,7 +10093,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="139" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
         <v>576</v>
       </c>
@@ -10121,7 +10125,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="140" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
         <v>580</v>
       </c>
@@ -10153,7 +10157,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="141" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
         <v>582</v>
       </c>
@@ -10185,7 +10189,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
         <v>583</v>
       </c>
@@ -10217,7 +10221,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="143" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" ht="195" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
         <v>584</v>
       </c>
@@ -10252,7 +10256,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="144" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" ht="180" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
         <v>585</v>
       </c>
@@ -12463,7 +12467,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M86" r:id="rId1"/>
+    <hyperlink ref="M86" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -12474,25 +12478,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F33" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="A196" sqref="A196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5703125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.5703125" style="8" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.85546875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.5703125" style="6" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="41.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26" style="6" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" style="6" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="52.7109375" style="8" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="16.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="8" width="16.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="6" width="31.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="6" width="33.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="41.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="6" width="26.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="6" width="11.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="8" width="52.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12629,7 +12633,9 @@
       <c r="J4" s="6" t="s">
         <v>924</v>
       </c>
-      <c r="K4"/>
+      <c r="K4" t="s">
+        <v>952</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -12662,7 +12668,9 @@
       <c r="J5" s="20" t="s">
         <v>940</v>
       </c>
-      <c r="K5"/>
+      <c r="K5" t="s">
+        <v>952</v>
+      </c>
       <c r="L5" s="19"/>
     </row>
     <row r="6" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12696,7 +12704,9 @@
       <c r="J6" s="8" t="s">
         <v>869</v>
       </c>
-      <c r="K6"/>
+      <c r="K6" t="s">
+        <v>959</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -12727,7 +12737,9 @@
       <c r="J7" s="6" t="s">
         <v>924</v>
       </c>
-      <c r="K7"/>
+      <c r="K7" t="s">
+        <v>952</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -12756,6 +12768,9 @@
       </c>
       <c r="J8" s="6" t="s">
         <v>924</v>
+      </c>
+      <c r="K8" t="s">
+        <v>952</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19212,7 +19227,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M82" r:id="rId1"/>
+    <hyperlink ref="M82" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added always run to after methods...
</commit_message>
<xml_diff>
--- a/Advantage Test Cases.xlsx
+++ b/Advantage Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4181" uniqueCount="1189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4186" uniqueCount="1190">
   <si>
     <t>Test Objective</t>
   </si>
@@ -5216,6 +5216,10 @@
   </si>
   <si>
     <t>fn_ViewofLessonplan</t>
+  </si>
+  <si>
+    <t>1. No.of submissions block getting disappeared after selecting type
+2.Enhancement: Generate button shows dropdown sign, it needed to remove</t>
   </si>
 </sst>
 </file>
@@ -5702,8 +5706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA209"/>
   <sheetViews>
-    <sheetView topLeftCell="H148" workbookViewId="0">
-      <selection activeCell="K148" sqref="K148"/>
+    <sheetView topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="A209" sqref="A209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12478,8 +12482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="A196" sqref="A196"/>
+    <sheetView tabSelected="1" topLeftCell="H192" workbookViewId="0">
+      <selection activeCell="L193" sqref="L193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13486,7 +13490,7 @@
         <v>924</v>
       </c>
       <c r="K30" t="s">
-        <v>952</v>
+        <v>959</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17010,7 +17014,7 @@
         <v>952</v>
       </c>
       <c r="L139" s="20" t="s">
-        <v>1126</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="140" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17432,7 +17436,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="153" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
         <v>651</v>
       </c>

</xml_diff>